<commit_message>
EUR YC - consolidate worksheets
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YCONBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YCONBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -2703,7 +2703,7 @@
         <v>104</v>
       </c>
       <c r="D11" s="86">
-        <v>41618.599942129629</v>
+        <v>41618.657037037039</v>
       </c>
       <c r="E11" s="58"/>
       <c r="F11" s="57"/>
@@ -2757,7 +2757,7 @@
       </c>
       <c r="D14" s="83" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_EURYCON#0002</v>
+        <v>_EURYCON#0004</v>
       </c>
       <c r="E14" s="58"/>
       <c r="F14" s="57"/>
@@ -2931,9 +2931,9 @@
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
         <v>41618</v>
       </c>
-      <c r="D27" s="64">
+      <c r="D27" s="64" t="e">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="E27" s="58"/>
       <c r="F27" s="57"/>
@@ -2944,9 +2944,9 @@
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
         <v>52579</v>
       </c>
-      <c r="D28" s="62">
+      <c r="D28" s="62" t="e">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.48973558874081424</v>
+        <v>#NUM!</v>
       </c>
       <c r="E28" s="58"/>
       <c r="F28" s="57"/>
@@ -2957,8 +2957,8 @@
         <v>0</v>
       </c>
       <c r="D29" s="59" t="str">
-        <f>_xll.ohRangeRetrieveError(Selected!I1)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(Selected!I1)</f>
+        <v>qlPiecewiseYieldCurveData - 1st instrument (maturity: December 11th, 2013) has an invalid quote</v>
       </c>
       <c r="E29" s="58"/>
       <c r="F29" s="57"/>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="F3" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E3,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_SWD#0002</v>
+        <v>EUR_YC1YRH_SWD#0004</v>
       </c>
       <c r="G3" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -3112,7 +3112,7 @@
       </c>
       <c r="F4" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_2WD#0002</v>
+        <v>EUR_YC1YRH_2WD#0004</v>
       </c>
       <c r="G4" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -3139,7 +3139,7 @@
       </c>
       <c r="F5" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_3WD#0002</v>
+        <v>EUR_YC1YRH_3WD#0004</v>
       </c>
       <c r="G5" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="F6" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_1MD#0002</v>
+        <v>EUR_YC1YRH_1MD#0004</v>
       </c>
       <c r="G6" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -3193,7 +3193,7 @@
       </c>
       <c r="F7" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_2MD#0002</v>
+        <v>EUR_YC1YRH_2MD#0004</v>
       </c>
       <c r="G7" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -3220,7 +3220,7 @@
       </c>
       <c r="F8" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_3MD#0002</v>
+        <v>EUR_YC1YRH_3MD#0004</v>
       </c>
       <c r="G8" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="F9" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_4MD#0002</v>
+        <v>EUR_YC1YRH_4MD#0004</v>
       </c>
       <c r="G9" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -3274,7 +3274,7 @@
       </c>
       <c r="F10" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E10,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_5MD#0002</v>
+        <v>EUR_YC1YRH_5MD#0004</v>
       </c>
       <c r="G10" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="F11" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E11,D11,C11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_6MD#0002</v>
+        <v>EUR_YC1YRH_6MD#0004</v>
       </c>
       <c r="G11" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>
@@ -3328,7 +3328,7 @@
       </c>
       <c r="F12" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E12,D12,C12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_7MD#0002</v>
+        <v>EUR_YC1YRH_7MD#0004</v>
       </c>
       <c r="G12" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F12)</f>
@@ -3355,7 +3355,7 @@
       </c>
       <c r="F13" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E13,D13,C13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_8MD#0002</v>
+        <v>EUR_YC1YRH_8MD#0004</v>
       </c>
       <c r="G13" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F13)</f>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="F14" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E14,D14,C14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_9MD#0002</v>
+        <v>EUR_YC1YRH_9MD#0004</v>
       </c>
       <c r="G14" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F14)</f>
@@ -3409,7 +3409,7 @@
       </c>
       <c r="F15" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E15,D15,C15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_10MD#0002</v>
+        <v>EUR_YC1YRH_10MD#0004</v>
       </c>
       <c r="G15" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F15)</f>
@@ -3436,7 +3436,7 @@
       </c>
       <c r="F16" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E16,D16,C16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_11MD#0002</v>
+        <v>EUR_YC1YRH_11MD#0004</v>
       </c>
       <c r="G16" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F16)</f>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="F17" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E17,D17,C17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_1YD#0002</v>
+        <v>EUR_YC1YRH_1YD#0004</v>
       </c>
       <c r="G17" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F17)</f>
@@ -3577,7 +3577,7 @@
       </c>
       <c r="H3" s="169" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_TND#0002</v>
+        <v>EUR_YCSTDRH_TND#0004</v>
       </c>
       <c r="I3" s="168" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="H4" s="166" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_SND#0002</v>
+        <v>EUR_YCSTDRH_SND#0004</v>
       </c>
       <c r="I4" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="H3" s="169" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCRH_TND#0002</v>
+        <v>EUR_YCRH_TND#0004</v>
       </c>
       <c r="I3" s="168" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -3758,7 +3758,7 @@
       </c>
       <c r="H4" s="166" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCRH_SND#0002</v>
+        <v>EUR_YCRH_SND#0004</v>
       </c>
       <c r="I4" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -3877,7 +3877,7 @@
       </c>
       <c r="H3" s="169" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_TND#0002</v>
+        <v>EUR_YCONRH_TND#0004</v>
       </c>
       <c r="I3" s="168" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -3909,7 +3909,7 @@
       </c>
       <c r="H4" s="166" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_SND#0002</v>
+        <v>EUR_YCONRH_SND#0004</v>
       </c>
       <c r="I4" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -4033,7 +4033,7 @@
       </c>
       <c r="H3" s="169" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_T1F1#0002</v>
+        <v>EUR_YC1MRH_T1F1#0004</v>
       </c>
       <c r="I3" s="168" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="H4" s="166" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_TOM1F1#0002</v>
+        <v>EUR_YC1MRH_TOM1F1#0004</v>
       </c>
       <c r="I4" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="H3" s="169" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_T3F1#0002</v>
+        <v>EUR_YC3MRH_T3F1#0004</v>
       </c>
       <c r="I3" s="168" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -4225,7 +4225,7 @@
       </c>
       <c r="H4" s="166" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_TOM3F1#0002</v>
+        <v>EUR_YC3MRH_TOM3F1#0004</v>
       </c>
       <c r="I4" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -4260,7 +4260,7 @@
       </c>
       <c r="H5" s="184" t="str">
         <f>_xll.qlFraRateHelper(G5,F5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1x4F#0002</v>
+        <v>EUR_YC3MRH_1x4F#0004</v>
       </c>
       <c r="I5" s="183" t="str">
         <f>_xll.ohRangeRetrieveError(H5)</f>
@@ -4295,7 +4295,7 @@
       </c>
       <c r="H6" s="184" t="str">
         <f>_xll.qlFraRateHelper(G6,F6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2x5F#0002</v>
+        <v>EUR_YC3MRH_2x5F#0004</v>
       </c>
       <c r="I6" s="183" t="str">
         <f>_xll.ohRangeRetrieveError(H6)</f>
@@ -4330,7 +4330,7 @@
       </c>
       <c r="H7" s="184" t="str">
         <f>_xll.qlFraRateHelper(G7,F7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3x6F#0002</v>
+        <v>EUR_YC3MRH_3x6F#0004</v>
       </c>
       <c r="I7" s="183" t="str">
         <f>_xll.ohRangeRetrieveError(H7)</f>
@@ -4365,7 +4365,7 @@
       </c>
       <c r="H8" s="184" t="str">
         <f>_xll.qlFraRateHelper(G8,F8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_4x7F#0002</v>
+        <v>EUR_YC3MRH_4x7F#0004</v>
       </c>
       <c r="I8" s="183" t="str">
         <f>_xll.ohRangeRetrieveError(H8)</f>
@@ -4400,7 +4400,7 @@
       </c>
       <c r="H9" s="184" t="str">
         <f>_xll.qlFraRateHelper(G9,F9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_5x8F#0002</v>
+        <v>EUR_YC3MRH_5x8F#0004</v>
       </c>
       <c r="I9" s="183" t="str">
         <f>_xll.ohRangeRetrieveError(H9)</f>
@@ -4435,7 +4435,7 @@
       </c>
       <c r="H10" s="166" t="str">
         <f>_xll.qlFraRateHelper(G10,F10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_6x9F#0002</v>
+        <v>EUR_YC3MRH_6x9F#0004</v>
       </c>
       <c r="I10" s="182" t="str">
         <f>_xll.ohRangeRetrieveError(H10)</f>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="I3" s="169" t="str">
         <f>_xll.qlFraRateHelper(H3,G3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_T6F1#0002</v>
+        <v>EUR_YC6MRH_T6F1#0004</v>
       </c>
       <c r="J3" s="168" t="str">
         <f>_xll.ohRangeRetrieveError(I3)</f>
@@ -4603,7 +4603,7 @@
       </c>
       <c r="I4" s="166" t="str">
         <f>_xll.qlFraRateHelper(H4,G4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_TOM6F1#0002</v>
+        <v>EUR_YC6MRH_TOM6F1#0004</v>
       </c>
       <c r="J4" s="165" t="str">
         <f>_xll.ohRangeRetrieveError(I4)</f>
@@ -4641,7 +4641,7 @@
       </c>
       <c r="I5" s="169" t="str">
         <f>_xll.qlFraRateHelper(H5,G5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_1x7F#0002</v>
+        <v>EUR_YC6MRH_1x7F#0004</v>
       </c>
       <c r="J5" s="189" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="I6" s="184" t="str">
         <f>_xll.qlFraRateHelper(H6,G6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_2x8F#0002</v>
+        <v>EUR_YC6MRH_2x8F#0004</v>
       </c>
       <c r="J6" s="183" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -4717,7 +4717,7 @@
       </c>
       <c r="I7" s="184" t="str">
         <f>_xll.qlFraRateHelper(H7,G7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_3x9F#0002</v>
+        <v>EUR_YC6MRH_3x9F#0004</v>
       </c>
       <c r="J7" s="183" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -4755,7 +4755,7 @@
       </c>
       <c r="I8" s="169" t="str">
         <f>_xll.qlFraRateHelper(H8,G8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_4x10F#0002</v>
+        <v>EUR_YC6MRH_4x10F#0004</v>
       </c>
       <c r="J8" s="189" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -4793,7 +4793,7 @@
       </c>
       <c r="I9" s="166" t="str">
         <f>_xll.qlFraRateHelper(H9,G9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_5x11F#0002</v>
+        <v>EUR_YC6MRH_5x11F#0004</v>
       </c>
       <c r="J9" s="182" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -4831,7 +4831,7 @@
       </c>
       <c r="I10" s="192" t="str">
         <f>_xll.qlFraRateHelper(H10,G10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_6x12F#0002</v>
+        <v>EUR_YC6MRH_6x12F#0004</v>
       </c>
       <c r="J10" s="191" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -5059,7 +5059,7 @@
       </c>
       <c r="I16" s="192" t="str">
         <f>_xll.qlFraRateHelper(H16,G16,B16,E16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_12x18F#0002</v>
+        <v>EUR_YC6MRH_12x18F#0004</v>
       </c>
       <c r="J16" s="191" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
@@ -5287,7 +5287,7 @@
       </c>
       <c r="I22" s="166" t="str">
         <f>_xll.qlFraRateHelper(H22,G22,B22,E22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_18x24F#0002</v>
+        <v>EUR_YC6MRH_18x24F#0004</v>
       </c>
       <c r="J22" s="182" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
@@ -5419,7 +5419,7 @@
       </c>
       <c r="I3" s="169" t="str">
         <f>_xll.qlFraRateHelper(H3,G3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_T12F1#0002</v>
+        <v>EUR_YC1YRH_T12F1#0004</v>
       </c>
       <c r="J3" s="206" t="str">
         <f>_xll.ohRangeRetrieveError(I3)</f>
@@ -5456,7 +5456,7 @@
       </c>
       <c r="I4" s="166" t="str">
         <f>_xll.qlFraRateHelper(H4,G4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_TOM12F1#0002</v>
+        <v>EUR_YC1YRH_TOM12F1#0004</v>
       </c>
       <c r="J4" s="205" t="str">
         <f>_xll.ohRangeRetrieveError(I4)</f>
@@ -5494,7 +5494,7 @@
       </c>
       <c r="I5" s="184" t="str">
         <f>_xll.qlFraRateHelper(H5,G5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_1x13F#0002</v>
+        <v>EUR_YC1YRH_1x13F#0004</v>
       </c>
       <c r="J5" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -5532,7 +5532,7 @@
       </c>
       <c r="I6" s="184" t="str">
         <f>_xll.qlFraRateHelper(H6,G6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_2x14F#0002</v>
+        <v>EUR_YC1YRH_2x14F#0004</v>
       </c>
       <c r="J6" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -5570,7 +5570,7 @@
       </c>
       <c r="I7" s="184" t="str">
         <f>_xll.qlFraRateHelper(H7,G7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_3x15F#0002</v>
+        <v>EUR_YC1YRH_3x15F#0004</v>
       </c>
       <c r="J7" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -5608,7 +5608,7 @@
       </c>
       <c r="I8" s="184" t="str">
         <f>_xll.qlFraRateHelper(H8,G8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_4x16F#0002</v>
+        <v>EUR_YC1YRH_4x16F#0004</v>
       </c>
       <c r="J8" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -5646,7 +5646,7 @@
       </c>
       <c r="I9" s="184" t="str">
         <f>_xll.qlFraRateHelper(H9,G9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_5x17F#0002</v>
+        <v>EUR_YC1YRH_5x17F#0004</v>
       </c>
       <c r="J9" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="I10" s="184" t="str">
         <f>_xll.qlFraRateHelper(H10,G10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_6x18F#0002</v>
+        <v>EUR_YC1YRH_6x18F#0004</v>
       </c>
       <c r="J10" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -5722,7 +5722,7 @@
       </c>
       <c r="I11" s="184" t="str">
         <f>_xll.qlFraRateHelper(H11,G11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_7x19F#0002</v>
+        <v>EUR_YC1YRH_7x19F#0004</v>
       </c>
       <c r="J11" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
@@ -5760,7 +5760,7 @@
       </c>
       <c r="I12" s="184" t="str">
         <f>_xll.qlFraRateHelper(H12,G12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_8x20F#0002</v>
+        <v>EUR_YC1YRH_8x20F#0004</v>
       </c>
       <c r="J12" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
@@ -5798,7 +5798,7 @@
       </c>
       <c r="I13" s="184" t="str">
         <f>_xll.qlFraRateHelper(H13,G13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_9x21F#0002</v>
+        <v>EUR_YC1YRH_9x21F#0004</v>
       </c>
       <c r="J13" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
@@ -5836,7 +5836,7 @@
       </c>
       <c r="I14" s="184" t="str">
         <f>_xll.qlFraRateHelper(H14,G14,B14,E14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_10x22F#0002</v>
+        <v>EUR_YC1YRH_10x22F#0004</v>
       </c>
       <c r="J14" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
@@ -5874,7 +5874,7 @@
       </c>
       <c r="I15" s="184" t="str">
         <f>_xll.qlFraRateHelper(H15,G15,B15,E15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_11x23F#0002</v>
+        <v>EUR_YC1YRH_11x23F#0004</v>
       </c>
       <c r="J15" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I15)</f>
@@ -5912,7 +5912,7 @@
       </c>
       <c r="I16" s="192" t="str">
         <f>_xll.qlFraRateHelper(H16,G16,B16,E16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_12x24F#0002</v>
+        <v>EUR_YC1YRH_12x24F#0004</v>
       </c>
       <c r="J16" s="204" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
@@ -5950,7 +5950,7 @@
       </c>
       <c r="I17" s="169" t="str">
         <f>_xll.qlFraRateHelper(H17,G17,B17,E17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_13x25F#0002</v>
+        <v>EUR_YC1YRH_13x25F#0004</v>
       </c>
       <c r="J17" s="203" t="str">
         <f>_xll.ohRangeRetrieveError(I17)</f>
@@ -5988,7 +5988,7 @@
       </c>
       <c r="I18" s="184" t="str">
         <f>_xll.qlFraRateHelper(H18,G18,B18,E18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_14x26F#0002</v>
+        <v>EUR_YC1YRH_14x26F#0004</v>
       </c>
       <c r="J18" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I18)</f>
@@ -6026,7 +6026,7 @@
       </c>
       <c r="I19" s="184" t="str">
         <f>_xll.qlFraRateHelper(H19,G19,B19,E19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_15x27F#0002</v>
+        <v>EUR_YC1YRH_15x27F#0004</v>
       </c>
       <c r="J19" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I19)</f>
@@ -6064,7 +6064,7 @@
       </c>
       <c r="I20" s="184" t="str">
         <f>_xll.qlFraRateHelper(H20,G20,B20,E20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_16x28F#0002</v>
+        <v>EUR_YC1YRH_16x28F#0004</v>
       </c>
       <c r="J20" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I20)</f>
@@ -6102,7 +6102,7 @@
       </c>
       <c r="I21" s="184" t="str">
         <f>_xll.qlFraRateHelper(H21,G21,B21,E21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_17x29F#0002</v>
+        <v>EUR_YC1YRH_17x29F#0004</v>
       </c>
       <c r="J21" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I21)</f>
@@ -6140,7 +6140,7 @@
       </c>
       <c r="I22" s="184" t="str">
         <f>_xll.qlFraRateHelper(H22,G22,B22,E22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_18x30F#0002</v>
+        <v>EUR_YC1YRH_18x30F#0004</v>
       </c>
       <c r="J22" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
@@ -6178,7 +6178,7 @@
       </c>
       <c r="I23" s="184" t="str">
         <f>_xll.qlFraRateHelper(H23,G23,B23,E23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_19x31F#0002</v>
+        <v>EUR_YC1YRH_19x31F#0004</v>
       </c>
       <c r="J23" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I23)</f>
@@ -6216,7 +6216,7 @@
       </c>
       <c r="I24" s="184" t="str">
         <f>_xll.qlFraRateHelper(H24,G24,B24,E24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_20x32F#0002</v>
+        <v>EUR_YC1YRH_20x32F#0004</v>
       </c>
       <c r="J24" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I24)</f>
@@ -6254,7 +6254,7 @@
       </c>
       <c r="I25" s="184" t="str">
         <f>_xll.qlFraRateHelper(H25,G25,B25,E25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_21x33F#0002</v>
+        <v>EUR_YC1YRH_21x33F#0004</v>
       </c>
       <c r="J25" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I25)</f>
@@ -6292,7 +6292,7 @@
       </c>
       <c r="I26" s="184" t="str">
         <f>_xll.qlFraRateHelper(H26,G26,B26,E26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_22x34F#0002</v>
+        <v>EUR_YC1YRH_22x34F#0004</v>
       </c>
       <c r="J26" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I26)</f>
@@ -6330,7 +6330,7 @@
       </c>
       <c r="I27" s="166" t="str">
         <f>_xll.qlFraRateHelper(H27,G27,B27,E27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_23x35F#0002</v>
+        <v>EUR_YC1YRH_23x35F#0004</v>
       </c>
       <c r="J27" s="201" t="str">
         <f>_xll.ohRangeRetrieveError(I27)</f>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="I28" s="169" t="str">
         <f>_xll.qlFraRateHelper(H28,G28,B28,E28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_25x37F#0002</v>
+        <v>EUR_YC1YRH_25x37F#0004</v>
       </c>
       <c r="J28" s="203" t="str">
         <f>_xll.ohRangeRetrieveError(I28)</f>
@@ -6406,7 +6406,7 @@
       </c>
       <c r="I29" s="184" t="str">
         <f>_xll.qlFraRateHelper(H29,G29,B29,E29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_26x38F#0002</v>
+        <v>EUR_YC1YRH_26x38F#0004</v>
       </c>
       <c r="J29" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I29)</f>
@@ -6444,7 +6444,7 @@
       </c>
       <c r="I30" s="184" t="str">
         <f>_xll.qlFraRateHelper(H30,G30,B30,E30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_27x39F#0002</v>
+        <v>EUR_YC1YRH_27x39F#0004</v>
       </c>
       <c r="J30" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I30)</f>
@@ -6482,7 +6482,7 @@
       </c>
       <c r="I31" s="184" t="str">
         <f>_xll.qlFraRateHelper(H31,G31,B31,E31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_28x40F#0002</v>
+        <v>EUR_YC1YRH_28x40F#0004</v>
       </c>
       <c r="J31" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I31)</f>
@@ -6520,7 +6520,7 @@
       </c>
       <c r="I32" s="184" t="str">
         <f>_xll.qlFraRateHelper(H32,G32,B32,E32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_29x41F#0002</v>
+        <v>EUR_YC1YRH_29x41F#0004</v>
       </c>
       <c r="J32" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I32)</f>
@@ -6558,7 +6558,7 @@
       </c>
       <c r="I33" s="184" t="str">
         <f>_xll.qlFraRateHelper(H33,G33,B33,E33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_30x42F#0002</v>
+        <v>EUR_YC1YRH_30x42F#0004</v>
       </c>
       <c r="J33" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I33)</f>
@@ -6596,7 +6596,7 @@
       </c>
       <c r="I34" s="184" t="str">
         <f>_xll.qlFraRateHelper(H34,G34,B34,E34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_31x43F#0002</v>
+        <v>EUR_YC1YRH_31x43F#0004</v>
       </c>
       <c r="J34" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I34)</f>
@@ -6634,7 +6634,7 @@
       </c>
       <c r="I35" s="184" t="str">
         <f>_xll.qlFraRateHelper(H35,G35,B35,E35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_32x44F#0002</v>
+        <v>EUR_YC1YRH_32x44F#0004</v>
       </c>
       <c r="J35" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I35)</f>
@@ -6672,7 +6672,7 @@
       </c>
       <c r="I36" s="184" t="str">
         <f>_xll.qlFraRateHelper(H36,G36,B36,E36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_33x45F#0002</v>
+        <v>EUR_YC1YRH_33x45F#0004</v>
       </c>
       <c r="J36" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I36)</f>
@@ -6710,7 +6710,7 @@
       </c>
       <c r="I37" s="184" t="str">
         <f>_xll.qlFraRateHelper(H37,G37,B37,E37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_34x46F#0002</v>
+        <v>EUR_YC1YRH_34x46F#0004</v>
       </c>
       <c r="J37" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I37)</f>
@@ -6748,7 +6748,7 @@
       </c>
       <c r="I38" s="166" t="str">
         <f>_xll.qlFraRateHelper(H38,G38,B38,E38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_35x47F#0002</v>
+        <v>EUR_YC1YRH_35x47F#0004</v>
       </c>
       <c r="J38" s="201" t="str">
         <f>_xll.ohRangeRetrieveError(I38)</f>
@@ -6786,7 +6786,7 @@
       </c>
       <c r="I39" s="184" t="str">
         <f>_xll.qlFraRateHelper(H39,G39,B39,E39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_37x49F#0002</v>
+        <v>EUR_YC1YRH_37x49F#0004</v>
       </c>
       <c r="J39" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I39)</f>
@@ -6824,7 +6824,7 @@
       </c>
       <c r="I40" s="184" t="str">
         <f>_xll.qlFraRateHelper(H40,G40,B40,E40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_38x50F#0002</v>
+        <v>EUR_YC1YRH_38x50F#0004</v>
       </c>
       <c r="J40" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I40)</f>
@@ -6862,7 +6862,7 @@
       </c>
       <c r="I41" s="184" t="str">
         <f>_xll.qlFraRateHelper(H41,G41,B41,E41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_39x51F#0002</v>
+        <v>EUR_YC1YRH_39x51F#0004</v>
       </c>
       <c r="J41" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I41)</f>
@@ -6900,7 +6900,7 @@
       </c>
       <c r="I42" s="184" t="str">
         <f>_xll.qlFraRateHelper(H42,G42,B42,E42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_40x52F#0002</v>
+        <v>EUR_YC1YRH_40x52F#0004</v>
       </c>
       <c r="J42" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I42)</f>
@@ -6938,7 +6938,7 @@
       </c>
       <c r="I43" s="184" t="str">
         <f>_xll.qlFraRateHelper(H43,G43,B43,E43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_41x53F#0002</v>
+        <v>EUR_YC1YRH_41x53F#0004</v>
       </c>
       <c r="J43" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I43)</f>
@@ -6976,7 +6976,7 @@
       </c>
       <c r="I44" s="184" t="str">
         <f>_xll.qlFraRateHelper(H44,G44,B44,E44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_42x54F#0002</v>
+        <v>EUR_YC1YRH_42x54F#0004</v>
       </c>
       <c r="J44" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I44)</f>
@@ -7014,7 +7014,7 @@
       </c>
       <c r="I45" s="184" t="str">
         <f>_xll.qlFraRateHelper(H45,G45,B45,E45,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_43x55F#0002</v>
+        <v>EUR_YC1YRH_43x55F#0004</v>
       </c>
       <c r="J45" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I45)</f>
@@ -7052,7 +7052,7 @@
       </c>
       <c r="I46" s="184" t="str">
         <f>_xll.qlFraRateHelper(H46,G46,B46,E46,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_44x56F#0002</v>
+        <v>EUR_YC1YRH_44x56F#0004</v>
       </c>
       <c r="J46" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I46)</f>
@@ -7090,7 +7090,7 @@
       </c>
       <c r="I47" s="184" t="str">
         <f>_xll.qlFraRateHelper(H47,G47,B47,E47,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_45x57F#0002</v>
+        <v>EUR_YC1YRH_45x57F#0004</v>
       </c>
       <c r="J47" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I47)</f>
@@ -7128,7 +7128,7 @@
       </c>
       <c r="I48" s="184" t="str">
         <f>_xll.qlFraRateHelper(H48,G48,B48,E48,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_46x58F#0002</v>
+        <v>EUR_YC1YRH_46x58F#0004</v>
       </c>
       <c r="J48" s="202" t="str">
         <f>_xll.ohRangeRetrieveError(I48)</f>
@@ -7166,7 +7166,7 @@
       </c>
       <c r="I49" s="166" t="str">
         <f>_xll.qlFraRateHelper(H49,G49,B49,E49,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1YRH_47x59F#0002</v>
+        <v>EUR_YC1YRH_47x59F#0004</v>
       </c>
       <c r="J49" s="201" t="str">
         <f>_xll.ohRangeRetrieveError(I49)</f>
@@ -7323,7 +7323,7 @@
       </c>
       <c r="L4" s="228" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YCSTDRH_AB6E_ibor6M#0004</v>
+        <v>EUR_YCSTDRH_AB6E_ibor6M#0006</v>
       </c>
       <c r="M4" s="227" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -9240,7 +9240,7 @@
       </c>
       <c r="L4" s="246" t="str">
         <f>_xll.qlEonia(K4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON_ibor#0004</v>
+        <v>EUR_YCRH_EON_ibor#0006</v>
       </c>
       <c r="M4" s="245" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -9299,7 +9299,7 @@
       </c>
       <c r="L6" s="238" t="str">
         <f>_xll.qlOISRateHelper(K6,2,C6,J6,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EONSW#0002</v>
+        <v>EUR_YCRH_EONSW#0006</v>
       </c>
       <c r="M6" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -9351,7 +9351,7 @@
       </c>
       <c r="L7" s="238" t="str">
         <f>_xll.qlOISRateHelper(K7,2,C7,J7,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON2W#0002</v>
+        <v>EUR_YCRH_EON2W#0006</v>
       </c>
       <c r="M7" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -9403,7 +9403,7 @@
       </c>
       <c r="L8" s="238" t="str">
         <f>_xll.qlOISRateHelper(K8,2,C8,J8,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON3W#0002</v>
+        <v>EUR_YCRH_EON3W#0006</v>
       </c>
       <c r="M8" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -9455,7 +9455,7 @@
       </c>
       <c r="L9" s="238" t="str">
         <f>_xll.qlOISRateHelper(K9,2,C9,J9,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON1M#0002</v>
+        <v>EUR_YCRH_EON1M#0006</v>
       </c>
       <c r="M9" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -9507,7 +9507,7 @@
       </c>
       <c r="L10" s="238" t="str">
         <f>_xll.qlOISRateHelper(K10,2,C10,J10,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON2M#0002</v>
+        <v>EUR_YCRH_EON2M#0006</v>
       </c>
       <c r="M10" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -9559,7 +9559,7 @@
       </c>
       <c r="L11" s="238" t="str">
         <f>_xll.qlOISRateHelper(K11,2,C11,J11,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON3M#0002</v>
+        <v>EUR_YCRH_EON3M#0006</v>
       </c>
       <c r="M11" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -9611,7 +9611,7 @@
       </c>
       <c r="L12" s="238" t="str">
         <f>_xll.qlOISRateHelper(K12,2,C12,J12,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON4M#0002</v>
+        <v>EUR_YCRH_EON4M#0006</v>
       </c>
       <c r="M12" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -9663,7 +9663,7 @@
       </c>
       <c r="L13" s="238" t="str">
         <f>_xll.qlOISRateHelper(K13,2,C13,J13,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON5M#0002</v>
+        <v>EUR_YCRH_EON5M#0006</v>
       </c>
       <c r="M13" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -9715,7 +9715,7 @@
       </c>
       <c r="L14" s="238" t="str">
         <f>_xll.qlOISRateHelper(K14,2,C14,J14,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON6M#0002</v>
+        <v>EUR_YCRH_EON6M#0006</v>
       </c>
       <c r="M14" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -9767,7 +9767,7 @@
       </c>
       <c r="L15" s="238" t="str">
         <f>_xll.qlOISRateHelper(K15,2,C15,J15,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON7M#0002</v>
+        <v>EUR_YCRH_EON7M#0006</v>
       </c>
       <c r="M15" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -9819,7 +9819,7 @@
       </c>
       <c r="L16" s="238" t="str">
         <f>_xll.qlOISRateHelper(K16,2,C16,J16,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON8M#0002</v>
+        <v>EUR_YCRH_EON8M#0006</v>
       </c>
       <c r="M16" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -9871,7 +9871,7 @@
       </c>
       <c r="L17" s="238" t="str">
         <f>_xll.qlOISRateHelper(K17,2,C17,J17,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON9M#0002</v>
+        <v>EUR_YCRH_EON9M#0006</v>
       </c>
       <c r="M17" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -9923,7 +9923,7 @@
       </c>
       <c r="L18" s="238" t="str">
         <f>_xll.qlOISRateHelper(K18,2,C18,J18,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON10M#0002</v>
+        <v>EUR_YCRH_EON10M#0006</v>
       </c>
       <c r="M18" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -9975,7 +9975,7 @@
       </c>
       <c r="L19" s="238" t="str">
         <f>_xll.qlOISRateHelper(K19,2,C19,J19,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON11M#0002</v>
+        <v>EUR_YCRH_EON11M#0006</v>
       </c>
       <c r="M19" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -10027,7 +10027,7 @@
       </c>
       <c r="L20" s="238" t="str">
         <f>_xll.qlOISRateHelper(K20,2,C20,J20,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON1Y#0002</v>
+        <v>EUR_YCRH_EON1Y#0006</v>
       </c>
       <c r="M20" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -10079,7 +10079,7 @@
       </c>
       <c r="L21" s="238" t="str">
         <f>_xll.qlOISRateHelper(K21,2,C21,J21,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON15M#0002</v>
+        <v>EUR_YCRH_EON15M#0006</v>
       </c>
       <c r="M21" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -10131,7 +10131,7 @@
       </c>
       <c r="L22" s="238" t="str">
         <f>_xll.qlOISRateHelper(K22,2,C22,J22,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON18M#0002</v>
+        <v>EUR_YCRH_EON18M#0006</v>
       </c>
       <c r="M22" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -10183,7 +10183,7 @@
       </c>
       <c r="L23" s="238" t="str">
         <f>_xll.qlOISRateHelper(K23,2,C23,J23,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON21M#0002</v>
+        <v>EUR_YCRH_EON21M#0006</v>
       </c>
       <c r="M23" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -10235,7 +10235,7 @@
       </c>
       <c r="L24" s="238" t="str">
         <f>_xll.qlOISRateHelper(K24,2,C24,J24,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON2Y#0002</v>
+        <v>EUR_YCRH_EON2Y#0006</v>
       </c>
       <c r="M24" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -10287,7 +10287,7 @@
       </c>
       <c r="L25" s="238" t="str">
         <f>_xll.qlOISRateHelper(K25,2,C25,J25,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON3Y#0002</v>
+        <v>EUR_YCRH_EON3Y#0006</v>
       </c>
       <c r="M25" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -10339,7 +10339,7 @@
       </c>
       <c r="L26" s="238" t="str">
         <f>_xll.qlOISRateHelper(K26,2,C26,J26,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON4Y#0002</v>
+        <v>EUR_YCRH_EON4Y#0006</v>
       </c>
       <c r="M26" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -10391,7 +10391,7 @@
       </c>
       <c r="L27" s="238" t="str">
         <f>_xll.qlOISRateHelper(K27,2,C27,J27,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON5Y#0002</v>
+        <v>EUR_YCRH_EON5Y#0006</v>
       </c>
       <c r="M27" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -10443,7 +10443,7 @@
       </c>
       <c r="L28" s="238" t="str">
         <f>_xll.qlOISRateHelper(K28,2,C28,J28,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON6Y#0002</v>
+        <v>EUR_YCRH_EON6Y#0006</v>
       </c>
       <c r="M28" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -10495,7 +10495,7 @@
       </c>
       <c r="L29" s="238" t="str">
         <f>_xll.qlOISRateHelper(K29,2,C29,J29,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON7Y#0002</v>
+        <v>EUR_YCRH_EON7Y#0006</v>
       </c>
       <c r="M29" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -10547,7 +10547,7 @@
       </c>
       <c r="L30" s="238" t="str">
         <f>_xll.qlOISRateHelper(K30,2,C30,J30,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON8Y#0002</v>
+        <v>EUR_YCRH_EON8Y#0006</v>
       </c>
       <c r="M30" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -10599,7 +10599,7 @@
       </c>
       <c r="L31" s="238" t="str">
         <f>_xll.qlOISRateHelper(K31,2,C31,J31,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON9Y#0002</v>
+        <v>EUR_YCRH_EON9Y#0006</v>
       </c>
       <c r="M31" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -10651,7 +10651,7 @@
       </c>
       <c r="L32" s="238" t="str">
         <f>_xll.qlOISRateHelper(K32,2,C32,J32,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON10Y#0002</v>
+        <v>EUR_YCRH_EON10Y#0006</v>
       </c>
       <c r="M32" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -10703,7 +10703,7 @@
       </c>
       <c r="L33" s="238" t="str">
         <f>_xll.qlOISRateHelper(K33,2,C33,J33,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON11Y#0002</v>
+        <v>EUR_YCRH_EON11Y#0006</v>
       </c>
       <c r="M33" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -10755,7 +10755,7 @@
       </c>
       <c r="L34" s="238" t="str">
         <f>_xll.qlOISRateHelper(K34,2,C34,J34,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON12Y#0002</v>
+        <v>EUR_YCRH_EON12Y#0006</v>
       </c>
       <c r="M34" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -10807,7 +10807,7 @@
       </c>
       <c r="L35" s="238" t="str">
         <f>_xll.qlOISRateHelper(K35,2,C35,J35,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON15Y#0002</v>
+        <v>EUR_YCRH_EON15Y#0006</v>
       </c>
       <c r="M35" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -10859,7 +10859,7 @@
       </c>
       <c r="L36" s="238" t="str">
         <f>_xll.qlOISRateHelper(K36,2,C36,J36,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON20Y#0002</v>
+        <v>EUR_YCRH_EON20Y#0006</v>
       </c>
       <c r="M36" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -10911,7 +10911,7 @@
       </c>
       <c r="L37" s="238" t="str">
         <f>_xll.qlOISRateHelper(K37,2,C37,J37,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON25Y#0002</v>
+        <v>EUR_YCRH_EON25Y#0006</v>
       </c>
       <c r="M37" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -10963,7 +10963,7 @@
       </c>
       <c r="L38" s="238" t="str">
         <f>_xll.qlOISRateHelper(K38,2,C38,J38,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_EON30Y#0002</v>
+        <v>EUR_YCRH_EON30Y#0006</v>
       </c>
       <c r="M38" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -11034,7 +11034,7 @@
       </c>
       <c r="L40" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K40,B40,B41,J40,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_ECBOISDEC12#0002</v>
+        <v>EUR_YCRH_ECBOISDEC12#0006</v>
       </c>
       <c r="M40" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -11087,7 +11087,7 @@
       </c>
       <c r="L41" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K41,B41,B42,J41,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_ECBOISJAN13#0002</v>
+        <v>EUR_YCRH_ECBOISJAN13#0006</v>
       </c>
       <c r="M41" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -11140,7 +11140,7 @@
       </c>
       <c r="L42" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K42,B42,B43,J42,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_ECBOISFEB13#0002</v>
+        <v>EUR_YCRH_ECBOISFEB13#0006</v>
       </c>
       <c r="M42" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>
@@ -11193,7 +11193,7 @@
       </c>
       <c r="L43" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K43,B43,B44,J43,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_ECBOISMAR13#0002</v>
+        <v>EUR_YCRH_ECBOISMAR13#0006</v>
       </c>
       <c r="M43" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L43)</f>
@@ -11246,7 +11246,7 @@
       </c>
       <c r="L44" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K44,B44,B45,J44,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_ECBOISAPR13#0002</v>
+        <v>EUR_YCRH_ECBOISAPR13#0006</v>
       </c>
       <c r="M44" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -11299,7 +11299,7 @@
       </c>
       <c r="L45" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K45,B45,B46,J45,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_ECBOISMAY13#0002</v>
+        <v>EUR_YCRH_ECBOISMAY13#0006</v>
       </c>
       <c r="M45" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -11352,7 +11352,7 @@
       </c>
       <c r="L46" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K46,B46,B47,J46,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_ECBOISJUN13#0002</v>
+        <v>EUR_YCRH_ECBOISJUN13#0006</v>
       </c>
       <c r="M46" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -11405,7 +11405,7 @@
       </c>
       <c r="L47" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K47,B47,B48,J47,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_ECBOISJUL13#0002</v>
+        <v>EUR_YCRH_ECBOISJUL13#0006</v>
       </c>
       <c r="M47" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -11458,7 +11458,7 @@
       </c>
       <c r="L48" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K48,B48,B49,J48,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_ECBOISAUG13#0002</v>
+        <v>EUR_YCRH_ECBOISAUG13#0006</v>
       </c>
       <c r="M48" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -11511,7 +11511,7 @@
       </c>
       <c r="L49" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K49,B49,B50,J49,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_ECBOISSEP13#0002</v>
+        <v>EUR_YCRH_ECBOISSEP13#0006</v>
       </c>
       <c r="M49" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -11564,7 +11564,7 @@
       </c>
       <c r="L50" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K50,B50,B51,J50,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_ECBOISOCT13#0002</v>
+        <v>EUR_YCRH_ECBOISOCT13#0006</v>
       </c>
       <c r="M50" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>
@@ -11617,7 +11617,7 @@
       </c>
       <c r="L51" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K51,B51,B52,J51,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCRH_ECBOISNOV13#0002</v>
+        <v>EUR_YCRH_ECBOISNOV13#0006</v>
       </c>
       <c r="M51" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L51)</f>
@@ -12937,9 +12937,9 @@
         <f t="shared" ref="E2:E33" si="0">RateHelperPrefix&amp;"_"&amp;$B2&amp;$C2&amp;$D2</f>
         <v>EUR_YCONRH_OND</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E2,Trigger)</f>
-        <v>1E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="G2" s="33"/>
       <c r="H2" s="26" t="b">
@@ -12970,9 +12970,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YCONRH_TND</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E3,Trigger)</f>
-        <v>1E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="26" t="b">
@@ -13003,9 +13003,9 @@
         <f t="shared" si="0"/>
         <v>EUR_YCONRH_SND</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="33" t="e">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
-        <v>1E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="G4" s="33"/>
       <c r="H4" s="26" t="b">
@@ -17937,7 +17937,7 @@
   <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -18057,7 +18057,7 @@
       </c>
       <c r="L4" s="246" t="str">
         <f>_xll.qlEonia(K4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON_iborON#0004</v>
+        <v>EUR_YCONRH_EON_iborON#0006</v>
       </c>
       <c r="M4" s="245" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -18116,7 +18116,7 @@
       </c>
       <c r="L6" s="238" t="str">
         <f>_xll.qlOISRateHelper(K6,2,C6,J6,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EONSW#0002</v>
+        <v>EUR_YCONRH_EONSW#0006</v>
       </c>
       <c r="M6" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -18168,7 +18168,7 @@
       </c>
       <c r="L7" s="238" t="str">
         <f>_xll.qlOISRateHelper(K7,2,C7,J7,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON2W#0002</v>
+        <v>EUR_YCONRH_EON2W#0006</v>
       </c>
       <c r="M7" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -18220,7 +18220,7 @@
       </c>
       <c r="L8" s="238" t="str">
         <f>_xll.qlOISRateHelper(K8,2,C8,J8,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON3W#0002</v>
+        <v>EUR_YCONRH_EON3W#0006</v>
       </c>
       <c r="M8" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -18272,7 +18272,7 @@
       </c>
       <c r="L9" s="238" t="str">
         <f>_xll.qlOISRateHelper(K9,2,C9,J9,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON1M#0002</v>
+        <v>EUR_YCONRH_EON1M#0006</v>
       </c>
       <c r="M9" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -18324,7 +18324,7 @@
       </c>
       <c r="L10" s="238" t="str">
         <f>_xll.qlOISRateHelper(K10,2,C10,J10,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON2M#0002</v>
+        <v>EUR_YCONRH_EON2M#0006</v>
       </c>
       <c r="M10" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -18376,7 +18376,7 @@
       </c>
       <c r="L11" s="238" t="str">
         <f>_xll.qlOISRateHelper(K11,2,C11,J11,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON3M#0002</v>
+        <v>EUR_YCONRH_EON3M#0006</v>
       </c>
       <c r="M11" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -18428,7 +18428,7 @@
       </c>
       <c r="L12" s="238" t="str">
         <f>_xll.qlOISRateHelper(K12,2,C12,J12,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON4M#0002</v>
+        <v>EUR_YCONRH_EON4M#0006</v>
       </c>
       <c r="M12" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -18480,7 +18480,7 @@
       </c>
       <c r="L13" s="238" t="str">
         <f>_xll.qlOISRateHelper(K13,2,C13,J13,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON5M#0002</v>
+        <v>EUR_YCONRH_EON5M#0006</v>
       </c>
       <c r="M13" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -18532,7 +18532,7 @@
       </c>
       <c r="L14" s="238" t="str">
         <f>_xll.qlOISRateHelper(K14,2,C14,J14,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON6M#0002</v>
+        <v>EUR_YCONRH_EON6M#0006</v>
       </c>
       <c r="M14" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -18584,7 +18584,7 @@
       </c>
       <c r="L15" s="238" t="str">
         <f>_xll.qlOISRateHelper(K15,2,C15,J15,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON7M#0002</v>
+        <v>EUR_YCONRH_EON7M#0006</v>
       </c>
       <c r="M15" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -18636,7 +18636,7 @@
       </c>
       <c r="L16" s="238" t="str">
         <f>_xll.qlOISRateHelper(K16,2,C16,J16,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON8M#0002</v>
+        <v>EUR_YCONRH_EON8M#0006</v>
       </c>
       <c r="M16" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -18688,7 +18688,7 @@
       </c>
       <c r="L17" s="238" t="str">
         <f>_xll.qlOISRateHelper(K17,2,C17,J17,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON9M#0002</v>
+        <v>EUR_YCONRH_EON9M#0006</v>
       </c>
       <c r="M17" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -18740,7 +18740,7 @@
       </c>
       <c r="L18" s="238" t="str">
         <f>_xll.qlOISRateHelper(K18,2,C18,J18,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON10M#0002</v>
+        <v>EUR_YCONRH_EON10M#0006</v>
       </c>
       <c r="M18" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -18792,7 +18792,7 @@
       </c>
       <c r="L19" s="238" t="str">
         <f>_xll.qlOISRateHelper(K19,2,C19,J19,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON11M#0002</v>
+        <v>EUR_YCONRH_EON11M#0006</v>
       </c>
       <c r="M19" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -18844,7 +18844,7 @@
       </c>
       <c r="L20" s="238" t="str">
         <f>_xll.qlOISRateHelper(K20,2,C20,J20,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON1Y#0002</v>
+        <v>EUR_YCONRH_EON1Y#0006</v>
       </c>
       <c r="M20" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -18896,7 +18896,7 @@
       </c>
       <c r="L21" s="238" t="str">
         <f>_xll.qlOISRateHelper(K21,2,C21,J21,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON15M#0002</v>
+        <v>EUR_YCONRH_EON15M#0006</v>
       </c>
       <c r="M21" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -18948,7 +18948,7 @@
       </c>
       <c r="L22" s="238" t="str">
         <f>_xll.qlOISRateHelper(K22,2,C22,J22,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON18M#0002</v>
+        <v>EUR_YCONRH_EON18M#0006</v>
       </c>
       <c r="M22" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -19000,7 +19000,7 @@
       </c>
       <c r="L23" s="238" t="str">
         <f>_xll.qlOISRateHelper(K23,2,C23,J23,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON21M#0002</v>
+        <v>EUR_YCONRH_EON21M#0006</v>
       </c>
       <c r="M23" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -19052,7 +19052,7 @@
       </c>
       <c r="L24" s="238" t="str">
         <f>_xll.qlOISRateHelper(K24,2,C24,J24,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON2Y#0002</v>
+        <v>EUR_YCONRH_EON2Y#0006</v>
       </c>
       <c r="M24" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -19104,7 +19104,7 @@
       </c>
       <c r="L25" s="238" t="str">
         <f>_xll.qlOISRateHelper(K25,2,C25,J25,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON3Y#0002</v>
+        <v>EUR_YCONRH_EON3Y#0006</v>
       </c>
       <c r="M25" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -19156,7 +19156,7 @@
       </c>
       <c r="L26" s="238" t="str">
         <f>_xll.qlOISRateHelper(K26,2,C26,J26,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON4Y#0002</v>
+        <v>EUR_YCONRH_EON4Y#0006</v>
       </c>
       <c r="M26" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -19208,7 +19208,7 @@
       </c>
       <c r="L27" s="238" t="str">
         <f>_xll.qlOISRateHelper(K27,2,C27,J27,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON5Y#0002</v>
+        <v>EUR_YCONRH_EON5Y#0006</v>
       </c>
       <c r="M27" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -19260,7 +19260,7 @@
       </c>
       <c r="L28" s="238" t="str">
         <f>_xll.qlOISRateHelper(K28,2,C28,J28,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON6Y#0002</v>
+        <v>EUR_YCONRH_EON6Y#0006</v>
       </c>
       <c r="M28" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -19312,7 +19312,7 @@
       </c>
       <c r="L29" s="238" t="str">
         <f>_xll.qlOISRateHelper(K29,2,C29,J29,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON7Y#0002</v>
+        <v>EUR_YCONRH_EON7Y#0006</v>
       </c>
       <c r="M29" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -19364,7 +19364,7 @@
       </c>
       <c r="L30" s="238" t="str">
         <f>_xll.qlOISRateHelper(K30,2,C30,J30,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON8Y#0002</v>
+        <v>EUR_YCONRH_EON8Y#0006</v>
       </c>
       <c r="M30" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -19416,7 +19416,7 @@
       </c>
       <c r="L31" s="238" t="str">
         <f>_xll.qlOISRateHelper(K31,2,C31,J31,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON9Y#0002</v>
+        <v>EUR_YCONRH_EON9Y#0006</v>
       </c>
       <c r="M31" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -19468,7 +19468,7 @@
       </c>
       <c r="L32" s="238" t="str">
         <f>_xll.qlOISRateHelper(K32,2,C32,J32,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON10Y#0002</v>
+        <v>EUR_YCONRH_EON10Y#0006</v>
       </c>
       <c r="M32" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -19520,7 +19520,7 @@
       </c>
       <c r="L33" s="238" t="str">
         <f>_xll.qlOISRateHelper(K33,2,C33,J33,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON11Y#0002</v>
+        <v>EUR_YCONRH_EON11Y#0006</v>
       </c>
       <c r="M33" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -19572,7 +19572,7 @@
       </c>
       <c r="L34" s="238" t="str">
         <f>_xll.qlOISRateHelper(K34,2,C34,J34,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON12Y#0002</v>
+        <v>EUR_YCONRH_EON12Y#0006</v>
       </c>
       <c r="M34" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -19624,7 +19624,7 @@
       </c>
       <c r="L35" s="238" t="str">
         <f>_xll.qlOISRateHelper(K35,2,C35,J35,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON15Y#0002</v>
+        <v>EUR_YCONRH_EON15Y#0006</v>
       </c>
       <c r="M35" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -19676,7 +19676,7 @@
       </c>
       <c r="L36" s="238" t="str">
         <f>_xll.qlOISRateHelper(K36,2,C36,J36,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON20Y#0002</v>
+        <v>EUR_YCONRH_EON20Y#0006</v>
       </c>
       <c r="M36" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -19728,7 +19728,7 @@
       </c>
       <c r="L37" s="238" t="str">
         <f>_xll.qlOISRateHelper(K37,2,C37,J37,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON25Y#0002</v>
+        <v>EUR_YCONRH_EON25Y#0006</v>
       </c>
       <c r="M37" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -19780,7 +19780,7 @@
       </c>
       <c r="L38" s="238" t="str">
         <f>_xll.qlOISRateHelper(K38,2,C38,J38,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_EON30Y#0002</v>
+        <v>EUR_YCONRH_EON30Y#0006</v>
       </c>
       <c r="M38" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -19851,7 +19851,7 @@
       </c>
       <c r="L40" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K40,B40,B41,J40,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_ECBOISDEC12#0002</v>
+        <v>EUR_YCONRH_ECBOISDEC12#0006</v>
       </c>
       <c r="M40" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -19904,7 +19904,7 @@
       </c>
       <c r="L41" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K41,B41,B42,J41,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_ECBOISJAN13#0002</v>
+        <v>EUR_YCONRH_ECBOISJAN13#0006</v>
       </c>
       <c r="M41" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -19957,7 +19957,7 @@
       </c>
       <c r="L42" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K42,B42,B43,J42,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_ECBOISFEB13#0002</v>
+        <v>EUR_YCONRH_ECBOISFEB13#0006</v>
       </c>
       <c r="M42" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>
@@ -20010,7 +20010,7 @@
       </c>
       <c r="L43" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K43,B43,B44,J43,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_ECBOISMAR13#0002</v>
+        <v>EUR_YCONRH_ECBOISMAR13#0006</v>
       </c>
       <c r="M43" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L43)</f>
@@ -20063,7 +20063,7 @@
       </c>
       <c r="L44" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K44,B44,B45,J44,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_ECBOISAPR13#0002</v>
+        <v>EUR_YCONRH_ECBOISAPR13#0006</v>
       </c>
       <c r="M44" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -20116,7 +20116,7 @@
       </c>
       <c r="L45" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K45,B45,B46,J45,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_ECBOISMAY13#0002</v>
+        <v>EUR_YCONRH_ECBOISMAY13#0006</v>
       </c>
       <c r="M45" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -20169,7 +20169,7 @@
       </c>
       <c r="L46" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K46,B46,B47,J46,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_ECBOISJUN13#0002</v>
+        <v>EUR_YCONRH_ECBOISJUN13#0006</v>
       </c>
       <c r="M46" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -20222,7 +20222,7 @@
       </c>
       <c r="L47" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K47,B47,B48,J47,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_ECBOISJUL13#0002</v>
+        <v>EUR_YCONRH_ECBOISJUL13#0006</v>
       </c>
       <c r="M47" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -20275,7 +20275,7 @@
       </c>
       <c r="L48" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K48,B48,B49,J48,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_ECBOISAUG13#0002</v>
+        <v>EUR_YCONRH_ECBOISAUG13#0006</v>
       </c>
       <c r="M48" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -20328,7 +20328,7 @@
       </c>
       <c r="L49" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K49,B49,B50,J49,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_ECBOISSEP13#0002</v>
+        <v>EUR_YCONRH_ECBOISSEP13#0006</v>
       </c>
       <c r="M49" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -20381,7 +20381,7 @@
       </c>
       <c r="L50" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K50,B50,B51,J50,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_ECBOISOCT13#0002</v>
+        <v>EUR_YCONRH_ECBOISOCT13#0006</v>
       </c>
       <c r="M50" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>
@@ -20434,7 +20434,7 @@
       </c>
       <c r="L51" s="238" t="str">
         <f>_xll.qlDatedOISRateHelper(K51,B51,B52,J51,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_ECBOISNOV13#0002</v>
+        <v>EUR_YCONRH_ECBOISNOV13#0006</v>
       </c>
       <c r="M51" s="115" t="str">
         <f>_xll.ohRangeRetrieveError(L51)</f>
@@ -21832,7 +21832,7 @@
       </c>
       <c r="L4" s="228" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC1MRH_xX1S_ibor1M#0004</v>
+        <v>EUR_YC1MRH_xX1S_ibor1M#0006</v>
       </c>
       <c r="M4" s="227" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -21893,7 +21893,7 @@
       </c>
       <c r="L6" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_2X1S#0002</v>
+        <v>EUR_YC1MRH_2X1S#0006</v>
       </c>
       <c r="M6" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -21938,7 +21938,7 @@
       </c>
       <c r="L7" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K7,$J7,$C7,Calendar,$F7,$G7,$H7,$L$4,$I7,B7,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_3X1S#0002</v>
+        <v>EUR_YC1MRH_3X1S#0006</v>
       </c>
       <c r="M7" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -21983,7 +21983,7 @@
       </c>
       <c r="L8" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K8,$J8,$C8,Calendar,$F8,$G8,$H8,$L$4,$I8,B8,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_4X1S#0002</v>
+        <v>EUR_YC1MRH_4X1S#0006</v>
       </c>
       <c r="M8" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -22028,7 +22028,7 @@
       </c>
       <c r="L9" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K9,$J9,$C9,Calendar,$F9,$G9,$H9,$L$4,$I9,B9,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_5X1S#0002</v>
+        <v>EUR_YC1MRH_5X1S#0006</v>
       </c>
       <c r="M9" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -22073,7 +22073,7 @@
       </c>
       <c r="L10" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_6X1S#0002</v>
+        <v>EUR_YC1MRH_6X1S#0006</v>
       </c>
       <c r="M10" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -22118,7 +22118,7 @@
       </c>
       <c r="L11" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_7X1S#0002</v>
+        <v>EUR_YC1MRH_7X1S#0006</v>
       </c>
       <c r="M11" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -22163,7 +22163,7 @@
       </c>
       <c r="L12" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_8X1S#0002</v>
+        <v>EUR_YC1MRH_8X1S#0006</v>
       </c>
       <c r="M12" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -22208,7 +22208,7 @@
       </c>
       <c r="L13" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_9X1S#0002</v>
+        <v>EUR_YC1MRH_9X1S#0006</v>
       </c>
       <c r="M13" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -22253,7 +22253,7 @@
       </c>
       <c r="L14" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_10X1S#0002</v>
+        <v>EUR_YC1MRH_10X1S#0006</v>
       </c>
       <c r="M14" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -22298,7 +22298,7 @@
       </c>
       <c r="L15" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_11X1S#0002</v>
+        <v>EUR_YC1MRH_11X1S#0006</v>
       </c>
       <c r="M15" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -22343,7 +22343,7 @@
       </c>
       <c r="L16" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_12X1S#0002</v>
+        <v>EUR_YC1MRH_12X1S#0006</v>
       </c>
       <c r="M16" s="132" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -22524,7 +22524,7 @@
       </c>
       <c r="L4" s="228" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>EUR_YC3MRH_AB3E_ibor3M#0004</v>
+        <v>EUR_YC3MRH_AB3E_ibor3M#0006</v>
       </c>
       <c r="M4" s="227" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -24347,7 +24347,7 @@
       </c>
       <c r="L44" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K44,$J44,$E44&amp;"M",Calendar,$F44,$G44,$H44,$L$4,$I44,B44,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1S12#0002</v>
+        <v>EUR_YC3MRH_1S12#0006</v>
       </c>
       <c r="M44" s="211" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -24392,7 +24392,7 @@
       </c>
       <c r="L45" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K45,$J45,$E45&amp;"M",Calendar,$F45,$G45,$H45,$L$4,$I45,B45,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2S12#0002</v>
+        <v>EUR_YC3MRH_2S12#0006</v>
       </c>
       <c r="M45" s="211" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -24437,7 +24437,7 @@
       </c>
       <c r="L46" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K46,$J46,$E46&amp;"M",Calendar,$F46,$G46,$H46,$L$4,$I46,B46,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3S12#0002</v>
+        <v>EUR_YC3MRH_3S12#0006</v>
       </c>
       <c r="M46" s="211" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -24482,7 +24482,7 @@
       </c>
       <c r="L47" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K47,$J47,$E47&amp;"M",Calendar,$F47,$G47,$H47,$L$4,$I47,B47,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_4S12#0002</v>
+        <v>EUR_YC3MRH_4S12#0006</v>
       </c>
       <c r="M47" s="211" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -24527,7 +24527,7 @@
       </c>
       <c r="L48" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K48,$J48,$E48&amp;"M",Calendar,$F48,$G48,$H48,$L$4,$I48,B48,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1S24#0002</v>
+        <v>EUR_YC3MRH_1S24#0006</v>
       </c>
       <c r="M48" s="211" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -24572,7 +24572,7 @@
       </c>
       <c r="L49" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K49,$J49,$E49&amp;"M",Calendar,$F49,$G49,$H49,$L$4,$I49,B49,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2S24#0002</v>
+        <v>EUR_YC3MRH_2S24#0006</v>
       </c>
       <c r="M49" s="211" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -24617,7 +24617,7 @@
       </c>
       <c r="L50" s="212" t="str">
         <f>_xll.qlSwapRateHelper2(K50,$J50,$E50&amp;"M",Calendar,$F50,$G50,$H50,$L$4,$I50,B50,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1S36#0002</v>
+        <v>EUR_YC3MRH_1S36#0006</v>
       </c>
       <c r="M50" s="211" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>
@@ -24706,9 +24706,9 @@
       <c r="H1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="3" t="e">
         <f t="array" ref="I1:I126">_xll.qlPiecewiseYieldCurveData(YieldCurve)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="L1" s="93">
         <v>1</v>
@@ -24729,9 +24729,9 @@
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
         <v>EUR_YCONRH_OND</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="10" t="e">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>1E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="F2" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -24745,8 +24745,8 @@
         <f>_xll.qlRateHelperLatestDate($D2)</f>
         <v>41619</v>
       </c>
-      <c r="I2" s="3">
-        <v>0.99999722222993825</v>
+      <c r="I2" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="L2" s="93">
         <v>1</v>
@@ -24769,9 +24769,9 @@
       <c r="D3" s="11" t="str">
         <v>EUR_YCONRH_TND</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="10" t="e">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>1E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="F3" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -24785,8 +24785,8 @@
         <f>_xll.qlRateHelperLatestDate($D3)</f>
         <v>41620</v>
       </c>
-      <c r="I3" s="3">
-        <v>0.99999444446759256</v>
+      <c r="I3" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J37" si="0">H3-H2</f>
@@ -24813,9 +24813,9 @@
       <c r="D4" s="11" t="str">
         <v>EUR_YCONRH_SND</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="10" t="e">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>1E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="F4" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -24829,8 +24829,8 @@
         <f>_xll.qlRateHelperLatestDate($D4)</f>
         <v>41621</v>
       </c>
-      <c r="I4" s="3">
-        <v>0.9999916667129628</v>
+      <c r="I4" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="0"/>
@@ -24873,8 +24873,8 @@
         <f>_xll.qlRateHelperLatestDate($D5)</f>
         <v>41627</v>
       </c>
-      <c r="I5" s="3">
-        <v>0.99997344502524632</v>
+      <c r="I5" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="0"/>
@@ -24918,8 +24918,8 @@
         <f>_xll.qlRateHelperLatestDate($D6)</f>
         <v>41635</v>
       </c>
-      <c r="I6" s="3">
-        <v>0.9999502799968969</v>
+      <c r="I6" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="0"/>
@@ -24936,7 +24936,7 @@
     <row r="7" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_RateHelpersSelected#0002</v>
+        <v>EUR_YCONRH_RateHelpersSelected#0004</v>
       </c>
       <c r="B7" s="12" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -24964,8 +24964,8 @@
         <f>_xll.qlRateHelperLatestDate($D7)</f>
         <v>41641</v>
       </c>
-      <c r="I7" s="3">
-        <v>0.99993261530087985</v>
+      <c r="I7" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="0"/>
@@ -25002,8 +25002,8 @@
         <f>_xll.qlRateHelperLatestDate($D8)</f>
         <v>41652</v>
       </c>
-      <c r="I8" s="3">
-        <v>0.99990023164576625</v>
+      <c r="I8" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="0"/>
@@ -25040,8 +25040,8 @@
         <f>_xll.qlRateHelperLatestDate($D9)</f>
         <v>41682</v>
       </c>
-      <c r="I9" s="3">
-        <v>0.99980331540047429</v>
+      <c r="I9" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="0"/>
@@ -25078,8 +25078,8 @@
         <f>_xll.qlRateHelperLatestDate($D10)</f>
         <v>41710</v>
       </c>
-      <c r="I10" s="3">
-        <v>0.99970702869684225</v>
+      <c r="I10" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="0"/>
@@ -25116,8 +25116,8 @@
         <f>_xll.qlRateHelperLatestDate($D11)</f>
         <v>41743</v>
       </c>
-      <c r="I11" s="3">
-        <v>0.99959485642386103</v>
+      <c r="I11" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="0"/>
@@ -25154,8 +25154,8 @@
         <f>_xll.qlRateHelperLatestDate($D12)</f>
         <v>41771</v>
       </c>
-      <c r="I12" s="3">
-        <v>0.99949555736574058</v>
+      <c r="I12" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="0"/>
@@ -25192,8 +25192,8 @@
         <f>_xll.qlRateHelperLatestDate($D13)</f>
         <v>41802</v>
       </c>
-      <c r="I13" s="3">
-        <v>0.99936795180269578</v>
+      <c r="I13" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="0"/>
@@ -25230,8 +25230,8 @@
         <f>_xll.qlRateHelperLatestDate($D14)</f>
         <v>41834</v>
       </c>
-      <c r="I14" s="3">
-        <v>0.99923413831435071</v>
+      <c r="I14" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="0"/>
@@ -25268,8 +25268,8 @@
         <f>_xll.qlRateHelperLatestDate($D15)</f>
         <v>41863</v>
       </c>
-      <c r="I15" s="3">
-        <v>0.99909750468276359</v>
+      <c r="I15" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="0"/>
@@ -25306,8 +25306,8 @@
         <f>_xll.qlRateHelperLatestDate($D16)</f>
         <v>41894</v>
       </c>
-      <c r="I16" s="3">
-        <v>0.99892243420861437</v>
+      <c r="I16" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="0"/>
@@ -25344,8 +25344,8 @@
         <f>_xll.qlRateHelperLatestDate($D17)</f>
         <v>41925</v>
       </c>
-      <c r="I17" s="3">
-        <v>0.99875058384462934</v>
+      <c r="I17" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="0"/>
@@ -25382,8 +25382,8 @@
         <f>_xll.qlRateHelperLatestDate($D18)</f>
         <v>41955</v>
       </c>
-      <c r="I18" s="3">
-        <v>0.99855416876722491</v>
+      <c r="I18" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="0"/>
@@ -25420,8 +25420,8 @@
         <f>_xll.qlRateHelperLatestDate($D19)</f>
         <v>41985</v>
       </c>
-      <c r="I19" s="3">
-        <v>0.99835464695996101</v>
+      <c r="I19" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="0"/>
@@ -25458,8 +25458,8 @@
         <f>_xll.qlRateHelperLatestDate($D20)</f>
         <v>42075</v>
       </c>
-      <c r="I20" s="3">
-        <v>0.99766041825925966</v>
+      <c r="I20" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="0"/>
@@ -25496,8 +25496,8 @@
         <f>_xll.qlRateHelperLatestDate($D21)</f>
         <v>42167</v>
       </c>
-      <c r="I21" s="3">
-        <v>0.99682564618501346</v>
+      <c r="I21" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="0"/>
@@ -25534,8 +25534,8 @@
         <f>_xll.qlRateHelperLatestDate($D22)</f>
         <v>42261</v>
       </c>
-      <c r="I22" s="3">
-        <v>0.99582158730107229</v>
+      <c r="I22" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" si="0"/>
@@ -25572,8 +25572,8 @@
         <f>_xll.qlRateHelperLatestDate($D23)</f>
         <v>42352</v>
       </c>
-      <c r="I23" s="3">
-        <v>0.99466546780230192</v>
+      <c r="I23" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="0"/>
@@ -25610,8 +25610,8 @@
         <f>_xll.qlRateHelperLatestDate($D24)</f>
         <v>42716</v>
       </c>
-      <c r="I24" s="3">
-        <v>0.98744218583387156</v>
+      <c r="I24" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="0"/>
@@ -25648,8 +25648,8 @@
         <f>_xll.qlRateHelperLatestDate($D25)</f>
         <v>43081</v>
       </c>
-      <c r="I25" s="3">
-        <v>0.97495248750322139</v>
+      <c r="I25" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="0"/>
@@ -25686,8 +25686,8 @@
         <f>_xll.qlRateHelperLatestDate($D26)</f>
         <v>43446</v>
       </c>
-      <c r="I26" s="3">
-        <v>0.95767931200207901</v>
+      <c r="I26" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J26" s="1">
         <f t="shared" si="0"/>
@@ -25724,8 +25724,8 @@
         <f>_xll.qlRateHelperLatestDate($D27)</f>
         <v>43811</v>
       </c>
-      <c r="I27" s="3">
-        <v>0.93791377028792011</v>
+      <c r="I27" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J27" s="1">
         <f t="shared" si="0"/>
@@ -25762,8 +25762,8 @@
         <f>_xll.qlRateHelperLatestDate($D28)</f>
         <v>44179</v>
       </c>
-      <c r="I28" s="3">
-        <v>0.91595762445272833</v>
+      <c r="I28" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J28" s="1">
         <f t="shared" si="0"/>
@@ -25800,8 +25800,8 @@
         <f>_xll.qlRateHelperLatestDate($D29)</f>
         <v>44543</v>
       </c>
-      <c r="I29" s="3">
-        <v>0.89263658304891269</v>
+      <c r="I29" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J29" s="1">
         <f t="shared" si="0"/>
@@ -25838,8 +25838,8 @@
         <f>_xll.qlRateHelperLatestDate($D30)</f>
         <v>44907</v>
       </c>
-      <c r="I30" s="3">
-        <v>0.86771637982000427</v>
+      <c r="I30" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" si="0"/>
@@ -25876,8 +25876,8 @@
         <f>_xll.qlRateHelperLatestDate($D31)</f>
         <v>45272</v>
       </c>
-      <c r="I31" s="3">
-        <v>0.84183446952600005</v>
+      <c r="I31" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" si="0"/>
@@ -25914,8 +25914,8 @@
         <f>_xll.qlRateHelperLatestDate($D32)</f>
         <v>45638</v>
       </c>
-      <c r="I32" s="3">
-        <v>0.81583825653245678</v>
+      <c r="I32" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="0"/>
@@ -25952,8 +25952,8 @@
         <f>_xll.qlRateHelperLatestDate($D33)</f>
         <v>46003</v>
       </c>
-      <c r="I33" s="3">
-        <v>0.79020313310282519</v>
+      <c r="I33" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J33" s="1">
         <f t="shared" si="0"/>
@@ -25990,8 +25990,8 @@
         <f>_xll.qlRateHelperLatestDate($D34)</f>
         <v>47099</v>
       </c>
-      <c r="I34" s="3">
-        <v>0.7180679579396908</v>
+      <c r="I34" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="0"/>
@@ -26028,8 +26028,8 @@
         <f>_xll.qlRateHelperLatestDate($D35)</f>
         <v>48925</v>
       </c>
-      <c r="I35" s="3">
-        <v>0.62409093322419695</v>
+      <c r="I35" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J35" s="1">
         <f t="shared" si="0"/>
@@ -26066,8 +26066,8 @@
         <f>_xll.qlRateHelperLatestDate($D36)</f>
         <v>50752</v>
       </c>
-      <c r="I36" s="3">
-        <v>0.55098020271125092</v>
+      <c r="I36" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J36" s="1">
         <f t="shared" si="0"/>
@@ -26104,8 +26104,8 @@
         <f>_xll.qlRateHelperLatestDate($D37)</f>
         <v>52579</v>
       </c>
-      <c r="I37" s="3">
-        <v>0.48973558874081424</v>
+      <c r="I37" s="3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="J37" s="1">
         <f t="shared" si="0"/>
@@ -26140,7 +26140,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I38" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="39" spans="3:14" x14ac:dyDescent="0.2">
@@ -26164,7 +26164,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I39" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="40" spans="3:14" x14ac:dyDescent="0.2">
@@ -26188,7 +26188,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I40" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="41" spans="3:14" x14ac:dyDescent="0.2">
@@ -26212,7 +26212,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I41" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="42" spans="3:14" x14ac:dyDescent="0.2">
@@ -26236,7 +26236,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I42" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="43" spans="3:14" x14ac:dyDescent="0.2">
@@ -26260,7 +26260,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I43" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="44" spans="3:14" x14ac:dyDescent="0.2">
@@ -26284,7 +26284,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I44" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="45" spans="3:14" x14ac:dyDescent="0.2">
@@ -26308,7 +26308,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I45" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="46" spans="3:14" x14ac:dyDescent="0.2">
@@ -26332,7 +26332,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I46" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="47" spans="3:14" x14ac:dyDescent="0.2">
@@ -26356,7 +26356,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I47" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="48" spans="3:14" x14ac:dyDescent="0.2">
@@ -26380,7 +26380,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I48" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="49" spans="4:9" x14ac:dyDescent="0.2">
@@ -26404,7 +26404,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I49" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="50" spans="4:9" x14ac:dyDescent="0.2">
@@ -26428,7 +26428,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I50" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="51" spans="4:9" x14ac:dyDescent="0.2">
@@ -26452,7 +26452,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I51" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.2">
@@ -26476,7 +26476,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I52" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="53" spans="4:9" x14ac:dyDescent="0.2">
@@ -26500,7 +26500,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I53" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="54" spans="4:9" x14ac:dyDescent="0.2">
@@ -26524,7 +26524,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I54" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="55" spans="4:9" x14ac:dyDescent="0.2">
@@ -26548,7 +26548,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I55" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="56" spans="4:9" x14ac:dyDescent="0.2">
@@ -26572,7 +26572,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I56" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="57" spans="4:9" x14ac:dyDescent="0.2">
@@ -26596,7 +26596,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I57" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="58" spans="4:9" x14ac:dyDescent="0.2">
@@ -26620,7 +26620,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I58" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="59" spans="4:9" x14ac:dyDescent="0.2">
@@ -26644,7 +26644,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I59" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="60" spans="4:9" x14ac:dyDescent="0.2">
@@ -26668,7 +26668,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I60" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="61" spans="4:9" x14ac:dyDescent="0.2">
@@ -26692,7 +26692,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I61" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="62" spans="4:9" x14ac:dyDescent="0.2">
@@ -26716,7 +26716,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I62" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="63" spans="4:9" x14ac:dyDescent="0.2">
@@ -26740,7 +26740,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I63" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="64" spans="4:9" x14ac:dyDescent="0.2">
@@ -26764,7 +26764,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I64" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="65" spans="4:9" x14ac:dyDescent="0.2">
@@ -26788,7 +26788,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I65" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="66" spans="4:9" x14ac:dyDescent="0.2">
@@ -26812,7 +26812,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I66" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="67" spans="4:9" x14ac:dyDescent="0.2">
@@ -26836,7 +26836,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I67" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="68" spans="4:9" x14ac:dyDescent="0.2">
@@ -26860,7 +26860,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I68" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="69" spans="4:9" x14ac:dyDescent="0.2">
@@ -26884,7 +26884,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I69" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="70" spans="4:9" x14ac:dyDescent="0.2">
@@ -26908,7 +26908,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I70" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="71" spans="4:9" x14ac:dyDescent="0.2">
@@ -26932,7 +26932,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I71" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="72" spans="4:9" x14ac:dyDescent="0.2">
@@ -26956,7 +26956,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I72" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="73" spans="4:9" x14ac:dyDescent="0.2">
@@ -26980,7 +26980,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I73" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="74" spans="4:9" x14ac:dyDescent="0.2">
@@ -27004,7 +27004,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I74" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="75" spans="4:9" x14ac:dyDescent="0.2">
@@ -27028,7 +27028,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I75" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="76" spans="4:9" x14ac:dyDescent="0.2">
@@ -27052,7 +27052,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I76" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="77" spans="4:9" x14ac:dyDescent="0.2">
@@ -27076,7 +27076,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I77" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="78" spans="4:9" x14ac:dyDescent="0.2">
@@ -27100,7 +27100,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I78" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="79" spans="4:9" x14ac:dyDescent="0.2">
@@ -27124,7 +27124,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I79" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="80" spans="4:9" x14ac:dyDescent="0.2">
@@ -27148,7 +27148,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I80" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="81" spans="4:9" x14ac:dyDescent="0.2">
@@ -27172,7 +27172,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I81" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="82" spans="4:9" x14ac:dyDescent="0.2">
@@ -27196,7 +27196,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I82" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="83" spans="4:9" x14ac:dyDescent="0.2">
@@ -27220,7 +27220,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I83" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="84" spans="4:9" x14ac:dyDescent="0.2">
@@ -27244,7 +27244,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I84" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="85" spans="4:9" x14ac:dyDescent="0.2">
@@ -27268,7 +27268,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I85" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="86" spans="4:9" x14ac:dyDescent="0.2">
@@ -27292,7 +27292,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I86" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="87" spans="4:9" x14ac:dyDescent="0.2">
@@ -27316,7 +27316,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I87" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="88" spans="4:9" x14ac:dyDescent="0.2">
@@ -27340,7 +27340,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I88" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="89" spans="4:9" x14ac:dyDescent="0.2">
@@ -27364,7 +27364,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I89" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="90" spans="4:9" x14ac:dyDescent="0.2">
@@ -27388,7 +27388,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I90" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="91" spans="4:9" x14ac:dyDescent="0.2">
@@ -27412,7 +27412,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I91" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="92" spans="4:9" x14ac:dyDescent="0.2">
@@ -27436,7 +27436,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I92" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="93" spans="4:9" x14ac:dyDescent="0.2">
@@ -27460,7 +27460,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I93" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="94" spans="4:9" x14ac:dyDescent="0.2">
@@ -27484,7 +27484,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I94" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="95" spans="4:9" x14ac:dyDescent="0.2">
@@ -27508,7 +27508,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I95" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="96" spans="4:9" x14ac:dyDescent="0.2">
@@ -27532,7 +27532,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I96" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="97" spans="4:9" x14ac:dyDescent="0.2">
@@ -27556,7 +27556,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I97" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="98" spans="4:9" x14ac:dyDescent="0.2">
@@ -27580,7 +27580,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I98" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="99" spans="4:9" x14ac:dyDescent="0.2">
@@ -27604,7 +27604,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I99" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="100" spans="4:9" x14ac:dyDescent="0.2">
@@ -27628,7 +27628,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I100" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="101" spans="4:9" x14ac:dyDescent="0.2">
@@ -27652,7 +27652,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I101" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="102" spans="4:9" x14ac:dyDescent="0.2">
@@ -27676,7 +27676,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I102" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="103" spans="4:9" x14ac:dyDescent="0.2">
@@ -27700,7 +27700,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I103" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="104" spans="4:9" x14ac:dyDescent="0.2">
@@ -27724,7 +27724,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I104" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="105" spans="4:9" x14ac:dyDescent="0.2">
@@ -27748,7 +27748,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I105" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="106" spans="4:9" x14ac:dyDescent="0.2">
@@ -27772,7 +27772,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I106" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="107" spans="4:9" x14ac:dyDescent="0.2">
@@ -27796,7 +27796,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I107" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="108" spans="4:9" x14ac:dyDescent="0.2">
@@ -27820,7 +27820,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I108" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="109" spans="4:9" x14ac:dyDescent="0.2">
@@ -27844,7 +27844,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I109" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="110" spans="4:9" x14ac:dyDescent="0.2">
@@ -27868,7 +27868,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I110" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="111" spans="4:9" x14ac:dyDescent="0.2">
@@ -27892,7 +27892,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I111" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="112" spans="4:9" x14ac:dyDescent="0.2">
@@ -27916,7 +27916,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I112" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="113" spans="4:9" x14ac:dyDescent="0.2">
@@ -27940,7 +27940,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I113" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="114" spans="4:9" x14ac:dyDescent="0.2">
@@ -27964,7 +27964,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I114" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="115" spans="4:9" x14ac:dyDescent="0.2">
@@ -27988,7 +27988,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I115" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="116" spans="4:9" x14ac:dyDescent="0.2">
@@ -28012,7 +28012,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I116" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="117" spans="4:9" x14ac:dyDescent="0.2">
@@ -28036,7 +28036,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I117" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="118" spans="4:9" x14ac:dyDescent="0.2">
@@ -28060,7 +28060,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I118" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="119" spans="4:9" x14ac:dyDescent="0.2">
@@ -28084,7 +28084,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I119" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="120" spans="4:9" x14ac:dyDescent="0.2">
@@ -28108,7 +28108,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I120" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="121" spans="4:9" x14ac:dyDescent="0.2">
@@ -28132,7 +28132,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I121" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="122" spans="4:9" x14ac:dyDescent="0.2">
@@ -28156,7 +28156,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I122" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="123" spans="4:9" x14ac:dyDescent="0.2">
@@ -28180,7 +28180,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I123" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="124" spans="4:9" x14ac:dyDescent="0.2">
@@ -28204,7 +28204,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I124" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="125" spans="4:9" x14ac:dyDescent="0.2">
@@ -28228,7 +28228,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I125" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="126" spans="4:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
@@ -28252,7 +28252,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I126" s="3" t="e">
-        <v>#N/A</v>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
@@ -28349,7 +28349,7 @@
       </c>
       <c r="F3" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E3,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_OND#0002</v>
+        <v>EUR_YCSTDRH_OND#0004</v>
       </c>
       <c r="G3" s="112" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -28376,7 +28376,7 @@
       </c>
       <c r="F4" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_SWD#0002</v>
+        <v>EUR_YCSTDRH_SWD#0004</v>
       </c>
       <c r="G4" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -28403,7 +28403,7 @@
       </c>
       <c r="F5" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_2WD#0002</v>
+        <v>EUR_YCSTDRH_2WD#0004</v>
       </c>
       <c r="G5" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -28430,7 +28430,7 @@
       </c>
       <c r="F6" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_3WD#0002</v>
+        <v>EUR_YCSTDRH_3WD#0004</v>
       </c>
       <c r="G6" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -28457,7 +28457,7 @@
       </c>
       <c r="F7" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_1MD#0002</v>
+        <v>EUR_YCSTDRH_1MD#0004</v>
       </c>
       <c r="G7" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -28484,7 +28484,7 @@
       </c>
       <c r="F8" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_2MD#0002</v>
+        <v>EUR_YCSTDRH_2MD#0004</v>
       </c>
       <c r="G8" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -28511,7 +28511,7 @@
       </c>
       <c r="F9" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_3MD#0002</v>
+        <v>EUR_YCSTDRH_3MD#0004</v>
       </c>
       <c r="G9" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -28538,7 +28538,7 @@
       </c>
       <c r="F10" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E10,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_4MD#0002</v>
+        <v>EUR_YCSTDRH_4MD#0004</v>
       </c>
       <c r="G10" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -28565,7 +28565,7 @@
       </c>
       <c r="F11" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E11,D11,C11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_5MD#0002</v>
+        <v>EUR_YCSTDRH_5MD#0004</v>
       </c>
       <c r="G11" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>
@@ -28592,7 +28592,7 @@
       </c>
       <c r="F12" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E12,D12,C12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_6MD#0002</v>
+        <v>EUR_YCSTDRH_6MD#0004</v>
       </c>
       <c r="G12" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F12)</f>
@@ -28619,7 +28619,7 @@
       </c>
       <c r="F13" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E13,D13,C13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_7MD#0002</v>
+        <v>EUR_YCSTDRH_7MD#0004</v>
       </c>
       <c r="G13" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F13)</f>
@@ -28646,7 +28646,7 @@
       </c>
       <c r="F14" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E14,D14,C14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_8MD#0002</v>
+        <v>EUR_YCSTDRH_8MD#0004</v>
       </c>
       <c r="G14" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F14)</f>
@@ -28673,7 +28673,7 @@
       </c>
       <c r="F15" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E15,D15,C15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_9MD#0002</v>
+        <v>EUR_YCSTDRH_9MD#0004</v>
       </c>
       <c r="G15" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F15)</f>
@@ -28700,7 +28700,7 @@
       </c>
       <c r="F16" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E16,D16,C16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_10MD#0002</v>
+        <v>EUR_YCSTDRH_10MD#0004</v>
       </c>
       <c r="G16" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F16)</f>
@@ -28727,7 +28727,7 @@
       </c>
       <c r="F17" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E17,D17,C17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_11MD#0002</v>
+        <v>EUR_YCSTDRH_11MD#0004</v>
       </c>
       <c r="G17" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F17)</f>
@@ -28754,7 +28754,7 @@
       </c>
       <c r="F18" s="106" t="str">
         <f>_xll.qlDepositRateHelper(E18,D18,C18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCSTDRH_1YD#0002</v>
+        <v>EUR_YCSTDRH_1YD#0004</v>
       </c>
       <c r="G18" s="105" t="str">
         <f>_xll.ohRangeRetrieveError(F18)</f>
@@ -28855,7 +28855,7 @@
       </c>
       <c r="F3" s="127" t="str">
         <f>_xll.qlDepositRateHelper(E3,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCRH_OND#0002</v>
+        <v>EUR_YCRH_OND#0004</v>
       </c>
       <c r="G3" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -28885,7 +28885,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -28958,7 +28960,7 @@
       </c>
       <c r="F3" s="127" t="str">
         <f>_xll.qlDepositRateHelper(E3,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YCONRH_OND#0002</v>
+        <v>EUR_YCONRH_OND#0004</v>
       </c>
       <c r="G3" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -29060,7 +29062,7 @@
       </c>
       <c r="F3" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E3,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_SWD#0002</v>
+        <v>EUR_YC1MRH_SWD#0004</v>
       </c>
       <c r="G3" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -29087,7 +29089,7 @@
       </c>
       <c r="F4" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_2WD#0002</v>
+        <v>EUR_YC1MRH_2WD#0004</v>
       </c>
       <c r="G4" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -29114,7 +29116,7 @@
       </c>
       <c r="F5" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_3WD#0002</v>
+        <v>EUR_YC1MRH_3WD#0004</v>
       </c>
       <c r="G5" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -29141,7 +29143,7 @@
       </c>
       <c r="F6" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC1MRH_1MD#0002</v>
+        <v>EUR_YC1MRH_1MD#0004</v>
       </c>
       <c r="G6" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -29245,7 +29247,7 @@
       </c>
       <c r="F3" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E3,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_SWD#0002</v>
+        <v>EUR_YC3MRH_SWD#0004</v>
       </c>
       <c r="G3" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -29272,7 +29274,7 @@
       </c>
       <c r="F4" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2WD#0002</v>
+        <v>EUR_YC3MRH_2WD#0004</v>
       </c>
       <c r="G4" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -29299,7 +29301,7 @@
       </c>
       <c r="F5" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3WD#0002</v>
+        <v>EUR_YC3MRH_3WD#0004</v>
       </c>
       <c r="G5" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -29326,7 +29328,7 @@
       </c>
       <c r="F6" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_1MD#0002</v>
+        <v>EUR_YC3MRH_1MD#0004</v>
       </c>
       <c r="G6" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -29353,7 +29355,7 @@
       </c>
       <c r="F7" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_2MD#0002</v>
+        <v>EUR_YC3MRH_2MD#0004</v>
       </c>
       <c r="G7" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -29380,7 +29382,7 @@
       </c>
       <c r="F8" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC3MRH_3MD#0002</v>
+        <v>EUR_YC3MRH_3MD#0004</v>
       </c>
       <c r="G8" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -29484,7 +29486,7 @@
       </c>
       <c r="F3" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E3,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_SWD#0002</v>
+        <v>EUR_YC6MRH_SWD#0004</v>
       </c>
       <c r="G3" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -29511,7 +29513,7 @@
       </c>
       <c r="F4" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_2WD#0002</v>
+        <v>EUR_YC6MRH_2WD#0004</v>
       </c>
       <c r="G4" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -29538,7 +29540,7 @@
       </c>
       <c r="F5" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_3WD#0002</v>
+        <v>EUR_YC6MRH_3WD#0004</v>
       </c>
       <c r="G5" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -29565,7 +29567,7 @@
       </c>
       <c r="F6" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_1MD#0002</v>
+        <v>EUR_YC6MRH_1MD#0004</v>
       </c>
       <c r="G6" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -29592,7 +29594,7 @@
       </c>
       <c r="F7" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_2MD#0002</v>
+        <v>EUR_YC6MRH_2MD#0004</v>
       </c>
       <c r="G7" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -29619,7 +29621,7 @@
       </c>
       <c r="F8" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_3MD#0002</v>
+        <v>EUR_YC6MRH_3MD#0004</v>
       </c>
       <c r="G8" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -29646,7 +29648,7 @@
       </c>
       <c r="F9" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_4MD#0002</v>
+        <v>EUR_YC6MRH_4MD#0004</v>
       </c>
       <c r="G9" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -29673,7 +29675,7 @@
       </c>
       <c r="F10" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E10,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_5MD#0002</v>
+        <v>EUR_YC6MRH_5MD#0004</v>
       </c>
       <c r="G10" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -29700,7 +29702,7 @@
       </c>
       <c r="F11" s="141" t="str">
         <f>_xll.qlDepositRateHelper(E11,D11,C11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>EUR_YC6MRH_6MD#0002</v>
+        <v>EUR_YC6MRH_6MD#0004</v>
       </c>
       <c r="G11" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>

</xml_diff>

<commit_message>
EURYCON - reconcile with R010202 prod
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_YCONBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_YCONBootstrapping.xlsx
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="190">
   <si>
     <t>Error</t>
   </si>
@@ -2415,7 +2415,7 @@
         <v>104</v>
       </c>
       <c r="D11" s="86">
-        <v>41662.585104166668</v>
+        <v>41663.415671296294</v>
       </c>
       <c r="E11" s="58"/>
       <c r="F11" s="57"/>
@@ -2654,11 +2654,11 @@
       <c r="B28" s="61"/>
       <c r="C28" s="63">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>52617</v>
+        <v>63576</v>
       </c>
       <c r="D28" s="62">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.48979097977701558</v>
+        <v>0.19963997166531142</v>
       </c>
       <c r="E28" s="58"/>
       <c r="F28" s="57"/>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="F2" s="33">
         <f>_xll.qlRateHelperQuoteValue($E2,Trigger)</f>
-        <v>1E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
       <c r="G2" s="33"/>
       <c r="H2" s="26" t="b">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="F3" s="33">
         <f>_xll.qlRateHelperQuoteValue($E3,Trigger)</f>
-        <v>1E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="26" t="b">
@@ -2854,7 +2854,7 @@
       </c>
       <c r="F4" s="27">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
-        <v>1E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="25" t="b">
@@ -4072,7 +4072,7 @@
       </c>
       <c r="F35" s="40">
         <f>_xll.qlRateHelperQuoteValue($E35,Trigger)</f>
-        <v>1.08E-3</v>
+        <v>1.99E-3</v>
       </c>
       <c r="G35" s="40" t="e">
         <f>_xll.qlSwapRateHelperSpread($E35,Trigger)</f>
@@ -4111,7 +4111,7 @@
       </c>
       <c r="F36" s="33">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
-        <v>1.06E-3</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="G36" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E36,Trigger)</f>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="F37" s="33">
         <f>_xll.qlRateHelperQuoteValue($E37,Trigger)</f>
-        <v>1.06E-3</v>
+        <v>2.0399999999999997E-3</v>
       </c>
       <c r="G37" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E37,Trigger)</f>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="F38" s="33">
         <f>_xll.qlRateHelperQuoteValue($E38,Trigger)</f>
-        <v>1.0600000000000002E-3</v>
+        <v>1.9599999999999999E-3</v>
       </c>
       <c r="G38" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E38,Trigger)</f>
@@ -4228,7 +4228,7 @@
       </c>
       <c r="F39" s="33">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
-        <v>1.1100000000000001E-3</v>
+        <v>1.9300000000000001E-3</v>
       </c>
       <c r="G39" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E39,Trigger)</f>
@@ -4267,7 +4267,7 @@
       </c>
       <c r="F40" s="33">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
-        <v>1.15E-3</v>
+        <v>1.9E-3</v>
       </c>
       <c r="G40" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E40,Trigger)</f>
@@ -4306,7 +4306,7 @@
       </c>
       <c r="F41" s="33">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
-        <v>1.17E-3</v>
+        <v>1.8400000000000001E-3</v>
       </c>
       <c r="G41" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E41,Trigger)</f>
@@ -4345,7 +4345,7 @@
       </c>
       <c r="F42" s="33">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
-        <v>1.1899999999999999E-3</v>
+        <v>1.7899999999999999E-3</v>
       </c>
       <c r="G42" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E42,Trigger)</f>
@@ -4384,7 +4384,7 @@
       </c>
       <c r="F43" s="33">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
-        <v>1.24E-3</v>
+        <v>1.7499999999999998E-3</v>
       </c>
       <c r="G43" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E43,Trigger)</f>
@@ -4423,7 +4423,7 @@
       </c>
       <c r="F44" s="33">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
-        <v>1.2800000000000001E-3</v>
+        <v>1.72E-3</v>
       </c>
       <c r="G44" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E44,Trigger)</f>
@@ -4462,7 +4462,7 @@
       </c>
       <c r="F45" s="33">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
-        <v>1.33E-3</v>
+        <v>1.6900000000000001E-3</v>
       </c>
       <c r="G45" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E45,Trigger)</f>
@@ -4501,7 +4501,7 @@
       </c>
       <c r="F46" s="33">
         <f>_xll.qlRateHelperQuoteValue($E46,Trigger)</f>
-        <v>1.4100000000000002E-3</v>
+        <v>1.66E-3</v>
       </c>
       <c r="G46" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E46,Trigger)</f>
@@ -4540,7 +4540,7 @@
       </c>
       <c r="F47" s="33">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
-        <v>1.47E-3</v>
+        <v>1.64E-3</v>
       </c>
       <c r="G47" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E47,Trigger)</f>
@@ -4579,7 +4579,7 @@
       </c>
       <c r="F48" s="33">
         <f>_xll.qlRateHelperQuoteValue($E48,Trigger)</f>
-        <v>1.5499999999999999E-3</v>
+        <v>1.6200000000000001E-3</v>
       </c>
       <c r="G48" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E48,Trigger)</f>
@@ -4618,7 +4618,7 @@
       </c>
       <c r="F49" s="33">
         <f>_xll.qlRateHelperQuoteValue($E49,Trigger)</f>
-        <v>1.6200000000000001E-3</v>
+        <v>1.6100000000000001E-3</v>
       </c>
       <c r="G49" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E49,Trigger)</f>
@@ -4660,7 +4660,7 @@
       </c>
       <c r="F50" s="33">
         <f>_xll.qlRateHelperQuoteValue($E50,Trigger)</f>
-        <v>1.8500000000000001E-3</v>
+        <v>1.6100000000000001E-3</v>
       </c>
       <c r="G50" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E50,Trigger)</f>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="F51" s="33">
         <f>_xll.qlRateHelperQuoteValue($E51,Trigger)</f>
-        <v>2.0900000000000003E-3</v>
+        <v>1.66E-3</v>
       </c>
       <c r="G51" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E51,Trigger)</f>
@@ -4744,7 +4744,7 @@
       </c>
       <c r="F52" s="33">
         <f>_xll.qlRateHelperQuoteValue($E52,Trigger)</f>
-        <v>2.3499999999999997E-3</v>
+        <v>1.7699999999999999E-3</v>
       </c>
       <c r="G52" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E52,Trigger)</f>
@@ -4786,7 +4786,7 @@
       </c>
       <c r="F53" s="33">
         <f>_xll.qlRateHelperQuoteValue($E53,Trigger)</f>
-        <v>2.63E-3</v>
+        <v>1.9500000000000001E-3</v>
       </c>
       <c r="G53" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E53,Trigger)</f>
@@ -4828,7 +4828,7 @@
       </c>
       <c r="F54" s="33">
         <f>_xll.qlRateHelperQuoteValue($E54,Trigger)</f>
-        <v>4.15E-3</v>
+        <v>3.32E-3</v>
       </c>
       <c r="G54" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E54,Trigger)</f>
@@ -4870,7 +4870,7 @@
       </c>
       <c r="F55" s="33">
         <f>_xll.qlRateHelperQuoteValue($E55,Trigger)</f>
-        <v>6.2399999999999999E-3</v>
+        <v>5.3900000000000007E-3</v>
       </c>
       <c r="G55" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E55,Trigger)</f>
@@ -4912,7 +4912,7 @@
       </c>
       <c r="F56" s="33">
         <f>_xll.qlRateHelperQuoteValue($E56,Trigger)</f>
-        <v>8.4899999999999993E-3</v>
+        <v>7.5900000000000004E-3</v>
       </c>
       <c r="G56" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E56,Trigger)</f>
@@ -4954,7 +4954,7 @@
       </c>
       <c r="F57" s="33">
         <f>_xll.qlRateHelperQuoteValue($E57,Trigger)</f>
-        <v>1.0459999999999999E-2</v>
+        <v>9.75E-3</v>
       </c>
       <c r="G57" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E57,Trigger)</f>
@@ -4996,7 +4996,7 @@
       </c>
       <c r="F58" s="33">
         <f>_xll.qlRateHelperQuoteValue($E58,Trigger)</f>
-        <v>1.2229999999999998E-2</v>
+        <v>1.1779999999999999E-2</v>
       </c>
       <c r="G58" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E58,Trigger)</f>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="F59" s="33">
         <f>_xll.qlRateHelperQuoteValue($E59,Trigger)</f>
-        <v>1.3809999999999999E-2</v>
+        <v>1.3640000000000001E-2</v>
       </c>
       <c r="G59" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E59,Trigger)</f>
@@ -5080,7 +5080,7 @@
       </c>
       <c r="F60" s="33">
         <f>_xll.qlRateHelperQuoteValue($E60,Trigger)</f>
-        <v>1.529E-2</v>
+        <v>1.5309999999999999E-2</v>
       </c>
       <c r="G60" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E60,Trigger)</f>
@@ -5122,7 +5122,7 @@
       </c>
       <c r="F61" s="33">
         <f>_xll.qlRateHelperQuoteValue($E61,Trigger)</f>
-        <v>1.6640000000000002E-2</v>
+        <v>1.6799999999999999E-2</v>
       </c>
       <c r="G61" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E61,Trigger)</f>
@@ -5164,7 +5164,7 @@
       </c>
       <c r="F62" s="33">
         <f>_xll.qlRateHelperQuoteValue($E62,Trigger)</f>
-        <v>1.7819999999999999E-2</v>
+        <v>1.8100000000000002E-2</v>
       </c>
       <c r="G62" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E62,Trigger)</f>
@@ -5207,7 +5207,7 @@
       </c>
       <c r="F63" s="33">
         <f>_xll.qlRateHelperQuoteValue($E63,Trigger)</f>
-        <v>1.8839999999999999E-2</v>
+        <v>1.925E-2</v>
       </c>
       <c r="G63" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E63,Trigger)</f>
@@ -5336,7 +5336,7 @@
       </c>
       <c r="F66" s="33">
         <f>_xll.qlRateHelperQuoteValue($E66,Trigger)</f>
-        <v>2.1049999999999999E-2</v>
+        <v>2.1789999999999997E-2</v>
       </c>
       <c r="G66" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E66,Trigger)</f>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="F71" s="33">
         <f>_xll.qlRateHelperQuoteValue($E71,Trigger)</f>
-        <v>2.2450000000000001E-2</v>
+        <v>2.367E-2</v>
       </c>
       <c r="G71" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E71,Trigger)</f>
@@ -5766,7 +5766,7 @@
       </c>
       <c r="F76" s="33">
         <f>_xll.qlRateHelperQuoteValue($E76,Trigger)</f>
-        <v>2.2809999999999997E-2</v>
+        <v>2.4310000000000002E-2</v>
       </c>
       <c r="G76" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E76,Trigger)</f>
@@ -5981,7 +5981,7 @@
       </c>
       <c r="F81" s="33">
         <f>_xll.qlRateHelperQuoteValue($E81,Trigger)</f>
-        <v>2.2889999999999997E-2</v>
+        <v>2.4479999999999998E-2</v>
       </c>
       <c r="G81" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E81,Trigger)</f>
@@ -6065,9 +6065,9 @@
         <f t="shared" si="5"/>
         <v>EUR_YCONRH_EON40Y</v>
       </c>
-      <c r="F83" s="33" t="e">
+      <c r="F83" s="33">
         <f>_xll.qlRateHelperQuoteValue($E83,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.495E-2</v>
       </c>
       <c r="G83" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E83,Trigger)</f>
@@ -6075,7 +6075,7 @@
       </c>
       <c r="H83" s="26" t="b">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I83" s="26">
         <v>50</v>
@@ -6083,13 +6083,13 @@
       <c r="J83" s="26">
         <v>1</v>
       </c>
-      <c r="K83" s="32" t="e">
+      <c r="K83" s="32">
         <f>_xll.qlRateHelperEarliestDate($E83,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L83" s="31" t="e">
+        <v>41660</v>
+      </c>
+      <c r="L83" s="31">
         <f>_xll.qlRateHelperLatestDate($E83,Trigger)</f>
-        <v>#NUM!</v>
+        <v>56270</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.2">
@@ -6108,9 +6108,9 @@
         <f t="shared" si="5"/>
         <v>EUR_YCONRH_EON50Y</v>
       </c>
-      <c r="F84" s="33" t="e">
+      <c r="F84" s="33">
         <f>_xll.qlRateHelperQuoteValue($E84,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.528E-2</v>
       </c>
       <c r="G84" s="33" t="e">
         <f>_xll.qlSwapRateHelperSpread($E84,Trigger)</f>
@@ -6118,7 +6118,7 @@
       </c>
       <c r="H84" s="26" t="b">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I84" s="26">
         <v>50</v>
@@ -6126,13 +6126,13 @@
       <c r="J84" s="26">
         <v>1</v>
       </c>
-      <c r="K84" s="32" t="e">
+      <c r="K84" s="32">
         <f>_xll.qlRateHelperEarliestDate($E84,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L84" s="31" t="e">
+        <v>41660</v>
+      </c>
+      <c r="L84" s="31">
         <f>_xll.qlRateHelperLatestDate($E84,Trigger)</f>
-        <v>#NUM!</v>
+        <v>59922</v>
       </c>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.2">
@@ -6151,9 +6151,9 @@
         <f t="shared" si="5"/>
         <v>EUR_YCONRH_EON60Y</v>
       </c>
-      <c r="F85" s="27" t="e">
+      <c r="F85" s="27">
         <f>_xll.qlRateHelperQuoteValue($E85,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.5510000000000001E-2</v>
       </c>
       <c r="G85" s="27" t="e">
         <f>_xll.qlSwapRateHelperSpread($E85,Trigger)</f>
@@ -6161,7 +6161,7 @@
       </c>
       <c r="H85" s="25" t="b">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I85" s="25">
         <v>50</v>
@@ -6169,13 +6169,13 @@
       <c r="J85" s="25">
         <v>1</v>
       </c>
-      <c r="K85" s="24" t="e">
+      <c r="K85" s="24">
         <f>_xll.qlRateHelperEarliestDate($E85,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L85" s="23" t="e">
+        <v>41660</v>
+      </c>
+      <c r="L85" s="23">
         <f>_xll.qlRateHelperLatestDate($E85,Trigger)</f>
-        <v>#NUM!</v>
+        <v>63576</v>
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.2">
@@ -7793,7 +7793,7 @@
   <cols>
     <col min="1" max="1" width="36.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" style="2" bestFit="1" customWidth="1"/>
@@ -7836,16 +7836,14 @@
       <c r="B2" s="18">
         <v>8</v>
       </c>
-      <c r="C2" s="92" t="s">
-        <v>117</v>
-      </c>
+      <c r="C2" s="92"/>
       <c r="D2" s="11" t="str">
         <f t="array" ref="D2:D126">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,RateHelpersIncluded),_xll.ohFilter(RateHelpersPriority,RateHelpersIncluded),nIMMFutures,nSerialFutures,FrontFuturesRollingDays,DepoInclusionCriteria,_xll.ohFilter(MinDistance,RateHelpersIncluded),Trigger)</f>
         <v>EUR_YCONRH_OND</v>
       </c>
       <c r="E2" s="10">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>1E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
       <c r="F2" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -7860,7 +7858,7 @@
         <v>41659</v>
       </c>
       <c r="I2" s="3">
-        <v>0.99999166673611051</v>
+        <v>0.99997083418400312</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>117</v>
@@ -7877,15 +7875,13 @@
       <c r="B3" s="17">
         <v>1</v>
       </c>
-      <c r="C3" s="92" t="s">
-        <v>118</v>
-      </c>
+      <c r="C3" s="92"/>
       <c r="D3" s="11" t="str">
         <v>EUR_YCONRH_TND</v>
       </c>
       <c r="E3" s="10">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>1E-3</v>
+        <v>3.4999999999999996E-3</v>
       </c>
       <c r="F3" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -7900,7 +7896,7 @@
         <v>41660</v>
       </c>
       <c r="I3" s="3">
-        <v>0.99998888898921767</v>
+        <v>0.99996111233961249</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>118</v>
@@ -7917,15 +7913,13 @@
       <c r="B4" s="17">
         <v>2</v>
       </c>
-      <c r="C4" s="92" t="s">
-        <v>119</v>
-      </c>
+      <c r="C4" s="92"/>
       <c r="D4" s="11" t="str">
         <v>EUR_YCONRH_SND</v>
       </c>
       <c r="E4" s="10">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>1E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="F4" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -7940,7 +7934,7 @@
         <v>41661</v>
       </c>
       <c r="I4" s="3">
-        <v>0.99998611125003567</v>
+        <v>0.99995416821346561</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>119</v>
@@ -7957,15 +7951,13 @@
       <c r="B5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="92" t="s">
-        <v>120</v>
-      </c>
+      <c r="C5" s="92"/>
       <c r="D5" s="11" t="str">
         <v>EUR_YCONRH_EONSW</v>
       </c>
       <c r="E5" s="10">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>1.08E-3</v>
+        <v>1.99E-3</v>
       </c>
       <c r="F5" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -7980,7 +7972,7 @@
         <v>41667</v>
       </c>
       <c r="I5" s="3">
-        <v>0.99996788966353423</v>
+        <v>0.9999224208970483</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>120</v>
@@ -7998,15 +7990,13 @@
         <f>_xll.ohRangeRetrieveError(Selected!D2)</f>
         <v/>
       </c>
-      <c r="C6" s="92" t="s">
-        <v>121</v>
-      </c>
+      <c r="C6" s="92"/>
       <c r="D6" s="11" t="str">
         <v>EUR_YCONRH_EON2W</v>
       </c>
       <c r="E6" s="10">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>1.06E-3</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="F6" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -8021,7 +8011,7 @@
         <v>41674</v>
       </c>
       <c r="I6" s="3">
-        <v>0.99994766892419962</v>
+        <v>0.99987945551741197</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>121</v>
@@ -8040,15 +8030,13 @@
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
         <v/>
       </c>
-      <c r="C7" s="92" t="s">
-        <v>122</v>
-      </c>
+      <c r="C7" s="92"/>
       <c r="D7" s="11" t="str">
         <v>EUR_YCONRH_EON3W</v>
       </c>
       <c r="E7" s="10">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>1.06E-3</v>
+        <v>2.0399999999999997E-3</v>
       </c>
       <c r="F7" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -8063,7 +8051,7 @@
         <v>41681</v>
       </c>
       <c r="I7" s="3">
-        <v>0.99992706016599742</v>
+        <v>0.99984213112600839</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>122</v>
@@ -8074,15 +8062,13 @@
       <c r="N7" s="95"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C8" s="92" t="s">
-        <v>123</v>
-      </c>
+      <c r="C8" s="92"/>
       <c r="D8" s="11" t="str">
         <v>EUR_YCONRH_EON1M</v>
       </c>
       <c r="E8" s="10">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>1.0600000000000002E-3</v>
+        <v>1.9599999999999999E-3</v>
       </c>
       <c r="F8" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -8097,7 +8083,7 @@
         <v>41691</v>
       </c>
       <c r="I8" s="3">
-        <v>0.99989762055640796</v>
+        <v>0.99979236960523143</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>123</v>
@@ -8108,15 +8094,13 @@
       <c r="N8" s="95"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C9" s="92" t="s">
-        <v>124</v>
-      </c>
+      <c r="C9" s="92"/>
       <c r="D9" s="11" t="str">
         <v>EUR_YCONRH_EON2M</v>
       </c>
       <c r="E9" s="10">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>1.1100000000000001E-3</v>
+        <v>1.9300000000000001E-3</v>
       </c>
       <c r="F9" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -8131,7 +8115,7 @@
         <v>41719</v>
       </c>
       <c r="I9" s="3">
-        <v>0.99980700743120288</v>
+        <v>0.99964491909811892</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>124</v>
@@ -8142,15 +8126,13 @@
       <c r="N9" s="95"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C10" s="92" t="s">
-        <v>125</v>
-      </c>
+      <c r="C10" s="92"/>
       <c r="D10" s="11" t="str">
         <v>EUR_YCONRH_EON3M</v>
       </c>
       <c r="E10" s="10">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>1.15E-3</v>
+        <v>1.9E-3</v>
       </c>
       <c r="F10" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -8165,7 +8147,7 @@
         <v>41751</v>
       </c>
       <c r="I10" s="3">
-        <v>0.99969828225244617</v>
+        <v>0.99948108378576095</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>125</v>
@@ -8176,15 +8158,13 @@
       <c r="N10" s="95"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C11" s="92" t="s">
-        <v>126</v>
-      </c>
+      <c r="C11" s="92"/>
       <c r="D11" s="11" t="str">
         <v>EUR_YCONRH_EON4M</v>
       </c>
       <c r="E11" s="10">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>1.17E-3</v>
+        <v>1.8400000000000001E-3</v>
       </c>
       <c r="F11" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -8199,7 +8179,7 @@
         <v>41780</v>
       </c>
       <c r="I11" s="3">
-        <v>0.9995990453617295</v>
+        <v>0.99934817878995463</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>126</v>
@@ -8210,15 +8190,13 @@
       <c r="N11" s="95"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C12" s="92" t="s">
-        <v>127</v>
-      </c>
+      <c r="C12" s="92"/>
       <c r="D12" s="11" t="str">
         <v>EUR_YCONRH_EON5M</v>
       </c>
       <c r="E12" s="10">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>1.1899999999999999E-3</v>
+        <v>1.7899999999999999E-3</v>
       </c>
       <c r="F12" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -8233,7 +8211,7 @@
         <v>41813</v>
       </c>
       <c r="I12" s="3">
-        <v>0.99948340025953641</v>
+        <v>0.99920097020153176</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>127</v>
@@ -8244,15 +8222,13 @@
       <c r="N12" s="95"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C13" s="92" t="s">
-        <v>128</v>
-      </c>
+      <c r="C13" s="92"/>
       <c r="D13" s="11" t="str">
         <v>EUR_YCONRH_EON6M</v>
       </c>
       <c r="E13" s="10">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>1.24E-3</v>
+        <v>1.7499999999999998E-3</v>
       </c>
       <c r="F13" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -8267,7 +8243,7 @@
         <v>41841</v>
       </c>
       <c r="I13" s="3">
-        <v>0.99936583990835925</v>
+        <v>0.99908205888918711</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>128</v>
@@ -8278,15 +8254,13 @@
       <c r="N13" s="95"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C14" s="92" t="s">
-        <v>129</v>
-      </c>
+      <c r="C14" s="92"/>
       <c r="D14" s="11" t="str">
         <v>EUR_YCONRH_EON7M</v>
       </c>
       <c r="E14" s="10">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>1.2800000000000001E-3</v>
+        <v>1.72E-3</v>
       </c>
       <c r="F14" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -8301,7 +8275,7 @@
         <v>41872</v>
       </c>
       <c r="I14" s="3">
-        <v>0.99923568733334334</v>
+        <v>0.99894928770553215</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>129</v>
@@ -8312,15 +8286,13 @@
       <c r="N14" s="95"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C15" s="92" t="s">
-        <v>130</v>
-      </c>
+      <c r="C15" s="92"/>
       <c r="D15" s="11" t="str">
         <v>EUR_YCONRH_EON8M</v>
       </c>
       <c r="E15" s="10">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>1.33E-3</v>
+        <v>1.6900000000000001E-3</v>
       </c>
       <c r="F15" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -8335,7 +8307,7 @@
         <v>41904</v>
       </c>
       <c r="I15" s="3">
-        <v>0.99908826642194193</v>
+        <v>0.998817022929681</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>130</v>
@@ -8346,15 +8318,13 @@
       <c r="N15" s="95"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C16" s="92" t="s">
-        <v>131</v>
-      </c>
+      <c r="C16" s="92"/>
       <c r="D16" s="11" t="str">
         <v>EUR_YCONRH_EON9M</v>
       </c>
       <c r="E16" s="10">
         <f>_xll.qlRateHelperRate($D16)</f>
-        <v>1.4100000000000002E-3</v>
+        <v>1.66E-3</v>
       </c>
       <c r="F16" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D16)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D16)),_xll.qlSwapRateHelperSpread($D16))</f>
@@ -8369,7 +8339,7 @@
         <v>41933</v>
       </c>
       <c r="I16" s="3">
-        <v>0.99892079293137592</v>
+        <v>0.99870391056686048</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>131</v>
@@ -8380,15 +8350,13 @@
       <c r="N16" s="95"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C17" s="92" t="s">
-        <v>132</v>
-      </c>
+      <c r="C17" s="92"/>
       <c r="D17" s="11" t="str">
         <v>EUR_YCONRH_EON10M</v>
       </c>
       <c r="E17" s="10">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>1.47E-3</v>
+        <v>1.64E-3</v>
       </c>
       <c r="F17" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -8403,7 +8371,7 @@
         <v>41964</v>
       </c>
       <c r="I17" s="3">
-        <v>0.99874910842928744</v>
+        <v>0.99857819249613777</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>132</v>
@@ -8414,15 +8382,13 @@
       <c r="N17" s="95"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C18" s="92" t="s">
-        <v>133</v>
-      </c>
+      <c r="C18" s="92"/>
       <c r="D18" s="11" t="str">
         <v>EUR_YCONRH_EON11M</v>
       </c>
       <c r="E18" s="10">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>1.5499999999999999E-3</v>
+        <v>1.6200000000000001E-3</v>
       </c>
       <c r="F18" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -8437,7 +8403,7 @@
         <v>41995</v>
       </c>
       <c r="I18" s="3">
-        <v>0.99854862129031519</v>
+        <v>0.99845594001004734</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>133</v>
@@ -8448,15 +8414,13 @@
       <c r="N18" s="95"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C19" s="92" t="s">
-        <v>134</v>
-      </c>
+      <c r="C19" s="92"/>
       <c r="D19" s="11" t="str">
         <v>EUR_YCONRH_EON1Y</v>
       </c>
       <c r="E19" s="10">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>1.6200000000000001E-3</v>
+        <v>1.6100000000000001E-3</v>
       </c>
       <c r="F19" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -8471,7 +8435,7 @@
         <v>42025</v>
       </c>
       <c r="I19" s="3">
-        <v>0.99834910059149629</v>
+        <v>0.99833147486404616</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>134</v>
@@ -8482,15 +8446,13 @@
       <c r="N19" s="95"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C20" s="92" t="s">
-        <v>135</v>
-      </c>
+      <c r="C20" s="92"/>
       <c r="D20" s="11" t="str">
         <v>EUR_YCONRH_EON15M</v>
       </c>
       <c r="E20" s="10">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>1.8500000000000001E-3</v>
+        <v>1.6100000000000001E-3</v>
       </c>
       <c r="F20" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -8505,7 +8467,7 @@
         <v>42115</v>
       </c>
       <c r="I20" s="3">
-        <v>0.99765487574758882</v>
+        <v>0.99792980811603904</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>135</v>
@@ -8516,15 +8478,13 @@
       <c r="N20" s="95"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C21" s="92" t="s">
-        <v>136</v>
-      </c>
+      <c r="C21" s="92"/>
       <c r="D21" s="11" t="str">
         <v>EUR_YCONRH_EON18M</v>
       </c>
       <c r="E21" s="10">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>2.0900000000000003E-3</v>
+        <v>1.66E-3</v>
       </c>
       <c r="F21" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -8539,7 +8499,7 @@
         <v>42206</v>
       </c>
       <c r="I21" s="3">
-        <v>0.99682588933071647</v>
+        <v>0.99744838350092679</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>136</v>
@@ -8550,15 +8510,13 @@
       <c r="N21" s="95"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C22" s="92" t="s">
-        <v>137</v>
-      </c>
+      <c r="C22" s="92"/>
       <c r="D22" s="11" t="str">
         <v>EUR_YCONRH_EON21M</v>
       </c>
       <c r="E22" s="10">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>2.3499999999999997E-3</v>
+        <v>1.7699999999999999E-3</v>
       </c>
       <c r="F22" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -8573,7 +8531,7 @@
         <v>42298</v>
       </c>
       <c r="I22" s="3">
-        <v>0.99583552171149303</v>
+        <v>0.99683152619764159</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>137</v>
@@ -8584,15 +8542,13 @@
       <c r="N22" s="95"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C23" s="92" t="s">
-        <v>138</v>
-      </c>
+      <c r="C23" s="92"/>
       <c r="D23" s="11" t="str">
         <v>EUR_YCONRH_EON2Y</v>
       </c>
       <c r="E23" s="10">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>2.63E-3</v>
+        <v>1.9500000000000001E-3</v>
       </c>
       <c r="F23" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -8607,7 +8563,7 @@
         <v>42390</v>
       </c>
       <c r="I23" s="3">
-        <v>0.994674436366217</v>
+        <v>0.99601811700071252</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>138</v>
@@ -8618,15 +8574,13 @@
       <c r="N23" s="95"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C24" s="92" t="s">
-        <v>139</v>
-      </c>
+      <c r="C24" s="92"/>
       <c r="D24" s="11" t="str">
         <v>EUR_YCONRH_EON3Y</v>
       </c>
       <c r="E24" s="10">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>4.15E-3</v>
+        <v>3.32E-3</v>
       </c>
       <c r="F24" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -8641,7 +8595,7 @@
         <v>42758</v>
       </c>
       <c r="I24" s="3">
-        <v>0.98741413546065604</v>
+        <v>0.9898884485996603</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>139</v>
@@ -8652,15 +8606,13 @@
       <c r="N24" s="95"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C25" s="92" t="s">
-        <v>140</v>
-      </c>
+      <c r="C25" s="92"/>
       <c r="D25" s="11" t="str">
         <v>EUR_YCONRH_EON4Y</v>
       </c>
       <c r="E25" s="10">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>6.2399999999999999E-3</v>
+        <v>5.3900000000000007E-3</v>
       </c>
       <c r="F25" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -8675,7 +8627,7 @@
         <v>43122</v>
       </c>
       <c r="I25" s="3">
-        <v>0.97493014849642678</v>
+        <v>0.97827670409658241</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>140</v>
@@ -8686,15 +8638,13 @@
       <c r="N25" s="95"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C26" s="92" t="s">
-        <v>141</v>
-      </c>
+      <c r="C26" s="92"/>
       <c r="D26" s="11" t="str">
         <v>EUR_YCONRH_EON5Y</v>
       </c>
       <c r="E26" s="10">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>8.4899999999999993E-3</v>
+        <v>7.5900000000000004E-3</v>
       </c>
       <c r="F26" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -8709,7 +8659,7 @@
         <v>43486</v>
       </c>
       <c r="I26" s="3">
-        <v>0.95767355592477621</v>
+        <v>0.96204288742283095</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>141</v>
@@ -8720,15 +8670,13 @@
       <c r="N26" s="95"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C27" s="92" t="s">
-        <v>142</v>
-      </c>
+      <c r="C27" s="92"/>
       <c r="D27" s="11" t="str">
         <v>EUR_YCONRH_EON6Y</v>
       </c>
       <c r="E27" s="10">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>1.0459999999999999E-2</v>
+        <v>9.75E-3</v>
       </c>
       <c r="F27" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -8743,7 +8691,7 @@
         <v>43851</v>
       </c>
       <c r="I27" s="3">
-        <v>0.93790802855675892</v>
+        <v>0.94194045624904854</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>142</v>
@@ -8754,15 +8702,13 @@
       <c r="N27" s="95"/>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C28" s="92" t="s">
-        <v>143</v>
-      </c>
+      <c r="C28" s="92"/>
       <c r="D28" s="11" t="str">
         <v>EUR_YCONRH_EON7Y</v>
       </c>
       <c r="E28" s="10">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>1.2229999999999998E-2</v>
+        <v>1.1779999999999999E-2</v>
       </c>
       <c r="F28" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -8777,7 +8723,7 @@
         <v>44217</v>
       </c>
       <c r="I28" s="3">
-        <v>0.91601339203174947</v>
+        <v>0.91885573553515287</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>143</v>
@@ -8788,15 +8734,13 @@
       <c r="N28" s="95"/>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C29" s="92" t="s">
-        <v>144</v>
-      </c>
+      <c r="C29" s="92"/>
       <c r="D29" s="11" t="str">
         <v>EUR_YCONRH_EON8Y</v>
       </c>
       <c r="E29" s="10">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>1.3809999999999999E-2</v>
+        <v>1.3640000000000001E-2</v>
       </c>
       <c r="F29" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -8811,7 +8755,7 @@
         <v>44582</v>
       </c>
       <c r="I29" s="3">
-        <v>0.89266562383078296</v>
+        <v>0.89369038192082451</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>144</v>
@@ -8822,15 +8766,13 @@
       <c r="N29" s="95"/>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C30" s="92" t="s">
-        <v>145</v>
-      </c>
+      <c r="C30" s="92"/>
       <c r="D30" s="11" t="str">
         <v>EUR_YCONRH_EON9Y</v>
       </c>
       <c r="E30" s="10">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>1.529E-2</v>
+        <v>1.5309999999999999E-2</v>
       </c>
       <c r="F30" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -8845,7 +8787,7 @@
         <v>44949</v>
       </c>
       <c r="I30" s="3">
-        <v>0.86763976099111229</v>
+        <v>0.86714509378014493</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>145</v>
@@ -8856,15 +8798,13 @@
       <c r="N30" s="95"/>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C31" s="92" t="s">
-        <v>146</v>
-      </c>
+      <c r="C31" s="92"/>
       <c r="D31" s="11" t="str">
         <v>EUR_YCONRH_EON10Y</v>
       </c>
       <c r="E31" s="10">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>1.6640000000000002E-2</v>
+        <v>1.6799999999999999E-2</v>
       </c>
       <c r="F31" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
@@ -8879,7 +8819,7 @@
         <v>45313</v>
       </c>
       <c r="I31" s="3">
-        <v>0.84179121550459013</v>
+        <v>0.83995120059952877</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>146</v>
@@ -8890,15 +8830,13 @@
       <c r="N31" s="95"/>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C32" s="92" t="s">
-        <v>147</v>
-      </c>
+      <c r="C32" s="92"/>
       <c r="D32" s="11" t="str">
         <v>EUR_YCONRH_EON11Y</v>
       </c>
       <c r="E32" s="10">
         <f>_xll.qlRateHelperRate($D32)</f>
-        <v>1.7819999999999999E-2</v>
+        <v>1.8100000000000002E-2</v>
       </c>
       <c r="F32" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D32)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D32)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D32)),_xll.qlSwapRateHelperSpread($D32))</f>
@@ -8913,7 +8851,7 @@
         <v>45678</v>
       </c>
       <c r="I32" s="3">
-        <v>0.81583281154782383</v>
+        <v>0.81265611287832606</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>147</v>
@@ -8924,15 +8862,13 @@
       <c r="N32" s="95"/>
     </row>
     <row r="33" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C33" s="92" t="s">
-        <v>148</v>
-      </c>
+      <c r="C33" s="92"/>
       <c r="D33" s="11" t="str">
         <v>EUR_YCONRH_EON12Y</v>
       </c>
       <c r="E33" s="10">
         <f>_xll.qlRateHelperRate($D33)</f>
-        <v>1.8839999999999999E-2</v>
+        <v>1.925E-2</v>
       </c>
       <c r="F33" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D33)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D33)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D33)),_xll.qlSwapRateHelperSpread($D33))</f>
@@ -8947,7 +8883,7 @@
         <v>46043</v>
       </c>
       <c r="I33" s="3">
-        <v>0.79019779638299315</v>
+        <v>0.78542607466459036</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>148</v>
@@ -8958,15 +8894,13 @@
       <c r="N33" s="95"/>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C34" s="92" t="s">
-        <v>149</v>
-      </c>
+      <c r="C34" s="92"/>
       <c r="D34" s="11" t="str">
         <v>EUR_YCONRH_EON15Y</v>
       </c>
       <c r="E34" s="10">
         <f>_xll.qlRateHelperRate($D34)</f>
-        <v>2.1049999999999999E-2</v>
+        <v>2.1789999999999997E-2</v>
       </c>
       <c r="F34" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D34)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D34)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D34)),_xll.qlSwapRateHelperSpread($D34))</f>
@@ -8981,7 +8915,7 @@
         <v>47140</v>
       </c>
       <c r="I34" s="3">
-        <v>0.71802133716517558</v>
+        <v>0.70841510945844055</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>149</v>
@@ -8992,15 +8926,13 @@
       <c r="N34" s="95"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C35" s="92" t="s">
-        <v>150</v>
-      </c>
+      <c r="C35" s="92"/>
       <c r="D35" s="11" t="str">
         <v>EUR_YCONRH_EON20Y</v>
       </c>
       <c r="E35" s="10">
         <f>_xll.qlRateHelperRate($D35)</f>
-        <v>2.2450000000000001E-2</v>
+        <v>2.367E-2</v>
       </c>
       <c r="F35" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D35)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D35)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D35)),_xll.qlSwapRateHelperSpread($D35))</f>
@@ -9015,7 +8947,7 @@
         <v>48967</v>
       </c>
       <c r="I35" s="3">
-        <v>0.62400815900005169</v>
+        <v>0.60571874773400769</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>150</v>
@@ -9026,15 +8958,13 @@
       <c r="N35" s="95"/>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C36" s="92" t="s">
-        <v>151</v>
-      </c>
+      <c r="C36" s="92"/>
       <c r="D36" s="11" t="str">
         <v>EUR_YCONRH_EON25Y</v>
       </c>
       <c r="E36" s="10">
         <f>_xll.qlRateHelperRate($D36)</f>
-        <v>2.2809999999999997E-2</v>
+        <v>2.4310000000000002E-2</v>
       </c>
       <c r="F36" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D36)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D36)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D36)),_xll.qlSwapRateHelperSpread($D36))</f>
@@ -9049,7 +8979,7 @@
         <v>50791</v>
       </c>
       <c r="I36" s="3">
-        <v>0.55100795740196762</v>
+        <v>0.5264220386416566</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>151</v>
@@ -9060,15 +8990,13 @@
       <c r="N36" s="95"/>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C37" s="92" t="s">
-        <v>152</v>
-      </c>
+      <c r="C37" s="92"/>
       <c r="D37" s="11" t="str">
         <v>EUR_YCONRH_EON30Y</v>
       </c>
       <c r="E37" s="10">
         <f>_xll.qlRateHelperRate($D37)</f>
-        <v>2.2889999999999997E-2</v>
+        <v>2.4479999999999998E-2</v>
       </c>
       <c r="F37" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D37)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D37)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D37)),_xll.qlSwapRateHelperSpread($D37))</f>
@@ -9083,7 +9011,7 @@
         <v>52617</v>
       </c>
       <c r="I37" s="3">
-        <v>0.48979097977701558</v>
+        <v>0.46258379896174923</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>152</v>
@@ -9094,27 +9022,27 @@
       <c r="N37" s="95"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D38" s="11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E38" s="10" t="e">
+      <c r="D38" s="11" t="str">
+        <v>EUR_YCONRH_EON40Y</v>
+      </c>
+      <c r="E38" s="10">
         <f>_xll.qlRateHelperRate($D38)</f>
-        <v>#VALUE!</v>
+        <v>2.495E-2</v>
       </c>
       <c r="F38" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D38)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D38)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D38)),_xll.qlSwapRateHelperSpread($D38))</f>
         <v>--</v>
       </c>
-      <c r="G38" s="9" t="e">
+      <c r="G38" s="9">
         <f>_xll.qlRateHelperEarliestDate($D38)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H38" s="8" t="e">
+        <v>41660</v>
+      </c>
+      <c r="H38" s="8">
         <f>_xll.qlRateHelperLatestDate($D38)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I38" s="3" t="e">
-        <v>#N/A</v>
+        <v>56270</v>
+      </c>
+      <c r="I38" s="3">
+        <v>0.35128901362079018</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>187</v>
@@ -9124,27 +9052,27 @@
       </c>
     </row>
     <row r="39" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D39" s="11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E39" s="10" t="e">
+      <c r="D39" s="11" t="str">
+        <v>EUR_YCONRH_EON50Y</v>
+      </c>
+      <c r="E39" s="10">
         <f>_xll.qlRateHelperRate($D39)</f>
-        <v>#VALUE!</v>
+        <v>2.528E-2</v>
       </c>
       <c r="F39" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D39)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D39)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D39)),_xll.qlSwapRateHelperSpread($D39))</f>
         <v>--</v>
       </c>
-      <c r="G39" s="9" t="e">
+      <c r="G39" s="9">
         <f>_xll.qlRateHelperEarliestDate($D39)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H39" s="8" t="e">
+        <v>41660</v>
+      </c>
+      <c r="H39" s="8">
         <f>_xll.qlRateHelperLatestDate($D39)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I39" s="3" t="e">
-        <v>#N/A</v>
+        <v>59922</v>
+      </c>
+      <c r="I39" s="3">
+        <v>0.26526490950122278</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>188</v>
@@ -9154,27 +9082,27 @@
       </c>
     </row>
     <row r="40" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D40" s="11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E40" s="10" t="e">
+      <c r="D40" s="11" t="str">
+        <v>EUR_YCONRH_EON60Y</v>
+      </c>
+      <c r="E40" s="10">
         <f>_xll.qlRateHelperRate($D40)</f>
-        <v>#VALUE!</v>
+        <v>2.5510000000000001E-2</v>
       </c>
       <c r="F40" s="10" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D40)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D40)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D40)),_xll.qlSwapRateHelperSpread($D40))</f>
         <v>--</v>
       </c>
-      <c r="G40" s="9" t="e">
+      <c r="G40" s="9">
         <f>_xll.qlRateHelperEarliestDate($D40)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H40" s="8" t="e">
+        <v>41660</v>
+      </c>
+      <c r="H40" s="8">
         <f>_xll.qlRateHelperLatestDate($D40)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I40" s="3" t="e">
-        <v>#N/A</v>
+        <v>63576</v>
+      </c>
+      <c r="I40" s="3">
+        <v>0.19963997166531142</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>189</v>
@@ -11528,7 +11456,7 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet20"/>
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -11623,8 +11551,8 @@
         <v>EUR_YCONRH_Swaps.xml</v>
       </c>
       <c r="L3" s="176">
-        <f ca="1">IF(Serialize,_xll.ohObjectSave(_xll.ohPack(L4:L38),SerializationPath&amp;K3,FileOverwrite,Serialize),"---")</f>
-        <v>34</v>
+        <f ca="1">IF(Serialize,_xll.ohObjectSave(_xll.ohPack(L4:L41),SerializationPath&amp;K3,FileOverwrite,Serialize),"---")</f>
+        <v>37</v>
       </c>
       <c r="M3" s="101" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L3)</f>
@@ -11692,18 +11620,18 @@
         <v>178</v>
       </c>
       <c r="H6" s="170" t="str">
-        <f t="shared" ref="H6:H38" si="0">MoneyMarketDayCounter</f>
+        <f t="shared" ref="H6:H41" si="0">MoneyMarketDayCounter</f>
         <v>Actual/360</v>
       </c>
       <c r="I6" s="169">
         <v>0</v>
       </c>
       <c r="J6" s="168" t="str">
-        <f t="shared" ref="J6:J38" si="1">Currency&amp;$D6&amp;$E6&amp;QuoteSuffix</f>
+        <f t="shared" ref="J6:J41" si="1">Currency&amp;$D6&amp;$E6&amp;QuoteSuffix</f>
         <v>EUREONSW_Quote</v>
       </c>
       <c r="K6" s="168" t="str">
-        <f t="shared" ref="K6:K38" si="2">$K$2&amp;"_"&amp;$D6&amp;$E6</f>
+        <f t="shared" ref="K6:K41" si="2">$K$2&amp;"_"&amp;$D6&amp;$E6</f>
         <v>EUR_YCONRH_EONSW</v>
       </c>
       <c r="L6" s="167" t="str">
@@ -11715,14 +11643,11 @@
         <v/>
       </c>
       <c r="N6" s="165"/>
-      <c r="P6" s="166">
-        <f>_xll.qlRateHelperEarliestDate($L6)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q6" s="166">
-        <f>_xll.qlRateHelperLatestDate($L6)</f>
-        <v>41667</v>
-      </c>
+      <c r="P6" s="166" t="str">
+        <f>_xll.ohObjectCallerAddress(J6)</f>
+        <v>[EUR_Market.xlsm]OIS!R5C6</v>
+      </c>
+      <c r="Q6" s="166"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="100"/>
@@ -11734,7 +11659,7 @@
         <v>109</v>
       </c>
       <c r="E7" s="171" t="str">
-        <f t="shared" ref="E7:E38" si="3">C7</f>
+        <f t="shared" ref="E7:E41" si="3">C7</f>
         <v>2W</v>
       </c>
       <c r="F7" s="170" t="s">
@@ -11767,14 +11692,8 @@
         <v/>
       </c>
       <c r="N7" s="165"/>
-      <c r="P7" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L7)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q7" s="166">
-        <f>_xll.qlRateHelperLatestDate($L7)</f>
-        <v>41674</v>
-      </c>
+      <c r="P7" s="166"/>
+      <c r="Q7" s="166"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="100"/>
@@ -11819,14 +11738,8 @@
         <v/>
       </c>
       <c r="N8" s="165"/>
-      <c r="P8" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L8)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q8" s="166">
-        <f>_xll.qlRateHelperLatestDate($L8)</f>
-        <v>41681</v>
-      </c>
+      <c r="P8" s="166"/>
+      <c r="Q8" s="166"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="100"/>
@@ -11871,14 +11784,8 @@
         <v/>
       </c>
       <c r="N9" s="165"/>
-      <c r="P9" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L9)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q9" s="166">
-        <f>_xll.qlRateHelperLatestDate($L9)</f>
-        <v>41691</v>
-      </c>
+      <c r="P9" s="166"/>
+      <c r="Q9" s="166"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="100"/>
@@ -11923,14 +11830,8 @@
         <v/>
       </c>
       <c r="N10" s="165"/>
-      <c r="P10" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L10)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q10" s="166">
-        <f>_xll.qlRateHelperLatestDate($L10)</f>
-        <v>41719</v>
-      </c>
+      <c r="P10" s="166"/>
+      <c r="Q10" s="166"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="100"/>
@@ -11975,14 +11876,8 @@
         <v/>
       </c>
       <c r="N11" s="165"/>
-      <c r="P11" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L11)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q11" s="166">
-        <f>_xll.qlRateHelperLatestDate($L11)</f>
-        <v>41751</v>
-      </c>
+      <c r="P11" s="166"/>
+      <c r="Q11" s="166"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="100"/>
@@ -12027,14 +11922,8 @@
         <v/>
       </c>
       <c r="N12" s="165"/>
-      <c r="P12" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L12)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q12" s="166">
-        <f>_xll.qlRateHelperLatestDate($L12)</f>
-        <v>41780</v>
-      </c>
+      <c r="P12" s="166"/>
+      <c r="Q12" s="166"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="100"/>
@@ -12079,14 +11968,8 @@
         <v/>
       </c>
       <c r="N13" s="165"/>
-      <c r="P13" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L13)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q13" s="166">
-        <f>_xll.qlRateHelperLatestDate($L13)</f>
-        <v>41813</v>
-      </c>
+      <c r="P13" s="166"/>
+      <c r="Q13" s="166"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="100"/>
@@ -12131,14 +12014,8 @@
         <v/>
       </c>
       <c r="N14" s="165"/>
-      <c r="P14" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L14)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q14" s="166">
-        <f>_xll.qlRateHelperLatestDate($L14)</f>
-        <v>41841</v>
-      </c>
+      <c r="P14" s="166"/>
+      <c r="Q14" s="166"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="100"/>
@@ -12183,14 +12060,8 @@
         <v/>
       </c>
       <c r="N15" s="165"/>
-      <c r="P15" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L15)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q15" s="166">
-        <f>_xll.qlRateHelperLatestDate($L15)</f>
-        <v>41872</v>
-      </c>
+      <c r="P15" s="166"/>
+      <c r="Q15" s="166"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="100"/>
@@ -12235,14 +12106,8 @@
         <v/>
       </c>
       <c r="N16" s="165"/>
-      <c r="P16" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L16)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q16" s="166">
-        <f>_xll.qlRateHelperLatestDate($L16)</f>
-        <v>41904</v>
-      </c>
+      <c r="P16" s="166"/>
+      <c r="Q16" s="166"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="100"/>
@@ -12287,14 +12152,8 @@
         <v/>
       </c>
       <c r="N17" s="165"/>
-      <c r="P17" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L17)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q17" s="166">
-        <f>_xll.qlRateHelperLatestDate($L17)</f>
-        <v>41933</v>
-      </c>
+      <c r="P17" s="166"/>
+      <c r="Q17" s="166"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="100"/>
@@ -12339,14 +12198,8 @@
         <v/>
       </c>
       <c r="N18" s="165"/>
-      <c r="P18" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L18)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q18" s="166">
-        <f>_xll.qlRateHelperLatestDate($L18)</f>
-        <v>41964</v>
-      </c>
+      <c r="P18" s="166"/>
+      <c r="Q18" s="166"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="100"/>
@@ -12391,14 +12244,8 @@
         <v/>
       </c>
       <c r="N19" s="165"/>
-      <c r="P19" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L19)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q19" s="166">
-        <f>_xll.qlRateHelperLatestDate($L19)</f>
-        <v>41995</v>
-      </c>
+      <c r="P19" s="166"/>
+      <c r="Q19" s="166"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="100"/>
@@ -12443,14 +12290,8 @@
         <v/>
       </c>
       <c r="N20" s="165"/>
-      <c r="P20" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L20)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q20" s="166">
-        <f>_xll.qlRateHelperLatestDate($L20)</f>
-        <v>42025</v>
-      </c>
+      <c r="P20" s="166"/>
+      <c r="Q20" s="166"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="100"/>
@@ -12495,14 +12336,8 @@
         <v/>
       </c>
       <c r="N21" s="165"/>
-      <c r="P21" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L21)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q21" s="166">
-        <f>_xll.qlRateHelperLatestDate($L21)</f>
-        <v>42115</v>
-      </c>
+      <c r="P21" s="166"/>
+      <c r="Q21" s="166"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="100"/>
@@ -12547,14 +12382,8 @@
         <v/>
       </c>
       <c r="N22" s="165"/>
-      <c r="P22" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L22)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q22" s="166">
-        <f>_xll.qlRateHelperLatestDate($L22)</f>
-        <v>42206</v>
-      </c>
+      <c r="P22" s="166"/>
+      <c r="Q22" s="166"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="100"/>
@@ -12599,14 +12428,8 @@
         <v/>
       </c>
       <c r="N23" s="165"/>
-      <c r="P23" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L23)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q23" s="166">
-        <f>_xll.qlRateHelperLatestDate($L23)</f>
-        <v>42298</v>
-      </c>
+      <c r="P23" s="166"/>
+      <c r="Q23" s="166"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="100"/>
@@ -12651,14 +12474,8 @@
         <v/>
       </c>
       <c r="N24" s="165"/>
-      <c r="P24" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L24)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q24" s="166">
-        <f>_xll.qlRateHelperLatestDate($L24)</f>
-        <v>42390</v>
-      </c>
+      <c r="P24" s="166"/>
+      <c r="Q24" s="166"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="100"/>
@@ -12703,14 +12520,8 @@
         <v/>
       </c>
       <c r="N25" s="165"/>
-      <c r="P25" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L25)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q25" s="166">
-        <f>_xll.qlRateHelperLatestDate($L25)</f>
-        <v>42758</v>
-      </c>
+      <c r="P25" s="166"/>
+      <c r="Q25" s="166"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="100"/>
@@ -12755,14 +12566,8 @@
         <v/>
       </c>
       <c r="N26" s="165"/>
-      <c r="P26" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L26)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q26" s="166">
-        <f>_xll.qlRateHelperLatestDate($L26)</f>
-        <v>43122</v>
-      </c>
+      <c r="P26" s="166"/>
+      <c r="Q26" s="166"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="100"/>
@@ -12807,14 +12612,8 @@
         <v/>
       </c>
       <c r="N27" s="165"/>
-      <c r="P27" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L27)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q27" s="166">
-        <f>_xll.qlRateHelperLatestDate($L27)</f>
-        <v>43486</v>
-      </c>
+      <c r="P27" s="166"/>
+      <c r="Q27" s="166"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="100"/>
@@ -12859,14 +12658,8 @@
         <v/>
       </c>
       <c r="N28" s="165"/>
-      <c r="P28" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L28)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q28" s="166">
-        <f>_xll.qlRateHelperLatestDate($L28)</f>
-        <v>43851</v>
-      </c>
+      <c r="P28" s="166"/>
+      <c r="Q28" s="166"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="100"/>
@@ -12911,14 +12704,8 @@
         <v/>
       </c>
       <c r="N29" s="165"/>
-      <c r="P29" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L29)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q29" s="166">
-        <f>_xll.qlRateHelperLatestDate($L29)</f>
-        <v>44217</v>
-      </c>
+      <c r="P29" s="166"/>
+      <c r="Q29" s="166"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="100"/>
@@ -12963,14 +12750,8 @@
         <v/>
       </c>
       <c r="N30" s="165"/>
-      <c r="P30" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L30)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q30" s="166">
-        <f>_xll.qlRateHelperLatestDate($L30)</f>
-        <v>44582</v>
-      </c>
+      <c r="P30" s="166"/>
+      <c r="Q30" s="166"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="100"/>
@@ -13015,14 +12796,8 @@
         <v/>
       </c>
       <c r="N31" s="165"/>
-      <c r="P31" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L31)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q31" s="166">
-        <f>_xll.qlRateHelperLatestDate($L31)</f>
-        <v>44949</v>
-      </c>
+      <c r="P31" s="166"/>
+      <c r="Q31" s="166"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="100"/>
@@ -13067,14 +12842,8 @@
         <v/>
       </c>
       <c r="N32" s="165"/>
-      <c r="P32" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L32)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q32" s="166">
-        <f>_xll.qlRateHelperLatestDate($L32)</f>
-        <v>45313</v>
-      </c>
+      <c r="P32" s="166"/>
+      <c r="Q32" s="166"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="100"/>
@@ -13119,14 +12888,8 @@
         <v/>
       </c>
       <c r="N33" s="165"/>
-      <c r="P33" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L33)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q33" s="166">
-        <f>_xll.qlRateHelperLatestDate($L33)</f>
-        <v>45678</v>
-      </c>
+      <c r="P33" s="166"/>
+      <c r="Q33" s="166"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="100"/>
@@ -13171,14 +12934,8 @@
         <v/>
       </c>
       <c r="N34" s="165"/>
-      <c r="P34" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L34)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q34" s="166">
-        <f>_xll.qlRateHelperLatestDate($L34)</f>
-        <v>46043</v>
-      </c>
+      <c r="P34" s="166"/>
+      <c r="Q34" s="166"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="100"/>
@@ -13223,14 +12980,8 @@
         <v/>
       </c>
       <c r="N35" s="165"/>
-      <c r="P35" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L35)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q35" s="166">
-        <f>_xll.qlRateHelperLatestDate($L35)</f>
-        <v>47140</v>
-      </c>
+      <c r="P35" s="166"/>
+      <c r="Q35" s="166"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="100"/>
@@ -13275,14 +13026,8 @@
         <v/>
       </c>
       <c r="N36" s="165"/>
-      <c r="P36" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L36)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q36" s="166">
-        <f>_xll.qlRateHelperLatestDate($L36)</f>
-        <v>48967</v>
-      </c>
+      <c r="P36" s="166"/>
+      <c r="Q36" s="166"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="100"/>
@@ -13327,14 +13072,8 @@
         <v/>
       </c>
       <c r="N37" s="165"/>
-      <c r="P37" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L37)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q37" s="166">
-        <f>_xll.qlRateHelperLatestDate($L37)</f>
-        <v>50791</v>
-      </c>
+      <c r="P37" s="166"/>
+      <c r="Q37" s="166"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="100"/>
@@ -13346,7 +13085,7 @@
         <v>109</v>
       </c>
       <c r="E38" s="171" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E38:E40" si="4">C38</f>
         <v>30Y</v>
       </c>
       <c r="F38" s="170" t="s">
@@ -13379,39 +13118,171 @@
         <v/>
       </c>
       <c r="N38" s="165"/>
-      <c r="P38" s="166">
-        <f>_xll.qlRateHelperEarliestDate(L38)</f>
-        <v>41660</v>
-      </c>
-      <c r="Q38" s="166">
-        <f>_xll.qlRateHelperLatestDate($L38)</f>
-        <v>52617</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="99"/>
-      <c r="B39" s="98"/>
-      <c r="C39" s="98"/>
-      <c r="D39" s="98"/>
-      <c r="E39" s="98"/>
-      <c r="F39" s="98"/>
-      <c r="G39" s="98"/>
-      <c r="H39" s="98"/>
-      <c r="I39" s="98"/>
-      <c r="J39" s="98"/>
-      <c r="K39" s="98"/>
-      <c r="L39" s="164"/>
-      <c r="M39" s="164"/>
-      <c r="N39" s="163"/>
+      <c r="P38" s="166"/>
+      <c r="Q38" s="166"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="100"/>
+      <c r="B39" s="172"/>
+      <c r="C39" s="171" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="172" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" s="171" t="str">
+        <f t="shared" si="4"/>
+        <v>40Y</v>
+      </c>
+      <c r="F39" s="170" t="s">
+        <v>179</v>
+      </c>
+      <c r="G39" s="170" t="s">
+        <v>172</v>
+      </c>
+      <c r="H39" s="170" t="str">
+        <f t="shared" si="0"/>
+        <v>Actual/360</v>
+      </c>
+      <c r="I39" s="169">
+        <v>0</v>
+      </c>
+      <c r="J39" s="168" t="str">
+        <f t="shared" si="1"/>
+        <v>EUREON40Y_Quote</v>
+      </c>
+      <c r="K39" s="168" t="str">
+        <f t="shared" si="2"/>
+        <v>EUR_YCONRH_EON40Y</v>
+      </c>
+      <c r="L39" s="167" t="str">
+        <f>_xll.qlOISRateHelper(K39,2,C39,J39,$L$4,Permanent,,ObjectOverwrite)</f>
+        <v>EUR_YCONRH_EON40Y#0000</v>
+      </c>
+      <c r="M39" s="101" t="str">
+        <f>_xll.ohRangeRetrieveError(L39)</f>
+        <v/>
+      </c>
+      <c r="N39" s="165"/>
       <c r="P39" s="166"/>
       <c r="Q39" s="166"/>
     </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="100"/>
+      <c r="B40" s="172"/>
+      <c r="C40" s="171" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="172" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="171" t="str">
+        <f t="shared" si="4"/>
+        <v>50Y</v>
+      </c>
+      <c r="F40" s="170" t="s">
+        <v>179</v>
+      </c>
+      <c r="G40" s="170" t="s">
+        <v>172</v>
+      </c>
+      <c r="H40" s="170" t="str">
+        <f t="shared" si="0"/>
+        <v>Actual/360</v>
+      </c>
+      <c r="I40" s="169">
+        <v>0</v>
+      </c>
+      <c r="J40" s="168" t="str">
+        <f t="shared" si="1"/>
+        <v>EUREON50Y_Quote</v>
+      </c>
+      <c r="K40" s="168" t="str">
+        <f t="shared" si="2"/>
+        <v>EUR_YCONRH_EON50Y</v>
+      </c>
+      <c r="L40" s="167" t="str">
+        <f>_xll.qlOISRateHelper(K40,2,C40,J40,$L$4,Permanent,,ObjectOverwrite)</f>
+        <v>EUR_YCONRH_EON50Y#0000</v>
+      </c>
+      <c r="M40" s="101" t="str">
+        <f>_xll.ohRangeRetrieveError(L40)</f>
+        <v/>
+      </c>
+      <c r="N40" s="165"/>
+      <c r="P40" s="166"/>
+      <c r="Q40" s="166"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="100"/>
+      <c r="B41" s="172"/>
+      <c r="C41" s="171" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="172" t="s">
+        <v>109</v>
+      </c>
+      <c r="E41" s="171" t="str">
+        <f t="shared" si="3"/>
+        <v>60Y</v>
+      </c>
+      <c r="F41" s="170" t="s">
+        <v>179</v>
+      </c>
+      <c r="G41" s="170" t="s">
+        <v>172</v>
+      </c>
+      <c r="H41" s="170" t="str">
+        <f t="shared" si="0"/>
+        <v>Actual/360</v>
+      </c>
+      <c r="I41" s="169">
+        <v>0</v>
+      </c>
+      <c r="J41" s="168" t="str">
+        <f t="shared" si="1"/>
+        <v>EUREON60Y_Quote</v>
+      </c>
+      <c r="K41" s="168" t="str">
+        <f t="shared" si="2"/>
+        <v>EUR_YCONRH_EON60Y</v>
+      </c>
+      <c r="L41" s="167" t="str">
+        <f>_xll.qlOISRateHelper(K41,2,C41,J41,$L$4,Permanent,,ObjectOverwrite)</f>
+        <v>EUR_YCONRH_EON60Y#0000</v>
+      </c>
+      <c r="M41" s="101" t="str">
+        <f>_xll.ohRangeRetrieveError(L41)</f>
+        <v/>
+      </c>
+      <c r="N41" s="165"/>
+      <c r="P41" s="166"/>
+      <c r="Q41" s="166"/>
+    </row>
+    <row r="42" spans="1:17" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="99"/>
+      <c r="B42" s="98"/>
+      <c r="C42" s="98"/>
+      <c r="D42" s="98"/>
+      <c r="E42" s="98"/>
+      <c r="F42" s="98"/>
+      <c r="G42" s="98"/>
+      <c r="H42" s="98"/>
+      <c r="I42" s="98"/>
+      <c r="J42" s="98"/>
+      <c r="K42" s="98"/>
+      <c r="L42" s="164"/>
+      <c r="M42" s="164"/>
+      <c r="N42" s="163"/>
+      <c r="P42" s="166"/>
+      <c r="Q42" s="166"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G38 JC6:JC38 SY6:SY38 ACU6:ACU38 AMQ6:AMQ38 AWM6:AWM38 BGI6:BGI38 BQE6:BQE38 CAA6:CAA38 CJW6:CJW38 CTS6:CTS38 DDO6:DDO38 DNK6:DNK38 DXG6:DXG38 EHC6:EHC38 EQY6:EQY38 FAU6:FAU38 FKQ6:FKQ38 FUM6:FUM38 GEI6:GEI38 GOE6:GOE38 GYA6:GYA38 HHW6:HHW38 HRS6:HRS38 IBO6:IBO38 ILK6:ILK38 IVG6:IVG38 JFC6:JFC38 JOY6:JOY38 JYU6:JYU38 KIQ6:KIQ38 KSM6:KSM38 LCI6:LCI38 LME6:LME38 LWA6:LWA38 MFW6:MFW38 MPS6:MPS38 MZO6:MZO38 NJK6:NJK38 NTG6:NTG38 ODC6:ODC38 OMY6:OMY38 OWU6:OWU38 PGQ6:PGQ38 PQM6:PQM38 QAI6:QAI38 QKE6:QKE38 QUA6:QUA38 RDW6:RDW38 RNS6:RNS38 RXO6:RXO38 SHK6:SHK38 SRG6:SRG38 TBC6:TBC38 TKY6:TKY38 TUU6:TUU38 UEQ6:UEQ38 UOM6:UOM38 UYI6:UYI38 VIE6:VIE38 VSA6:VSA38 WBW6:WBW38 WLS6:WLS38 WVO6:WVO38 G65506:G65574 JC65506:JC65574 SY65506:SY65574 ACU65506:ACU65574 AMQ65506:AMQ65574 AWM65506:AWM65574 BGI65506:BGI65574 BQE65506:BQE65574 CAA65506:CAA65574 CJW65506:CJW65574 CTS65506:CTS65574 DDO65506:DDO65574 DNK65506:DNK65574 DXG65506:DXG65574 EHC65506:EHC65574 EQY65506:EQY65574 FAU65506:FAU65574 FKQ65506:FKQ65574 FUM65506:FUM65574 GEI65506:GEI65574 GOE65506:GOE65574 GYA65506:GYA65574 HHW65506:HHW65574 HRS65506:HRS65574 IBO65506:IBO65574 ILK65506:ILK65574 IVG65506:IVG65574 JFC65506:JFC65574 JOY65506:JOY65574 JYU65506:JYU65574 KIQ65506:KIQ65574 KSM65506:KSM65574 LCI65506:LCI65574 LME65506:LME65574 LWA65506:LWA65574 MFW65506:MFW65574 MPS65506:MPS65574 MZO65506:MZO65574 NJK65506:NJK65574 NTG65506:NTG65574 ODC65506:ODC65574 OMY65506:OMY65574 OWU65506:OWU65574 PGQ65506:PGQ65574 PQM65506:PQM65574 QAI65506:QAI65574 QKE65506:QKE65574 QUA65506:QUA65574 RDW65506:RDW65574 RNS65506:RNS65574 RXO65506:RXO65574 SHK65506:SHK65574 SRG65506:SRG65574 TBC65506:TBC65574 TKY65506:TKY65574 TUU65506:TUU65574 UEQ65506:UEQ65574 UOM65506:UOM65574 UYI65506:UYI65574 VIE65506:VIE65574 VSA65506:VSA65574 WBW65506:WBW65574 WLS65506:WLS65574 WVO65506:WVO65574 G131042:G131110 JC131042:JC131110 SY131042:SY131110 ACU131042:ACU131110 AMQ131042:AMQ131110 AWM131042:AWM131110 BGI131042:BGI131110 BQE131042:BQE131110 CAA131042:CAA131110 CJW131042:CJW131110 CTS131042:CTS131110 DDO131042:DDO131110 DNK131042:DNK131110 DXG131042:DXG131110 EHC131042:EHC131110 EQY131042:EQY131110 FAU131042:FAU131110 FKQ131042:FKQ131110 FUM131042:FUM131110 GEI131042:GEI131110 GOE131042:GOE131110 GYA131042:GYA131110 HHW131042:HHW131110 HRS131042:HRS131110 IBO131042:IBO131110 ILK131042:ILK131110 IVG131042:IVG131110 JFC131042:JFC131110 JOY131042:JOY131110 JYU131042:JYU131110 KIQ131042:KIQ131110 KSM131042:KSM131110 LCI131042:LCI131110 LME131042:LME131110 LWA131042:LWA131110 MFW131042:MFW131110 MPS131042:MPS131110 MZO131042:MZO131110 NJK131042:NJK131110 NTG131042:NTG131110 ODC131042:ODC131110 OMY131042:OMY131110 OWU131042:OWU131110 PGQ131042:PGQ131110 PQM131042:PQM131110 QAI131042:QAI131110 QKE131042:QKE131110 QUA131042:QUA131110 RDW131042:RDW131110 RNS131042:RNS131110 RXO131042:RXO131110 SHK131042:SHK131110 SRG131042:SRG131110 TBC131042:TBC131110 TKY131042:TKY131110 TUU131042:TUU131110 UEQ131042:UEQ131110 UOM131042:UOM131110 UYI131042:UYI131110 VIE131042:VIE131110 VSA131042:VSA131110 WBW131042:WBW131110 WLS131042:WLS131110 WVO131042:WVO131110 G196578:G196646 JC196578:JC196646 SY196578:SY196646 ACU196578:ACU196646 AMQ196578:AMQ196646 AWM196578:AWM196646 BGI196578:BGI196646 BQE196578:BQE196646 CAA196578:CAA196646 CJW196578:CJW196646 CTS196578:CTS196646 DDO196578:DDO196646 DNK196578:DNK196646 DXG196578:DXG196646 EHC196578:EHC196646 EQY196578:EQY196646 FAU196578:FAU196646 FKQ196578:FKQ196646 FUM196578:FUM196646 GEI196578:GEI196646 GOE196578:GOE196646 GYA196578:GYA196646 HHW196578:HHW196646 HRS196578:HRS196646 IBO196578:IBO196646 ILK196578:ILK196646 IVG196578:IVG196646 JFC196578:JFC196646 JOY196578:JOY196646 JYU196578:JYU196646 KIQ196578:KIQ196646 KSM196578:KSM196646 LCI196578:LCI196646 LME196578:LME196646 LWA196578:LWA196646 MFW196578:MFW196646 MPS196578:MPS196646 MZO196578:MZO196646 NJK196578:NJK196646 NTG196578:NTG196646 ODC196578:ODC196646 OMY196578:OMY196646 OWU196578:OWU196646 PGQ196578:PGQ196646 PQM196578:PQM196646 QAI196578:QAI196646 QKE196578:QKE196646 QUA196578:QUA196646 RDW196578:RDW196646 RNS196578:RNS196646 RXO196578:RXO196646 SHK196578:SHK196646 SRG196578:SRG196646 TBC196578:TBC196646 TKY196578:TKY196646 TUU196578:TUU196646 UEQ196578:UEQ196646 UOM196578:UOM196646 UYI196578:UYI196646 VIE196578:VIE196646 VSA196578:VSA196646 WBW196578:WBW196646 WLS196578:WLS196646 WVO196578:WVO196646 G262114:G262182 JC262114:JC262182 SY262114:SY262182 ACU262114:ACU262182 AMQ262114:AMQ262182 AWM262114:AWM262182 BGI262114:BGI262182 BQE262114:BQE262182 CAA262114:CAA262182 CJW262114:CJW262182 CTS262114:CTS262182 DDO262114:DDO262182 DNK262114:DNK262182 DXG262114:DXG262182 EHC262114:EHC262182 EQY262114:EQY262182 FAU262114:FAU262182 FKQ262114:FKQ262182 FUM262114:FUM262182 GEI262114:GEI262182 GOE262114:GOE262182 GYA262114:GYA262182 HHW262114:HHW262182 HRS262114:HRS262182 IBO262114:IBO262182 ILK262114:ILK262182 IVG262114:IVG262182 JFC262114:JFC262182 JOY262114:JOY262182 JYU262114:JYU262182 KIQ262114:KIQ262182 KSM262114:KSM262182 LCI262114:LCI262182 LME262114:LME262182 LWA262114:LWA262182 MFW262114:MFW262182 MPS262114:MPS262182 MZO262114:MZO262182 NJK262114:NJK262182 NTG262114:NTG262182 ODC262114:ODC262182 OMY262114:OMY262182 OWU262114:OWU262182 PGQ262114:PGQ262182 PQM262114:PQM262182 QAI262114:QAI262182 QKE262114:QKE262182 QUA262114:QUA262182 RDW262114:RDW262182 RNS262114:RNS262182 RXO262114:RXO262182 SHK262114:SHK262182 SRG262114:SRG262182 TBC262114:TBC262182 TKY262114:TKY262182 TUU262114:TUU262182 UEQ262114:UEQ262182 UOM262114:UOM262182 UYI262114:UYI262182 VIE262114:VIE262182 VSA262114:VSA262182 WBW262114:WBW262182 WLS262114:WLS262182 WVO262114:WVO262182 G327650:G327718 JC327650:JC327718 SY327650:SY327718 ACU327650:ACU327718 AMQ327650:AMQ327718 AWM327650:AWM327718 BGI327650:BGI327718 BQE327650:BQE327718 CAA327650:CAA327718 CJW327650:CJW327718 CTS327650:CTS327718 DDO327650:DDO327718 DNK327650:DNK327718 DXG327650:DXG327718 EHC327650:EHC327718 EQY327650:EQY327718 FAU327650:FAU327718 FKQ327650:FKQ327718 FUM327650:FUM327718 GEI327650:GEI327718 GOE327650:GOE327718 GYA327650:GYA327718 HHW327650:HHW327718 HRS327650:HRS327718 IBO327650:IBO327718 ILK327650:ILK327718 IVG327650:IVG327718 JFC327650:JFC327718 JOY327650:JOY327718 JYU327650:JYU327718 KIQ327650:KIQ327718 KSM327650:KSM327718 LCI327650:LCI327718 LME327650:LME327718 LWA327650:LWA327718 MFW327650:MFW327718 MPS327650:MPS327718 MZO327650:MZO327718 NJK327650:NJK327718 NTG327650:NTG327718 ODC327650:ODC327718 OMY327650:OMY327718 OWU327650:OWU327718 PGQ327650:PGQ327718 PQM327650:PQM327718 QAI327650:QAI327718 QKE327650:QKE327718 QUA327650:QUA327718 RDW327650:RDW327718 RNS327650:RNS327718 RXO327650:RXO327718 SHK327650:SHK327718 SRG327650:SRG327718 TBC327650:TBC327718 TKY327650:TKY327718 TUU327650:TUU327718 UEQ327650:UEQ327718 UOM327650:UOM327718 UYI327650:UYI327718 VIE327650:VIE327718 VSA327650:VSA327718 WBW327650:WBW327718 WLS327650:WLS327718 WVO327650:WVO327718 G393186:G393254 JC393186:JC393254 SY393186:SY393254 ACU393186:ACU393254 AMQ393186:AMQ393254 AWM393186:AWM393254 BGI393186:BGI393254 BQE393186:BQE393254 CAA393186:CAA393254 CJW393186:CJW393254 CTS393186:CTS393254 DDO393186:DDO393254 DNK393186:DNK393254 DXG393186:DXG393254 EHC393186:EHC393254 EQY393186:EQY393254 FAU393186:FAU393254 FKQ393186:FKQ393254 FUM393186:FUM393254 GEI393186:GEI393254 GOE393186:GOE393254 GYA393186:GYA393254 HHW393186:HHW393254 HRS393186:HRS393254 IBO393186:IBO393254 ILK393186:ILK393254 IVG393186:IVG393254 JFC393186:JFC393254 JOY393186:JOY393254 JYU393186:JYU393254 KIQ393186:KIQ393254 KSM393186:KSM393254 LCI393186:LCI393254 LME393186:LME393254 LWA393186:LWA393254 MFW393186:MFW393254 MPS393186:MPS393254 MZO393186:MZO393254 NJK393186:NJK393254 NTG393186:NTG393254 ODC393186:ODC393254 OMY393186:OMY393254 OWU393186:OWU393254 PGQ393186:PGQ393254 PQM393186:PQM393254 QAI393186:QAI393254 QKE393186:QKE393254 QUA393186:QUA393254 RDW393186:RDW393254 RNS393186:RNS393254 RXO393186:RXO393254 SHK393186:SHK393254 SRG393186:SRG393254 TBC393186:TBC393254 TKY393186:TKY393254 TUU393186:TUU393254 UEQ393186:UEQ393254 UOM393186:UOM393254 UYI393186:UYI393254 VIE393186:VIE393254 VSA393186:VSA393254 WBW393186:WBW393254 WLS393186:WLS393254 WVO393186:WVO393254 G458722:G458790 JC458722:JC458790 SY458722:SY458790 ACU458722:ACU458790 AMQ458722:AMQ458790 AWM458722:AWM458790 BGI458722:BGI458790 BQE458722:BQE458790 CAA458722:CAA458790 CJW458722:CJW458790 CTS458722:CTS458790 DDO458722:DDO458790 DNK458722:DNK458790 DXG458722:DXG458790 EHC458722:EHC458790 EQY458722:EQY458790 FAU458722:FAU458790 FKQ458722:FKQ458790 FUM458722:FUM458790 GEI458722:GEI458790 GOE458722:GOE458790 GYA458722:GYA458790 HHW458722:HHW458790 HRS458722:HRS458790 IBO458722:IBO458790 ILK458722:ILK458790 IVG458722:IVG458790 JFC458722:JFC458790 JOY458722:JOY458790 JYU458722:JYU458790 KIQ458722:KIQ458790 KSM458722:KSM458790 LCI458722:LCI458790 LME458722:LME458790 LWA458722:LWA458790 MFW458722:MFW458790 MPS458722:MPS458790 MZO458722:MZO458790 NJK458722:NJK458790 NTG458722:NTG458790 ODC458722:ODC458790 OMY458722:OMY458790 OWU458722:OWU458790 PGQ458722:PGQ458790 PQM458722:PQM458790 QAI458722:QAI458790 QKE458722:QKE458790 QUA458722:QUA458790 RDW458722:RDW458790 RNS458722:RNS458790 RXO458722:RXO458790 SHK458722:SHK458790 SRG458722:SRG458790 TBC458722:TBC458790 TKY458722:TKY458790 TUU458722:TUU458790 UEQ458722:UEQ458790 UOM458722:UOM458790 UYI458722:UYI458790 VIE458722:VIE458790 VSA458722:VSA458790 WBW458722:WBW458790 WLS458722:WLS458790 WVO458722:WVO458790 G524258:G524326 JC524258:JC524326 SY524258:SY524326 ACU524258:ACU524326 AMQ524258:AMQ524326 AWM524258:AWM524326 BGI524258:BGI524326 BQE524258:BQE524326 CAA524258:CAA524326 CJW524258:CJW524326 CTS524258:CTS524326 DDO524258:DDO524326 DNK524258:DNK524326 DXG524258:DXG524326 EHC524258:EHC524326 EQY524258:EQY524326 FAU524258:FAU524326 FKQ524258:FKQ524326 FUM524258:FUM524326 GEI524258:GEI524326 GOE524258:GOE524326 GYA524258:GYA524326 HHW524258:HHW524326 HRS524258:HRS524326 IBO524258:IBO524326 ILK524258:ILK524326 IVG524258:IVG524326 JFC524258:JFC524326 JOY524258:JOY524326 JYU524258:JYU524326 KIQ524258:KIQ524326 KSM524258:KSM524326 LCI524258:LCI524326 LME524258:LME524326 LWA524258:LWA524326 MFW524258:MFW524326 MPS524258:MPS524326 MZO524258:MZO524326 NJK524258:NJK524326 NTG524258:NTG524326 ODC524258:ODC524326 OMY524258:OMY524326 OWU524258:OWU524326 PGQ524258:PGQ524326 PQM524258:PQM524326 QAI524258:QAI524326 QKE524258:QKE524326 QUA524258:QUA524326 RDW524258:RDW524326 RNS524258:RNS524326 RXO524258:RXO524326 SHK524258:SHK524326 SRG524258:SRG524326 TBC524258:TBC524326 TKY524258:TKY524326 TUU524258:TUU524326 UEQ524258:UEQ524326 UOM524258:UOM524326 UYI524258:UYI524326 VIE524258:VIE524326 VSA524258:VSA524326 WBW524258:WBW524326 WLS524258:WLS524326 WVO524258:WVO524326 G589794:G589862 JC589794:JC589862 SY589794:SY589862 ACU589794:ACU589862 AMQ589794:AMQ589862 AWM589794:AWM589862 BGI589794:BGI589862 BQE589794:BQE589862 CAA589794:CAA589862 CJW589794:CJW589862 CTS589794:CTS589862 DDO589794:DDO589862 DNK589794:DNK589862 DXG589794:DXG589862 EHC589794:EHC589862 EQY589794:EQY589862 FAU589794:FAU589862 FKQ589794:FKQ589862 FUM589794:FUM589862 GEI589794:GEI589862 GOE589794:GOE589862 GYA589794:GYA589862 HHW589794:HHW589862 HRS589794:HRS589862 IBO589794:IBO589862 ILK589794:ILK589862 IVG589794:IVG589862 JFC589794:JFC589862 JOY589794:JOY589862 JYU589794:JYU589862 KIQ589794:KIQ589862 KSM589794:KSM589862 LCI589794:LCI589862 LME589794:LME589862 LWA589794:LWA589862 MFW589794:MFW589862 MPS589794:MPS589862 MZO589794:MZO589862 NJK589794:NJK589862 NTG589794:NTG589862 ODC589794:ODC589862 OMY589794:OMY589862 OWU589794:OWU589862 PGQ589794:PGQ589862 PQM589794:PQM589862 QAI589794:QAI589862 QKE589794:QKE589862 QUA589794:QUA589862 RDW589794:RDW589862 RNS589794:RNS589862 RXO589794:RXO589862 SHK589794:SHK589862 SRG589794:SRG589862 TBC589794:TBC589862 TKY589794:TKY589862 TUU589794:TUU589862 UEQ589794:UEQ589862 UOM589794:UOM589862 UYI589794:UYI589862 VIE589794:VIE589862 VSA589794:VSA589862 WBW589794:WBW589862 WLS589794:WLS589862 WVO589794:WVO589862 G655330:G655398 JC655330:JC655398 SY655330:SY655398 ACU655330:ACU655398 AMQ655330:AMQ655398 AWM655330:AWM655398 BGI655330:BGI655398 BQE655330:BQE655398 CAA655330:CAA655398 CJW655330:CJW655398 CTS655330:CTS655398 DDO655330:DDO655398 DNK655330:DNK655398 DXG655330:DXG655398 EHC655330:EHC655398 EQY655330:EQY655398 FAU655330:FAU655398 FKQ655330:FKQ655398 FUM655330:FUM655398 GEI655330:GEI655398 GOE655330:GOE655398 GYA655330:GYA655398 HHW655330:HHW655398 HRS655330:HRS655398 IBO655330:IBO655398 ILK655330:ILK655398 IVG655330:IVG655398 JFC655330:JFC655398 JOY655330:JOY655398 JYU655330:JYU655398 KIQ655330:KIQ655398 KSM655330:KSM655398 LCI655330:LCI655398 LME655330:LME655398 LWA655330:LWA655398 MFW655330:MFW655398 MPS655330:MPS655398 MZO655330:MZO655398 NJK655330:NJK655398 NTG655330:NTG655398 ODC655330:ODC655398 OMY655330:OMY655398 OWU655330:OWU655398 PGQ655330:PGQ655398 PQM655330:PQM655398 QAI655330:QAI655398 QKE655330:QKE655398 QUA655330:QUA655398 RDW655330:RDW655398 RNS655330:RNS655398 RXO655330:RXO655398 SHK655330:SHK655398 SRG655330:SRG655398 TBC655330:TBC655398 TKY655330:TKY655398 TUU655330:TUU655398 UEQ655330:UEQ655398 UOM655330:UOM655398 UYI655330:UYI655398 VIE655330:VIE655398 VSA655330:VSA655398 WBW655330:WBW655398 WLS655330:WLS655398 WVO655330:WVO655398 G720866:G720934 JC720866:JC720934 SY720866:SY720934 ACU720866:ACU720934 AMQ720866:AMQ720934 AWM720866:AWM720934 BGI720866:BGI720934 BQE720866:BQE720934 CAA720866:CAA720934 CJW720866:CJW720934 CTS720866:CTS720934 DDO720866:DDO720934 DNK720866:DNK720934 DXG720866:DXG720934 EHC720866:EHC720934 EQY720866:EQY720934 FAU720866:FAU720934 FKQ720866:FKQ720934 FUM720866:FUM720934 GEI720866:GEI720934 GOE720866:GOE720934 GYA720866:GYA720934 HHW720866:HHW720934 HRS720866:HRS720934 IBO720866:IBO720934 ILK720866:ILK720934 IVG720866:IVG720934 JFC720866:JFC720934 JOY720866:JOY720934 JYU720866:JYU720934 KIQ720866:KIQ720934 KSM720866:KSM720934 LCI720866:LCI720934 LME720866:LME720934 LWA720866:LWA720934 MFW720866:MFW720934 MPS720866:MPS720934 MZO720866:MZO720934 NJK720866:NJK720934 NTG720866:NTG720934 ODC720866:ODC720934 OMY720866:OMY720934 OWU720866:OWU720934 PGQ720866:PGQ720934 PQM720866:PQM720934 QAI720866:QAI720934 QKE720866:QKE720934 QUA720866:QUA720934 RDW720866:RDW720934 RNS720866:RNS720934 RXO720866:RXO720934 SHK720866:SHK720934 SRG720866:SRG720934 TBC720866:TBC720934 TKY720866:TKY720934 TUU720866:TUU720934 UEQ720866:UEQ720934 UOM720866:UOM720934 UYI720866:UYI720934 VIE720866:VIE720934 VSA720866:VSA720934 WBW720866:WBW720934 WLS720866:WLS720934 WVO720866:WVO720934 G786402:G786470 JC786402:JC786470 SY786402:SY786470 ACU786402:ACU786470 AMQ786402:AMQ786470 AWM786402:AWM786470 BGI786402:BGI786470 BQE786402:BQE786470 CAA786402:CAA786470 CJW786402:CJW786470 CTS786402:CTS786470 DDO786402:DDO786470 DNK786402:DNK786470 DXG786402:DXG786470 EHC786402:EHC786470 EQY786402:EQY786470 FAU786402:FAU786470 FKQ786402:FKQ786470 FUM786402:FUM786470 GEI786402:GEI786470 GOE786402:GOE786470 GYA786402:GYA786470 HHW786402:HHW786470 HRS786402:HRS786470 IBO786402:IBO786470 ILK786402:ILK786470 IVG786402:IVG786470 JFC786402:JFC786470 JOY786402:JOY786470 JYU786402:JYU786470 KIQ786402:KIQ786470 KSM786402:KSM786470 LCI786402:LCI786470 LME786402:LME786470 LWA786402:LWA786470 MFW786402:MFW786470 MPS786402:MPS786470 MZO786402:MZO786470 NJK786402:NJK786470 NTG786402:NTG786470 ODC786402:ODC786470 OMY786402:OMY786470 OWU786402:OWU786470 PGQ786402:PGQ786470 PQM786402:PQM786470 QAI786402:QAI786470 QKE786402:QKE786470 QUA786402:QUA786470 RDW786402:RDW786470 RNS786402:RNS786470 RXO786402:RXO786470 SHK786402:SHK786470 SRG786402:SRG786470 TBC786402:TBC786470 TKY786402:TKY786470 TUU786402:TUU786470 UEQ786402:UEQ786470 UOM786402:UOM786470 UYI786402:UYI786470 VIE786402:VIE786470 VSA786402:VSA786470 WBW786402:WBW786470 WLS786402:WLS786470 WVO786402:WVO786470 G851938:G852006 JC851938:JC852006 SY851938:SY852006 ACU851938:ACU852006 AMQ851938:AMQ852006 AWM851938:AWM852006 BGI851938:BGI852006 BQE851938:BQE852006 CAA851938:CAA852006 CJW851938:CJW852006 CTS851938:CTS852006 DDO851938:DDO852006 DNK851938:DNK852006 DXG851938:DXG852006 EHC851938:EHC852006 EQY851938:EQY852006 FAU851938:FAU852006 FKQ851938:FKQ852006 FUM851938:FUM852006 GEI851938:GEI852006 GOE851938:GOE852006 GYA851938:GYA852006 HHW851938:HHW852006 HRS851938:HRS852006 IBO851938:IBO852006 ILK851938:ILK852006 IVG851938:IVG852006 JFC851938:JFC852006 JOY851938:JOY852006 JYU851938:JYU852006 KIQ851938:KIQ852006 KSM851938:KSM852006 LCI851938:LCI852006 LME851938:LME852006 LWA851938:LWA852006 MFW851938:MFW852006 MPS851938:MPS852006 MZO851938:MZO852006 NJK851938:NJK852006 NTG851938:NTG852006 ODC851938:ODC852006 OMY851938:OMY852006 OWU851938:OWU852006 PGQ851938:PGQ852006 PQM851938:PQM852006 QAI851938:QAI852006 QKE851938:QKE852006 QUA851938:QUA852006 RDW851938:RDW852006 RNS851938:RNS852006 RXO851938:RXO852006 SHK851938:SHK852006 SRG851938:SRG852006 TBC851938:TBC852006 TKY851938:TKY852006 TUU851938:TUU852006 UEQ851938:UEQ852006 UOM851938:UOM852006 UYI851938:UYI852006 VIE851938:VIE852006 VSA851938:VSA852006 WBW851938:WBW852006 WLS851938:WLS852006 WVO851938:WVO852006 G917474:G917542 JC917474:JC917542 SY917474:SY917542 ACU917474:ACU917542 AMQ917474:AMQ917542 AWM917474:AWM917542 BGI917474:BGI917542 BQE917474:BQE917542 CAA917474:CAA917542 CJW917474:CJW917542 CTS917474:CTS917542 DDO917474:DDO917542 DNK917474:DNK917542 DXG917474:DXG917542 EHC917474:EHC917542 EQY917474:EQY917542 FAU917474:FAU917542 FKQ917474:FKQ917542 FUM917474:FUM917542 GEI917474:GEI917542 GOE917474:GOE917542 GYA917474:GYA917542 HHW917474:HHW917542 HRS917474:HRS917542 IBO917474:IBO917542 ILK917474:ILK917542 IVG917474:IVG917542 JFC917474:JFC917542 JOY917474:JOY917542 JYU917474:JYU917542 KIQ917474:KIQ917542 KSM917474:KSM917542 LCI917474:LCI917542 LME917474:LME917542 LWA917474:LWA917542 MFW917474:MFW917542 MPS917474:MPS917542 MZO917474:MZO917542 NJK917474:NJK917542 NTG917474:NTG917542 ODC917474:ODC917542 OMY917474:OMY917542 OWU917474:OWU917542 PGQ917474:PGQ917542 PQM917474:PQM917542 QAI917474:QAI917542 QKE917474:QKE917542 QUA917474:QUA917542 RDW917474:RDW917542 RNS917474:RNS917542 RXO917474:RXO917542 SHK917474:SHK917542 SRG917474:SRG917542 TBC917474:TBC917542 TKY917474:TKY917542 TUU917474:TUU917542 UEQ917474:UEQ917542 UOM917474:UOM917542 UYI917474:UYI917542 VIE917474:VIE917542 VSA917474:VSA917542 WBW917474:WBW917542 WLS917474:WLS917542 WVO917474:WVO917542 G983010:G983078 JC983010:JC983078 SY983010:SY983078 ACU983010:ACU983078 AMQ983010:AMQ983078 AWM983010:AWM983078 BGI983010:BGI983078 BQE983010:BQE983078 CAA983010:CAA983078 CJW983010:CJW983078 CTS983010:CTS983078 DDO983010:DDO983078 DNK983010:DNK983078 DXG983010:DXG983078 EHC983010:EHC983078 EQY983010:EQY983078 FAU983010:FAU983078 FKQ983010:FKQ983078 FUM983010:FUM983078 GEI983010:GEI983078 GOE983010:GOE983078 GYA983010:GYA983078 HHW983010:HHW983078 HRS983010:HRS983078 IBO983010:IBO983078 ILK983010:ILK983078 IVG983010:IVG983078 JFC983010:JFC983078 JOY983010:JOY983078 JYU983010:JYU983078 KIQ983010:KIQ983078 KSM983010:KSM983078 LCI983010:LCI983078 LME983010:LME983078 LWA983010:LWA983078 MFW983010:MFW983078 MPS983010:MPS983078 MZO983010:MZO983078 NJK983010:NJK983078 NTG983010:NTG983078 ODC983010:ODC983078 OMY983010:OMY983078 OWU983010:OWU983078 PGQ983010:PGQ983078 PQM983010:PQM983078 QAI983010:QAI983078 QKE983010:QKE983078 QUA983010:QUA983078 RDW983010:RDW983078 RNS983010:RNS983078 RXO983010:RXO983078 SHK983010:SHK983078 SRG983010:SRG983078 TBC983010:TBC983078 TKY983010:TKY983078 TUU983010:TUU983078 UEQ983010:UEQ983078 UOM983010:UOM983078 UYI983010:UYI983078 VIE983010:VIE983078 VSA983010:VSA983078 WBW983010:WBW983078 WLS983010:WLS983078 WVO983010:WVO983078">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVO983013:WVO983081 G65509:G65577 JC65509:JC65577 SY65509:SY65577 ACU65509:ACU65577 AMQ65509:AMQ65577 AWM65509:AWM65577 BGI65509:BGI65577 BQE65509:BQE65577 CAA65509:CAA65577 CJW65509:CJW65577 CTS65509:CTS65577 DDO65509:DDO65577 DNK65509:DNK65577 DXG65509:DXG65577 EHC65509:EHC65577 EQY65509:EQY65577 FAU65509:FAU65577 FKQ65509:FKQ65577 FUM65509:FUM65577 GEI65509:GEI65577 GOE65509:GOE65577 GYA65509:GYA65577 HHW65509:HHW65577 HRS65509:HRS65577 IBO65509:IBO65577 ILK65509:ILK65577 IVG65509:IVG65577 JFC65509:JFC65577 JOY65509:JOY65577 JYU65509:JYU65577 KIQ65509:KIQ65577 KSM65509:KSM65577 LCI65509:LCI65577 LME65509:LME65577 LWA65509:LWA65577 MFW65509:MFW65577 MPS65509:MPS65577 MZO65509:MZO65577 NJK65509:NJK65577 NTG65509:NTG65577 ODC65509:ODC65577 OMY65509:OMY65577 OWU65509:OWU65577 PGQ65509:PGQ65577 PQM65509:PQM65577 QAI65509:QAI65577 QKE65509:QKE65577 QUA65509:QUA65577 RDW65509:RDW65577 RNS65509:RNS65577 RXO65509:RXO65577 SHK65509:SHK65577 SRG65509:SRG65577 TBC65509:TBC65577 TKY65509:TKY65577 TUU65509:TUU65577 UEQ65509:UEQ65577 UOM65509:UOM65577 UYI65509:UYI65577 VIE65509:VIE65577 VSA65509:VSA65577 WBW65509:WBW65577 WLS65509:WLS65577 WVO65509:WVO65577 G131045:G131113 JC131045:JC131113 SY131045:SY131113 ACU131045:ACU131113 AMQ131045:AMQ131113 AWM131045:AWM131113 BGI131045:BGI131113 BQE131045:BQE131113 CAA131045:CAA131113 CJW131045:CJW131113 CTS131045:CTS131113 DDO131045:DDO131113 DNK131045:DNK131113 DXG131045:DXG131113 EHC131045:EHC131113 EQY131045:EQY131113 FAU131045:FAU131113 FKQ131045:FKQ131113 FUM131045:FUM131113 GEI131045:GEI131113 GOE131045:GOE131113 GYA131045:GYA131113 HHW131045:HHW131113 HRS131045:HRS131113 IBO131045:IBO131113 ILK131045:ILK131113 IVG131045:IVG131113 JFC131045:JFC131113 JOY131045:JOY131113 JYU131045:JYU131113 KIQ131045:KIQ131113 KSM131045:KSM131113 LCI131045:LCI131113 LME131045:LME131113 LWA131045:LWA131113 MFW131045:MFW131113 MPS131045:MPS131113 MZO131045:MZO131113 NJK131045:NJK131113 NTG131045:NTG131113 ODC131045:ODC131113 OMY131045:OMY131113 OWU131045:OWU131113 PGQ131045:PGQ131113 PQM131045:PQM131113 QAI131045:QAI131113 QKE131045:QKE131113 QUA131045:QUA131113 RDW131045:RDW131113 RNS131045:RNS131113 RXO131045:RXO131113 SHK131045:SHK131113 SRG131045:SRG131113 TBC131045:TBC131113 TKY131045:TKY131113 TUU131045:TUU131113 UEQ131045:UEQ131113 UOM131045:UOM131113 UYI131045:UYI131113 VIE131045:VIE131113 VSA131045:VSA131113 WBW131045:WBW131113 WLS131045:WLS131113 WVO131045:WVO131113 G196581:G196649 JC196581:JC196649 SY196581:SY196649 ACU196581:ACU196649 AMQ196581:AMQ196649 AWM196581:AWM196649 BGI196581:BGI196649 BQE196581:BQE196649 CAA196581:CAA196649 CJW196581:CJW196649 CTS196581:CTS196649 DDO196581:DDO196649 DNK196581:DNK196649 DXG196581:DXG196649 EHC196581:EHC196649 EQY196581:EQY196649 FAU196581:FAU196649 FKQ196581:FKQ196649 FUM196581:FUM196649 GEI196581:GEI196649 GOE196581:GOE196649 GYA196581:GYA196649 HHW196581:HHW196649 HRS196581:HRS196649 IBO196581:IBO196649 ILK196581:ILK196649 IVG196581:IVG196649 JFC196581:JFC196649 JOY196581:JOY196649 JYU196581:JYU196649 KIQ196581:KIQ196649 KSM196581:KSM196649 LCI196581:LCI196649 LME196581:LME196649 LWA196581:LWA196649 MFW196581:MFW196649 MPS196581:MPS196649 MZO196581:MZO196649 NJK196581:NJK196649 NTG196581:NTG196649 ODC196581:ODC196649 OMY196581:OMY196649 OWU196581:OWU196649 PGQ196581:PGQ196649 PQM196581:PQM196649 QAI196581:QAI196649 QKE196581:QKE196649 QUA196581:QUA196649 RDW196581:RDW196649 RNS196581:RNS196649 RXO196581:RXO196649 SHK196581:SHK196649 SRG196581:SRG196649 TBC196581:TBC196649 TKY196581:TKY196649 TUU196581:TUU196649 UEQ196581:UEQ196649 UOM196581:UOM196649 UYI196581:UYI196649 VIE196581:VIE196649 VSA196581:VSA196649 WBW196581:WBW196649 WLS196581:WLS196649 WVO196581:WVO196649 G262117:G262185 JC262117:JC262185 SY262117:SY262185 ACU262117:ACU262185 AMQ262117:AMQ262185 AWM262117:AWM262185 BGI262117:BGI262185 BQE262117:BQE262185 CAA262117:CAA262185 CJW262117:CJW262185 CTS262117:CTS262185 DDO262117:DDO262185 DNK262117:DNK262185 DXG262117:DXG262185 EHC262117:EHC262185 EQY262117:EQY262185 FAU262117:FAU262185 FKQ262117:FKQ262185 FUM262117:FUM262185 GEI262117:GEI262185 GOE262117:GOE262185 GYA262117:GYA262185 HHW262117:HHW262185 HRS262117:HRS262185 IBO262117:IBO262185 ILK262117:ILK262185 IVG262117:IVG262185 JFC262117:JFC262185 JOY262117:JOY262185 JYU262117:JYU262185 KIQ262117:KIQ262185 KSM262117:KSM262185 LCI262117:LCI262185 LME262117:LME262185 LWA262117:LWA262185 MFW262117:MFW262185 MPS262117:MPS262185 MZO262117:MZO262185 NJK262117:NJK262185 NTG262117:NTG262185 ODC262117:ODC262185 OMY262117:OMY262185 OWU262117:OWU262185 PGQ262117:PGQ262185 PQM262117:PQM262185 QAI262117:QAI262185 QKE262117:QKE262185 QUA262117:QUA262185 RDW262117:RDW262185 RNS262117:RNS262185 RXO262117:RXO262185 SHK262117:SHK262185 SRG262117:SRG262185 TBC262117:TBC262185 TKY262117:TKY262185 TUU262117:TUU262185 UEQ262117:UEQ262185 UOM262117:UOM262185 UYI262117:UYI262185 VIE262117:VIE262185 VSA262117:VSA262185 WBW262117:WBW262185 WLS262117:WLS262185 WVO262117:WVO262185 G327653:G327721 JC327653:JC327721 SY327653:SY327721 ACU327653:ACU327721 AMQ327653:AMQ327721 AWM327653:AWM327721 BGI327653:BGI327721 BQE327653:BQE327721 CAA327653:CAA327721 CJW327653:CJW327721 CTS327653:CTS327721 DDO327653:DDO327721 DNK327653:DNK327721 DXG327653:DXG327721 EHC327653:EHC327721 EQY327653:EQY327721 FAU327653:FAU327721 FKQ327653:FKQ327721 FUM327653:FUM327721 GEI327653:GEI327721 GOE327653:GOE327721 GYA327653:GYA327721 HHW327653:HHW327721 HRS327653:HRS327721 IBO327653:IBO327721 ILK327653:ILK327721 IVG327653:IVG327721 JFC327653:JFC327721 JOY327653:JOY327721 JYU327653:JYU327721 KIQ327653:KIQ327721 KSM327653:KSM327721 LCI327653:LCI327721 LME327653:LME327721 LWA327653:LWA327721 MFW327653:MFW327721 MPS327653:MPS327721 MZO327653:MZO327721 NJK327653:NJK327721 NTG327653:NTG327721 ODC327653:ODC327721 OMY327653:OMY327721 OWU327653:OWU327721 PGQ327653:PGQ327721 PQM327653:PQM327721 QAI327653:QAI327721 QKE327653:QKE327721 QUA327653:QUA327721 RDW327653:RDW327721 RNS327653:RNS327721 RXO327653:RXO327721 SHK327653:SHK327721 SRG327653:SRG327721 TBC327653:TBC327721 TKY327653:TKY327721 TUU327653:TUU327721 UEQ327653:UEQ327721 UOM327653:UOM327721 UYI327653:UYI327721 VIE327653:VIE327721 VSA327653:VSA327721 WBW327653:WBW327721 WLS327653:WLS327721 WVO327653:WVO327721 G393189:G393257 JC393189:JC393257 SY393189:SY393257 ACU393189:ACU393257 AMQ393189:AMQ393257 AWM393189:AWM393257 BGI393189:BGI393257 BQE393189:BQE393257 CAA393189:CAA393257 CJW393189:CJW393257 CTS393189:CTS393257 DDO393189:DDO393257 DNK393189:DNK393257 DXG393189:DXG393257 EHC393189:EHC393257 EQY393189:EQY393257 FAU393189:FAU393257 FKQ393189:FKQ393257 FUM393189:FUM393257 GEI393189:GEI393257 GOE393189:GOE393257 GYA393189:GYA393257 HHW393189:HHW393257 HRS393189:HRS393257 IBO393189:IBO393257 ILK393189:ILK393257 IVG393189:IVG393257 JFC393189:JFC393257 JOY393189:JOY393257 JYU393189:JYU393257 KIQ393189:KIQ393257 KSM393189:KSM393257 LCI393189:LCI393257 LME393189:LME393257 LWA393189:LWA393257 MFW393189:MFW393257 MPS393189:MPS393257 MZO393189:MZO393257 NJK393189:NJK393257 NTG393189:NTG393257 ODC393189:ODC393257 OMY393189:OMY393257 OWU393189:OWU393257 PGQ393189:PGQ393257 PQM393189:PQM393257 QAI393189:QAI393257 QKE393189:QKE393257 QUA393189:QUA393257 RDW393189:RDW393257 RNS393189:RNS393257 RXO393189:RXO393257 SHK393189:SHK393257 SRG393189:SRG393257 TBC393189:TBC393257 TKY393189:TKY393257 TUU393189:TUU393257 UEQ393189:UEQ393257 UOM393189:UOM393257 UYI393189:UYI393257 VIE393189:VIE393257 VSA393189:VSA393257 WBW393189:WBW393257 WLS393189:WLS393257 WVO393189:WVO393257 G458725:G458793 JC458725:JC458793 SY458725:SY458793 ACU458725:ACU458793 AMQ458725:AMQ458793 AWM458725:AWM458793 BGI458725:BGI458793 BQE458725:BQE458793 CAA458725:CAA458793 CJW458725:CJW458793 CTS458725:CTS458793 DDO458725:DDO458793 DNK458725:DNK458793 DXG458725:DXG458793 EHC458725:EHC458793 EQY458725:EQY458793 FAU458725:FAU458793 FKQ458725:FKQ458793 FUM458725:FUM458793 GEI458725:GEI458793 GOE458725:GOE458793 GYA458725:GYA458793 HHW458725:HHW458793 HRS458725:HRS458793 IBO458725:IBO458793 ILK458725:ILK458793 IVG458725:IVG458793 JFC458725:JFC458793 JOY458725:JOY458793 JYU458725:JYU458793 KIQ458725:KIQ458793 KSM458725:KSM458793 LCI458725:LCI458793 LME458725:LME458793 LWA458725:LWA458793 MFW458725:MFW458793 MPS458725:MPS458793 MZO458725:MZO458793 NJK458725:NJK458793 NTG458725:NTG458793 ODC458725:ODC458793 OMY458725:OMY458793 OWU458725:OWU458793 PGQ458725:PGQ458793 PQM458725:PQM458793 QAI458725:QAI458793 QKE458725:QKE458793 QUA458725:QUA458793 RDW458725:RDW458793 RNS458725:RNS458793 RXO458725:RXO458793 SHK458725:SHK458793 SRG458725:SRG458793 TBC458725:TBC458793 TKY458725:TKY458793 TUU458725:TUU458793 UEQ458725:UEQ458793 UOM458725:UOM458793 UYI458725:UYI458793 VIE458725:VIE458793 VSA458725:VSA458793 WBW458725:WBW458793 WLS458725:WLS458793 WVO458725:WVO458793 G524261:G524329 JC524261:JC524329 SY524261:SY524329 ACU524261:ACU524329 AMQ524261:AMQ524329 AWM524261:AWM524329 BGI524261:BGI524329 BQE524261:BQE524329 CAA524261:CAA524329 CJW524261:CJW524329 CTS524261:CTS524329 DDO524261:DDO524329 DNK524261:DNK524329 DXG524261:DXG524329 EHC524261:EHC524329 EQY524261:EQY524329 FAU524261:FAU524329 FKQ524261:FKQ524329 FUM524261:FUM524329 GEI524261:GEI524329 GOE524261:GOE524329 GYA524261:GYA524329 HHW524261:HHW524329 HRS524261:HRS524329 IBO524261:IBO524329 ILK524261:ILK524329 IVG524261:IVG524329 JFC524261:JFC524329 JOY524261:JOY524329 JYU524261:JYU524329 KIQ524261:KIQ524329 KSM524261:KSM524329 LCI524261:LCI524329 LME524261:LME524329 LWA524261:LWA524329 MFW524261:MFW524329 MPS524261:MPS524329 MZO524261:MZO524329 NJK524261:NJK524329 NTG524261:NTG524329 ODC524261:ODC524329 OMY524261:OMY524329 OWU524261:OWU524329 PGQ524261:PGQ524329 PQM524261:PQM524329 QAI524261:QAI524329 QKE524261:QKE524329 QUA524261:QUA524329 RDW524261:RDW524329 RNS524261:RNS524329 RXO524261:RXO524329 SHK524261:SHK524329 SRG524261:SRG524329 TBC524261:TBC524329 TKY524261:TKY524329 TUU524261:TUU524329 UEQ524261:UEQ524329 UOM524261:UOM524329 UYI524261:UYI524329 VIE524261:VIE524329 VSA524261:VSA524329 WBW524261:WBW524329 WLS524261:WLS524329 WVO524261:WVO524329 G589797:G589865 JC589797:JC589865 SY589797:SY589865 ACU589797:ACU589865 AMQ589797:AMQ589865 AWM589797:AWM589865 BGI589797:BGI589865 BQE589797:BQE589865 CAA589797:CAA589865 CJW589797:CJW589865 CTS589797:CTS589865 DDO589797:DDO589865 DNK589797:DNK589865 DXG589797:DXG589865 EHC589797:EHC589865 EQY589797:EQY589865 FAU589797:FAU589865 FKQ589797:FKQ589865 FUM589797:FUM589865 GEI589797:GEI589865 GOE589797:GOE589865 GYA589797:GYA589865 HHW589797:HHW589865 HRS589797:HRS589865 IBO589797:IBO589865 ILK589797:ILK589865 IVG589797:IVG589865 JFC589797:JFC589865 JOY589797:JOY589865 JYU589797:JYU589865 KIQ589797:KIQ589865 KSM589797:KSM589865 LCI589797:LCI589865 LME589797:LME589865 LWA589797:LWA589865 MFW589797:MFW589865 MPS589797:MPS589865 MZO589797:MZO589865 NJK589797:NJK589865 NTG589797:NTG589865 ODC589797:ODC589865 OMY589797:OMY589865 OWU589797:OWU589865 PGQ589797:PGQ589865 PQM589797:PQM589865 QAI589797:QAI589865 QKE589797:QKE589865 QUA589797:QUA589865 RDW589797:RDW589865 RNS589797:RNS589865 RXO589797:RXO589865 SHK589797:SHK589865 SRG589797:SRG589865 TBC589797:TBC589865 TKY589797:TKY589865 TUU589797:TUU589865 UEQ589797:UEQ589865 UOM589797:UOM589865 UYI589797:UYI589865 VIE589797:VIE589865 VSA589797:VSA589865 WBW589797:WBW589865 WLS589797:WLS589865 WVO589797:WVO589865 G655333:G655401 JC655333:JC655401 SY655333:SY655401 ACU655333:ACU655401 AMQ655333:AMQ655401 AWM655333:AWM655401 BGI655333:BGI655401 BQE655333:BQE655401 CAA655333:CAA655401 CJW655333:CJW655401 CTS655333:CTS655401 DDO655333:DDO655401 DNK655333:DNK655401 DXG655333:DXG655401 EHC655333:EHC655401 EQY655333:EQY655401 FAU655333:FAU655401 FKQ655333:FKQ655401 FUM655333:FUM655401 GEI655333:GEI655401 GOE655333:GOE655401 GYA655333:GYA655401 HHW655333:HHW655401 HRS655333:HRS655401 IBO655333:IBO655401 ILK655333:ILK655401 IVG655333:IVG655401 JFC655333:JFC655401 JOY655333:JOY655401 JYU655333:JYU655401 KIQ655333:KIQ655401 KSM655333:KSM655401 LCI655333:LCI655401 LME655333:LME655401 LWA655333:LWA655401 MFW655333:MFW655401 MPS655333:MPS655401 MZO655333:MZO655401 NJK655333:NJK655401 NTG655333:NTG655401 ODC655333:ODC655401 OMY655333:OMY655401 OWU655333:OWU655401 PGQ655333:PGQ655401 PQM655333:PQM655401 QAI655333:QAI655401 QKE655333:QKE655401 QUA655333:QUA655401 RDW655333:RDW655401 RNS655333:RNS655401 RXO655333:RXO655401 SHK655333:SHK655401 SRG655333:SRG655401 TBC655333:TBC655401 TKY655333:TKY655401 TUU655333:TUU655401 UEQ655333:UEQ655401 UOM655333:UOM655401 UYI655333:UYI655401 VIE655333:VIE655401 VSA655333:VSA655401 WBW655333:WBW655401 WLS655333:WLS655401 WVO655333:WVO655401 G720869:G720937 JC720869:JC720937 SY720869:SY720937 ACU720869:ACU720937 AMQ720869:AMQ720937 AWM720869:AWM720937 BGI720869:BGI720937 BQE720869:BQE720937 CAA720869:CAA720937 CJW720869:CJW720937 CTS720869:CTS720937 DDO720869:DDO720937 DNK720869:DNK720937 DXG720869:DXG720937 EHC720869:EHC720937 EQY720869:EQY720937 FAU720869:FAU720937 FKQ720869:FKQ720937 FUM720869:FUM720937 GEI720869:GEI720937 GOE720869:GOE720937 GYA720869:GYA720937 HHW720869:HHW720937 HRS720869:HRS720937 IBO720869:IBO720937 ILK720869:ILK720937 IVG720869:IVG720937 JFC720869:JFC720937 JOY720869:JOY720937 JYU720869:JYU720937 KIQ720869:KIQ720937 KSM720869:KSM720937 LCI720869:LCI720937 LME720869:LME720937 LWA720869:LWA720937 MFW720869:MFW720937 MPS720869:MPS720937 MZO720869:MZO720937 NJK720869:NJK720937 NTG720869:NTG720937 ODC720869:ODC720937 OMY720869:OMY720937 OWU720869:OWU720937 PGQ720869:PGQ720937 PQM720869:PQM720937 QAI720869:QAI720937 QKE720869:QKE720937 QUA720869:QUA720937 RDW720869:RDW720937 RNS720869:RNS720937 RXO720869:RXO720937 SHK720869:SHK720937 SRG720869:SRG720937 TBC720869:TBC720937 TKY720869:TKY720937 TUU720869:TUU720937 UEQ720869:UEQ720937 UOM720869:UOM720937 UYI720869:UYI720937 VIE720869:VIE720937 VSA720869:VSA720937 WBW720869:WBW720937 WLS720869:WLS720937 WVO720869:WVO720937 G786405:G786473 JC786405:JC786473 SY786405:SY786473 ACU786405:ACU786473 AMQ786405:AMQ786473 AWM786405:AWM786473 BGI786405:BGI786473 BQE786405:BQE786473 CAA786405:CAA786473 CJW786405:CJW786473 CTS786405:CTS786473 DDO786405:DDO786473 DNK786405:DNK786473 DXG786405:DXG786473 EHC786405:EHC786473 EQY786405:EQY786473 FAU786405:FAU786473 FKQ786405:FKQ786473 FUM786405:FUM786473 GEI786405:GEI786473 GOE786405:GOE786473 GYA786405:GYA786473 HHW786405:HHW786473 HRS786405:HRS786473 IBO786405:IBO786473 ILK786405:ILK786473 IVG786405:IVG786473 JFC786405:JFC786473 JOY786405:JOY786473 JYU786405:JYU786473 KIQ786405:KIQ786473 KSM786405:KSM786473 LCI786405:LCI786473 LME786405:LME786473 LWA786405:LWA786473 MFW786405:MFW786473 MPS786405:MPS786473 MZO786405:MZO786473 NJK786405:NJK786473 NTG786405:NTG786473 ODC786405:ODC786473 OMY786405:OMY786473 OWU786405:OWU786473 PGQ786405:PGQ786473 PQM786405:PQM786473 QAI786405:QAI786473 QKE786405:QKE786473 QUA786405:QUA786473 RDW786405:RDW786473 RNS786405:RNS786473 RXO786405:RXO786473 SHK786405:SHK786473 SRG786405:SRG786473 TBC786405:TBC786473 TKY786405:TKY786473 TUU786405:TUU786473 UEQ786405:UEQ786473 UOM786405:UOM786473 UYI786405:UYI786473 VIE786405:VIE786473 VSA786405:VSA786473 WBW786405:WBW786473 WLS786405:WLS786473 WVO786405:WVO786473 G851941:G852009 JC851941:JC852009 SY851941:SY852009 ACU851941:ACU852009 AMQ851941:AMQ852009 AWM851941:AWM852009 BGI851941:BGI852009 BQE851941:BQE852009 CAA851941:CAA852009 CJW851941:CJW852009 CTS851941:CTS852009 DDO851941:DDO852009 DNK851941:DNK852009 DXG851941:DXG852009 EHC851941:EHC852009 EQY851941:EQY852009 FAU851941:FAU852009 FKQ851941:FKQ852009 FUM851941:FUM852009 GEI851941:GEI852009 GOE851941:GOE852009 GYA851941:GYA852009 HHW851941:HHW852009 HRS851941:HRS852009 IBO851941:IBO852009 ILK851941:ILK852009 IVG851941:IVG852009 JFC851941:JFC852009 JOY851941:JOY852009 JYU851941:JYU852009 KIQ851941:KIQ852009 KSM851941:KSM852009 LCI851941:LCI852009 LME851941:LME852009 LWA851941:LWA852009 MFW851941:MFW852009 MPS851941:MPS852009 MZO851941:MZO852009 NJK851941:NJK852009 NTG851941:NTG852009 ODC851941:ODC852009 OMY851941:OMY852009 OWU851941:OWU852009 PGQ851941:PGQ852009 PQM851941:PQM852009 QAI851941:QAI852009 QKE851941:QKE852009 QUA851941:QUA852009 RDW851941:RDW852009 RNS851941:RNS852009 RXO851941:RXO852009 SHK851941:SHK852009 SRG851941:SRG852009 TBC851941:TBC852009 TKY851941:TKY852009 TUU851941:TUU852009 UEQ851941:UEQ852009 UOM851941:UOM852009 UYI851941:UYI852009 VIE851941:VIE852009 VSA851941:VSA852009 WBW851941:WBW852009 WLS851941:WLS852009 WVO851941:WVO852009 G917477:G917545 JC917477:JC917545 SY917477:SY917545 ACU917477:ACU917545 AMQ917477:AMQ917545 AWM917477:AWM917545 BGI917477:BGI917545 BQE917477:BQE917545 CAA917477:CAA917545 CJW917477:CJW917545 CTS917477:CTS917545 DDO917477:DDO917545 DNK917477:DNK917545 DXG917477:DXG917545 EHC917477:EHC917545 EQY917477:EQY917545 FAU917477:FAU917545 FKQ917477:FKQ917545 FUM917477:FUM917545 GEI917477:GEI917545 GOE917477:GOE917545 GYA917477:GYA917545 HHW917477:HHW917545 HRS917477:HRS917545 IBO917477:IBO917545 ILK917477:ILK917545 IVG917477:IVG917545 JFC917477:JFC917545 JOY917477:JOY917545 JYU917477:JYU917545 KIQ917477:KIQ917545 KSM917477:KSM917545 LCI917477:LCI917545 LME917477:LME917545 LWA917477:LWA917545 MFW917477:MFW917545 MPS917477:MPS917545 MZO917477:MZO917545 NJK917477:NJK917545 NTG917477:NTG917545 ODC917477:ODC917545 OMY917477:OMY917545 OWU917477:OWU917545 PGQ917477:PGQ917545 PQM917477:PQM917545 QAI917477:QAI917545 QKE917477:QKE917545 QUA917477:QUA917545 RDW917477:RDW917545 RNS917477:RNS917545 RXO917477:RXO917545 SHK917477:SHK917545 SRG917477:SRG917545 TBC917477:TBC917545 TKY917477:TKY917545 TUU917477:TUU917545 UEQ917477:UEQ917545 UOM917477:UOM917545 UYI917477:UYI917545 VIE917477:VIE917545 VSA917477:VSA917545 WBW917477:WBW917545 WLS917477:WLS917545 WVO917477:WVO917545 G983013:G983081 JC983013:JC983081 SY983013:SY983081 ACU983013:ACU983081 AMQ983013:AMQ983081 AWM983013:AWM983081 BGI983013:BGI983081 BQE983013:BQE983081 CAA983013:CAA983081 CJW983013:CJW983081 CTS983013:CTS983081 DDO983013:DDO983081 DNK983013:DNK983081 DXG983013:DXG983081 EHC983013:EHC983081 EQY983013:EQY983081 FAU983013:FAU983081 FKQ983013:FKQ983081 FUM983013:FUM983081 GEI983013:GEI983081 GOE983013:GOE983081 GYA983013:GYA983081 HHW983013:HHW983081 HRS983013:HRS983081 IBO983013:IBO983081 ILK983013:ILK983081 IVG983013:IVG983081 JFC983013:JFC983081 JOY983013:JOY983081 JYU983013:JYU983081 KIQ983013:KIQ983081 KSM983013:KSM983081 LCI983013:LCI983081 LME983013:LME983081 LWA983013:LWA983081 MFW983013:MFW983081 MPS983013:MPS983081 MZO983013:MZO983081 NJK983013:NJK983081 NTG983013:NTG983081 ODC983013:ODC983081 OMY983013:OMY983081 OWU983013:OWU983081 PGQ983013:PGQ983081 PQM983013:PQM983081 QAI983013:QAI983081 QKE983013:QKE983081 QUA983013:QUA983081 RDW983013:RDW983081 RNS983013:RNS983081 RXO983013:RXO983081 SHK983013:SHK983081 SRG983013:SRG983081 TBC983013:TBC983081 TKY983013:TKY983081 TUU983013:TUU983081 UEQ983013:UEQ983081 UOM983013:UOM983081 UYI983013:UYI983081 VIE983013:VIE983081 VSA983013:VSA983081 WBW983013:WBW983081 WLS983013:WLS983081 G6:G41 JC6:JC41 SY6:SY41 ACU6:ACU41 AMQ6:AMQ41 AWM6:AWM41 BGI6:BGI41 BQE6:BQE41 CAA6:CAA41 CJW6:CJW41 CTS6:CTS41 DDO6:DDO41 DNK6:DNK41 DXG6:DXG41 EHC6:EHC41 EQY6:EQY41 FAU6:FAU41 FKQ6:FKQ41 FUM6:FUM41 GEI6:GEI41 GOE6:GOE41 GYA6:GYA41 HHW6:HHW41 HRS6:HRS41 IBO6:IBO41 ILK6:ILK41 IVG6:IVG41 JFC6:JFC41 JOY6:JOY41 JYU6:JYU41 KIQ6:KIQ41 KSM6:KSM41 LCI6:LCI41 LME6:LME41 LWA6:LWA41 MFW6:MFW41 MPS6:MPS41 MZO6:MZO41 NJK6:NJK41 NTG6:NTG41 ODC6:ODC41 OMY6:OMY41 OWU6:OWU41 PGQ6:PGQ41 PQM6:PQM41 QAI6:QAI41 QKE6:QKE41 QUA6:QUA41 RDW6:RDW41 RNS6:RNS41 RXO6:RXO41 SHK6:SHK41 SRG6:SRG41 TBC6:TBC41 TKY6:TKY41 TUU6:TUU41 UEQ6:UEQ41 UOM6:UOM41 UYI6:UYI41 VIE6:VIE41 VSA6:VSA41 WBW6:WBW41 WLS6:WLS41 WVO6:WVO41">
       <formula1>"Following,Modified Following,Preceding,Modified Preceding,Month End Reference,Unadjusted Month End,Unadjusted"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F38 JB6:JB38 SX6:SX38 ACT6:ACT38 AMP6:AMP38 AWL6:AWL38 BGH6:BGH38 BQD6:BQD38 BZZ6:BZZ38 CJV6:CJV38 CTR6:CTR38 DDN6:DDN38 DNJ6:DNJ38 DXF6:DXF38 EHB6:EHB38 EQX6:EQX38 FAT6:FAT38 FKP6:FKP38 FUL6:FUL38 GEH6:GEH38 GOD6:GOD38 GXZ6:GXZ38 HHV6:HHV38 HRR6:HRR38 IBN6:IBN38 ILJ6:ILJ38 IVF6:IVF38 JFB6:JFB38 JOX6:JOX38 JYT6:JYT38 KIP6:KIP38 KSL6:KSL38 LCH6:LCH38 LMD6:LMD38 LVZ6:LVZ38 MFV6:MFV38 MPR6:MPR38 MZN6:MZN38 NJJ6:NJJ38 NTF6:NTF38 ODB6:ODB38 OMX6:OMX38 OWT6:OWT38 PGP6:PGP38 PQL6:PQL38 QAH6:QAH38 QKD6:QKD38 QTZ6:QTZ38 RDV6:RDV38 RNR6:RNR38 RXN6:RXN38 SHJ6:SHJ38 SRF6:SRF38 TBB6:TBB38 TKX6:TKX38 TUT6:TUT38 UEP6:UEP38 UOL6:UOL38 UYH6:UYH38 VID6:VID38 VRZ6:VRZ38 WBV6:WBV38 WLR6:WLR38 WVN6:WVN38 F65506:F65574 JB65506:JB65574 SX65506:SX65574 ACT65506:ACT65574 AMP65506:AMP65574 AWL65506:AWL65574 BGH65506:BGH65574 BQD65506:BQD65574 BZZ65506:BZZ65574 CJV65506:CJV65574 CTR65506:CTR65574 DDN65506:DDN65574 DNJ65506:DNJ65574 DXF65506:DXF65574 EHB65506:EHB65574 EQX65506:EQX65574 FAT65506:FAT65574 FKP65506:FKP65574 FUL65506:FUL65574 GEH65506:GEH65574 GOD65506:GOD65574 GXZ65506:GXZ65574 HHV65506:HHV65574 HRR65506:HRR65574 IBN65506:IBN65574 ILJ65506:ILJ65574 IVF65506:IVF65574 JFB65506:JFB65574 JOX65506:JOX65574 JYT65506:JYT65574 KIP65506:KIP65574 KSL65506:KSL65574 LCH65506:LCH65574 LMD65506:LMD65574 LVZ65506:LVZ65574 MFV65506:MFV65574 MPR65506:MPR65574 MZN65506:MZN65574 NJJ65506:NJJ65574 NTF65506:NTF65574 ODB65506:ODB65574 OMX65506:OMX65574 OWT65506:OWT65574 PGP65506:PGP65574 PQL65506:PQL65574 QAH65506:QAH65574 QKD65506:QKD65574 QTZ65506:QTZ65574 RDV65506:RDV65574 RNR65506:RNR65574 RXN65506:RXN65574 SHJ65506:SHJ65574 SRF65506:SRF65574 TBB65506:TBB65574 TKX65506:TKX65574 TUT65506:TUT65574 UEP65506:UEP65574 UOL65506:UOL65574 UYH65506:UYH65574 VID65506:VID65574 VRZ65506:VRZ65574 WBV65506:WBV65574 WLR65506:WLR65574 WVN65506:WVN65574 F131042:F131110 JB131042:JB131110 SX131042:SX131110 ACT131042:ACT131110 AMP131042:AMP131110 AWL131042:AWL131110 BGH131042:BGH131110 BQD131042:BQD131110 BZZ131042:BZZ131110 CJV131042:CJV131110 CTR131042:CTR131110 DDN131042:DDN131110 DNJ131042:DNJ131110 DXF131042:DXF131110 EHB131042:EHB131110 EQX131042:EQX131110 FAT131042:FAT131110 FKP131042:FKP131110 FUL131042:FUL131110 GEH131042:GEH131110 GOD131042:GOD131110 GXZ131042:GXZ131110 HHV131042:HHV131110 HRR131042:HRR131110 IBN131042:IBN131110 ILJ131042:ILJ131110 IVF131042:IVF131110 JFB131042:JFB131110 JOX131042:JOX131110 JYT131042:JYT131110 KIP131042:KIP131110 KSL131042:KSL131110 LCH131042:LCH131110 LMD131042:LMD131110 LVZ131042:LVZ131110 MFV131042:MFV131110 MPR131042:MPR131110 MZN131042:MZN131110 NJJ131042:NJJ131110 NTF131042:NTF131110 ODB131042:ODB131110 OMX131042:OMX131110 OWT131042:OWT131110 PGP131042:PGP131110 PQL131042:PQL131110 QAH131042:QAH131110 QKD131042:QKD131110 QTZ131042:QTZ131110 RDV131042:RDV131110 RNR131042:RNR131110 RXN131042:RXN131110 SHJ131042:SHJ131110 SRF131042:SRF131110 TBB131042:TBB131110 TKX131042:TKX131110 TUT131042:TUT131110 UEP131042:UEP131110 UOL131042:UOL131110 UYH131042:UYH131110 VID131042:VID131110 VRZ131042:VRZ131110 WBV131042:WBV131110 WLR131042:WLR131110 WVN131042:WVN131110 F196578:F196646 JB196578:JB196646 SX196578:SX196646 ACT196578:ACT196646 AMP196578:AMP196646 AWL196578:AWL196646 BGH196578:BGH196646 BQD196578:BQD196646 BZZ196578:BZZ196646 CJV196578:CJV196646 CTR196578:CTR196646 DDN196578:DDN196646 DNJ196578:DNJ196646 DXF196578:DXF196646 EHB196578:EHB196646 EQX196578:EQX196646 FAT196578:FAT196646 FKP196578:FKP196646 FUL196578:FUL196646 GEH196578:GEH196646 GOD196578:GOD196646 GXZ196578:GXZ196646 HHV196578:HHV196646 HRR196578:HRR196646 IBN196578:IBN196646 ILJ196578:ILJ196646 IVF196578:IVF196646 JFB196578:JFB196646 JOX196578:JOX196646 JYT196578:JYT196646 KIP196578:KIP196646 KSL196578:KSL196646 LCH196578:LCH196646 LMD196578:LMD196646 LVZ196578:LVZ196646 MFV196578:MFV196646 MPR196578:MPR196646 MZN196578:MZN196646 NJJ196578:NJJ196646 NTF196578:NTF196646 ODB196578:ODB196646 OMX196578:OMX196646 OWT196578:OWT196646 PGP196578:PGP196646 PQL196578:PQL196646 QAH196578:QAH196646 QKD196578:QKD196646 QTZ196578:QTZ196646 RDV196578:RDV196646 RNR196578:RNR196646 RXN196578:RXN196646 SHJ196578:SHJ196646 SRF196578:SRF196646 TBB196578:TBB196646 TKX196578:TKX196646 TUT196578:TUT196646 UEP196578:UEP196646 UOL196578:UOL196646 UYH196578:UYH196646 VID196578:VID196646 VRZ196578:VRZ196646 WBV196578:WBV196646 WLR196578:WLR196646 WVN196578:WVN196646 F262114:F262182 JB262114:JB262182 SX262114:SX262182 ACT262114:ACT262182 AMP262114:AMP262182 AWL262114:AWL262182 BGH262114:BGH262182 BQD262114:BQD262182 BZZ262114:BZZ262182 CJV262114:CJV262182 CTR262114:CTR262182 DDN262114:DDN262182 DNJ262114:DNJ262182 DXF262114:DXF262182 EHB262114:EHB262182 EQX262114:EQX262182 FAT262114:FAT262182 FKP262114:FKP262182 FUL262114:FUL262182 GEH262114:GEH262182 GOD262114:GOD262182 GXZ262114:GXZ262182 HHV262114:HHV262182 HRR262114:HRR262182 IBN262114:IBN262182 ILJ262114:ILJ262182 IVF262114:IVF262182 JFB262114:JFB262182 JOX262114:JOX262182 JYT262114:JYT262182 KIP262114:KIP262182 KSL262114:KSL262182 LCH262114:LCH262182 LMD262114:LMD262182 LVZ262114:LVZ262182 MFV262114:MFV262182 MPR262114:MPR262182 MZN262114:MZN262182 NJJ262114:NJJ262182 NTF262114:NTF262182 ODB262114:ODB262182 OMX262114:OMX262182 OWT262114:OWT262182 PGP262114:PGP262182 PQL262114:PQL262182 QAH262114:QAH262182 QKD262114:QKD262182 QTZ262114:QTZ262182 RDV262114:RDV262182 RNR262114:RNR262182 RXN262114:RXN262182 SHJ262114:SHJ262182 SRF262114:SRF262182 TBB262114:TBB262182 TKX262114:TKX262182 TUT262114:TUT262182 UEP262114:UEP262182 UOL262114:UOL262182 UYH262114:UYH262182 VID262114:VID262182 VRZ262114:VRZ262182 WBV262114:WBV262182 WLR262114:WLR262182 WVN262114:WVN262182 F327650:F327718 JB327650:JB327718 SX327650:SX327718 ACT327650:ACT327718 AMP327650:AMP327718 AWL327650:AWL327718 BGH327650:BGH327718 BQD327650:BQD327718 BZZ327650:BZZ327718 CJV327650:CJV327718 CTR327650:CTR327718 DDN327650:DDN327718 DNJ327650:DNJ327718 DXF327650:DXF327718 EHB327650:EHB327718 EQX327650:EQX327718 FAT327650:FAT327718 FKP327650:FKP327718 FUL327650:FUL327718 GEH327650:GEH327718 GOD327650:GOD327718 GXZ327650:GXZ327718 HHV327650:HHV327718 HRR327650:HRR327718 IBN327650:IBN327718 ILJ327650:ILJ327718 IVF327650:IVF327718 JFB327650:JFB327718 JOX327650:JOX327718 JYT327650:JYT327718 KIP327650:KIP327718 KSL327650:KSL327718 LCH327650:LCH327718 LMD327650:LMD327718 LVZ327650:LVZ327718 MFV327650:MFV327718 MPR327650:MPR327718 MZN327650:MZN327718 NJJ327650:NJJ327718 NTF327650:NTF327718 ODB327650:ODB327718 OMX327650:OMX327718 OWT327650:OWT327718 PGP327650:PGP327718 PQL327650:PQL327718 QAH327650:QAH327718 QKD327650:QKD327718 QTZ327650:QTZ327718 RDV327650:RDV327718 RNR327650:RNR327718 RXN327650:RXN327718 SHJ327650:SHJ327718 SRF327650:SRF327718 TBB327650:TBB327718 TKX327650:TKX327718 TUT327650:TUT327718 UEP327650:UEP327718 UOL327650:UOL327718 UYH327650:UYH327718 VID327650:VID327718 VRZ327650:VRZ327718 WBV327650:WBV327718 WLR327650:WLR327718 WVN327650:WVN327718 F393186:F393254 JB393186:JB393254 SX393186:SX393254 ACT393186:ACT393254 AMP393186:AMP393254 AWL393186:AWL393254 BGH393186:BGH393254 BQD393186:BQD393254 BZZ393186:BZZ393254 CJV393186:CJV393254 CTR393186:CTR393254 DDN393186:DDN393254 DNJ393186:DNJ393254 DXF393186:DXF393254 EHB393186:EHB393254 EQX393186:EQX393254 FAT393186:FAT393254 FKP393186:FKP393254 FUL393186:FUL393254 GEH393186:GEH393254 GOD393186:GOD393254 GXZ393186:GXZ393254 HHV393186:HHV393254 HRR393186:HRR393254 IBN393186:IBN393254 ILJ393186:ILJ393254 IVF393186:IVF393254 JFB393186:JFB393254 JOX393186:JOX393254 JYT393186:JYT393254 KIP393186:KIP393254 KSL393186:KSL393254 LCH393186:LCH393254 LMD393186:LMD393254 LVZ393186:LVZ393254 MFV393186:MFV393254 MPR393186:MPR393254 MZN393186:MZN393254 NJJ393186:NJJ393254 NTF393186:NTF393254 ODB393186:ODB393254 OMX393186:OMX393254 OWT393186:OWT393254 PGP393186:PGP393254 PQL393186:PQL393254 QAH393186:QAH393254 QKD393186:QKD393254 QTZ393186:QTZ393254 RDV393186:RDV393254 RNR393186:RNR393254 RXN393186:RXN393254 SHJ393186:SHJ393254 SRF393186:SRF393254 TBB393186:TBB393254 TKX393186:TKX393254 TUT393186:TUT393254 UEP393186:UEP393254 UOL393186:UOL393254 UYH393186:UYH393254 VID393186:VID393254 VRZ393186:VRZ393254 WBV393186:WBV393254 WLR393186:WLR393254 WVN393186:WVN393254 F458722:F458790 JB458722:JB458790 SX458722:SX458790 ACT458722:ACT458790 AMP458722:AMP458790 AWL458722:AWL458790 BGH458722:BGH458790 BQD458722:BQD458790 BZZ458722:BZZ458790 CJV458722:CJV458790 CTR458722:CTR458790 DDN458722:DDN458790 DNJ458722:DNJ458790 DXF458722:DXF458790 EHB458722:EHB458790 EQX458722:EQX458790 FAT458722:FAT458790 FKP458722:FKP458790 FUL458722:FUL458790 GEH458722:GEH458790 GOD458722:GOD458790 GXZ458722:GXZ458790 HHV458722:HHV458790 HRR458722:HRR458790 IBN458722:IBN458790 ILJ458722:ILJ458790 IVF458722:IVF458790 JFB458722:JFB458790 JOX458722:JOX458790 JYT458722:JYT458790 KIP458722:KIP458790 KSL458722:KSL458790 LCH458722:LCH458790 LMD458722:LMD458790 LVZ458722:LVZ458790 MFV458722:MFV458790 MPR458722:MPR458790 MZN458722:MZN458790 NJJ458722:NJJ458790 NTF458722:NTF458790 ODB458722:ODB458790 OMX458722:OMX458790 OWT458722:OWT458790 PGP458722:PGP458790 PQL458722:PQL458790 QAH458722:QAH458790 QKD458722:QKD458790 QTZ458722:QTZ458790 RDV458722:RDV458790 RNR458722:RNR458790 RXN458722:RXN458790 SHJ458722:SHJ458790 SRF458722:SRF458790 TBB458722:TBB458790 TKX458722:TKX458790 TUT458722:TUT458790 UEP458722:UEP458790 UOL458722:UOL458790 UYH458722:UYH458790 VID458722:VID458790 VRZ458722:VRZ458790 WBV458722:WBV458790 WLR458722:WLR458790 WVN458722:WVN458790 F524258:F524326 JB524258:JB524326 SX524258:SX524326 ACT524258:ACT524326 AMP524258:AMP524326 AWL524258:AWL524326 BGH524258:BGH524326 BQD524258:BQD524326 BZZ524258:BZZ524326 CJV524258:CJV524326 CTR524258:CTR524326 DDN524258:DDN524326 DNJ524258:DNJ524326 DXF524258:DXF524326 EHB524258:EHB524326 EQX524258:EQX524326 FAT524258:FAT524326 FKP524258:FKP524326 FUL524258:FUL524326 GEH524258:GEH524326 GOD524258:GOD524326 GXZ524258:GXZ524326 HHV524258:HHV524326 HRR524258:HRR524326 IBN524258:IBN524326 ILJ524258:ILJ524326 IVF524258:IVF524326 JFB524258:JFB524326 JOX524258:JOX524326 JYT524258:JYT524326 KIP524258:KIP524326 KSL524258:KSL524326 LCH524258:LCH524326 LMD524258:LMD524326 LVZ524258:LVZ524326 MFV524258:MFV524326 MPR524258:MPR524326 MZN524258:MZN524326 NJJ524258:NJJ524326 NTF524258:NTF524326 ODB524258:ODB524326 OMX524258:OMX524326 OWT524258:OWT524326 PGP524258:PGP524326 PQL524258:PQL524326 QAH524258:QAH524326 QKD524258:QKD524326 QTZ524258:QTZ524326 RDV524258:RDV524326 RNR524258:RNR524326 RXN524258:RXN524326 SHJ524258:SHJ524326 SRF524258:SRF524326 TBB524258:TBB524326 TKX524258:TKX524326 TUT524258:TUT524326 UEP524258:UEP524326 UOL524258:UOL524326 UYH524258:UYH524326 VID524258:VID524326 VRZ524258:VRZ524326 WBV524258:WBV524326 WLR524258:WLR524326 WVN524258:WVN524326 F589794:F589862 JB589794:JB589862 SX589794:SX589862 ACT589794:ACT589862 AMP589794:AMP589862 AWL589794:AWL589862 BGH589794:BGH589862 BQD589794:BQD589862 BZZ589794:BZZ589862 CJV589794:CJV589862 CTR589794:CTR589862 DDN589794:DDN589862 DNJ589794:DNJ589862 DXF589794:DXF589862 EHB589794:EHB589862 EQX589794:EQX589862 FAT589794:FAT589862 FKP589794:FKP589862 FUL589794:FUL589862 GEH589794:GEH589862 GOD589794:GOD589862 GXZ589794:GXZ589862 HHV589794:HHV589862 HRR589794:HRR589862 IBN589794:IBN589862 ILJ589794:ILJ589862 IVF589794:IVF589862 JFB589794:JFB589862 JOX589794:JOX589862 JYT589794:JYT589862 KIP589794:KIP589862 KSL589794:KSL589862 LCH589794:LCH589862 LMD589794:LMD589862 LVZ589794:LVZ589862 MFV589794:MFV589862 MPR589794:MPR589862 MZN589794:MZN589862 NJJ589794:NJJ589862 NTF589794:NTF589862 ODB589794:ODB589862 OMX589794:OMX589862 OWT589794:OWT589862 PGP589794:PGP589862 PQL589794:PQL589862 QAH589794:QAH589862 QKD589794:QKD589862 QTZ589794:QTZ589862 RDV589794:RDV589862 RNR589794:RNR589862 RXN589794:RXN589862 SHJ589794:SHJ589862 SRF589794:SRF589862 TBB589794:TBB589862 TKX589794:TKX589862 TUT589794:TUT589862 UEP589794:UEP589862 UOL589794:UOL589862 UYH589794:UYH589862 VID589794:VID589862 VRZ589794:VRZ589862 WBV589794:WBV589862 WLR589794:WLR589862 WVN589794:WVN589862 F655330:F655398 JB655330:JB655398 SX655330:SX655398 ACT655330:ACT655398 AMP655330:AMP655398 AWL655330:AWL655398 BGH655330:BGH655398 BQD655330:BQD655398 BZZ655330:BZZ655398 CJV655330:CJV655398 CTR655330:CTR655398 DDN655330:DDN655398 DNJ655330:DNJ655398 DXF655330:DXF655398 EHB655330:EHB655398 EQX655330:EQX655398 FAT655330:FAT655398 FKP655330:FKP655398 FUL655330:FUL655398 GEH655330:GEH655398 GOD655330:GOD655398 GXZ655330:GXZ655398 HHV655330:HHV655398 HRR655330:HRR655398 IBN655330:IBN655398 ILJ655330:ILJ655398 IVF655330:IVF655398 JFB655330:JFB655398 JOX655330:JOX655398 JYT655330:JYT655398 KIP655330:KIP655398 KSL655330:KSL655398 LCH655330:LCH655398 LMD655330:LMD655398 LVZ655330:LVZ655398 MFV655330:MFV655398 MPR655330:MPR655398 MZN655330:MZN655398 NJJ655330:NJJ655398 NTF655330:NTF655398 ODB655330:ODB655398 OMX655330:OMX655398 OWT655330:OWT655398 PGP655330:PGP655398 PQL655330:PQL655398 QAH655330:QAH655398 QKD655330:QKD655398 QTZ655330:QTZ655398 RDV655330:RDV655398 RNR655330:RNR655398 RXN655330:RXN655398 SHJ655330:SHJ655398 SRF655330:SRF655398 TBB655330:TBB655398 TKX655330:TKX655398 TUT655330:TUT655398 UEP655330:UEP655398 UOL655330:UOL655398 UYH655330:UYH655398 VID655330:VID655398 VRZ655330:VRZ655398 WBV655330:WBV655398 WLR655330:WLR655398 WVN655330:WVN655398 F720866:F720934 JB720866:JB720934 SX720866:SX720934 ACT720866:ACT720934 AMP720866:AMP720934 AWL720866:AWL720934 BGH720866:BGH720934 BQD720866:BQD720934 BZZ720866:BZZ720934 CJV720866:CJV720934 CTR720866:CTR720934 DDN720866:DDN720934 DNJ720866:DNJ720934 DXF720866:DXF720934 EHB720866:EHB720934 EQX720866:EQX720934 FAT720866:FAT720934 FKP720866:FKP720934 FUL720866:FUL720934 GEH720866:GEH720934 GOD720866:GOD720934 GXZ720866:GXZ720934 HHV720866:HHV720934 HRR720866:HRR720934 IBN720866:IBN720934 ILJ720866:ILJ720934 IVF720866:IVF720934 JFB720866:JFB720934 JOX720866:JOX720934 JYT720866:JYT720934 KIP720866:KIP720934 KSL720866:KSL720934 LCH720866:LCH720934 LMD720866:LMD720934 LVZ720866:LVZ720934 MFV720866:MFV720934 MPR720866:MPR720934 MZN720866:MZN720934 NJJ720866:NJJ720934 NTF720866:NTF720934 ODB720866:ODB720934 OMX720866:OMX720934 OWT720866:OWT720934 PGP720866:PGP720934 PQL720866:PQL720934 QAH720866:QAH720934 QKD720866:QKD720934 QTZ720866:QTZ720934 RDV720866:RDV720934 RNR720866:RNR720934 RXN720866:RXN720934 SHJ720866:SHJ720934 SRF720866:SRF720934 TBB720866:TBB720934 TKX720866:TKX720934 TUT720866:TUT720934 UEP720866:UEP720934 UOL720866:UOL720934 UYH720866:UYH720934 VID720866:VID720934 VRZ720866:VRZ720934 WBV720866:WBV720934 WLR720866:WLR720934 WVN720866:WVN720934 F786402:F786470 JB786402:JB786470 SX786402:SX786470 ACT786402:ACT786470 AMP786402:AMP786470 AWL786402:AWL786470 BGH786402:BGH786470 BQD786402:BQD786470 BZZ786402:BZZ786470 CJV786402:CJV786470 CTR786402:CTR786470 DDN786402:DDN786470 DNJ786402:DNJ786470 DXF786402:DXF786470 EHB786402:EHB786470 EQX786402:EQX786470 FAT786402:FAT786470 FKP786402:FKP786470 FUL786402:FUL786470 GEH786402:GEH786470 GOD786402:GOD786470 GXZ786402:GXZ786470 HHV786402:HHV786470 HRR786402:HRR786470 IBN786402:IBN786470 ILJ786402:ILJ786470 IVF786402:IVF786470 JFB786402:JFB786470 JOX786402:JOX786470 JYT786402:JYT786470 KIP786402:KIP786470 KSL786402:KSL786470 LCH786402:LCH786470 LMD786402:LMD786470 LVZ786402:LVZ786470 MFV786402:MFV786470 MPR786402:MPR786470 MZN786402:MZN786470 NJJ786402:NJJ786470 NTF786402:NTF786470 ODB786402:ODB786470 OMX786402:OMX786470 OWT786402:OWT786470 PGP786402:PGP786470 PQL786402:PQL786470 QAH786402:QAH786470 QKD786402:QKD786470 QTZ786402:QTZ786470 RDV786402:RDV786470 RNR786402:RNR786470 RXN786402:RXN786470 SHJ786402:SHJ786470 SRF786402:SRF786470 TBB786402:TBB786470 TKX786402:TKX786470 TUT786402:TUT786470 UEP786402:UEP786470 UOL786402:UOL786470 UYH786402:UYH786470 VID786402:VID786470 VRZ786402:VRZ786470 WBV786402:WBV786470 WLR786402:WLR786470 WVN786402:WVN786470 F851938:F852006 JB851938:JB852006 SX851938:SX852006 ACT851938:ACT852006 AMP851938:AMP852006 AWL851938:AWL852006 BGH851938:BGH852006 BQD851938:BQD852006 BZZ851938:BZZ852006 CJV851938:CJV852006 CTR851938:CTR852006 DDN851938:DDN852006 DNJ851938:DNJ852006 DXF851938:DXF852006 EHB851938:EHB852006 EQX851938:EQX852006 FAT851938:FAT852006 FKP851938:FKP852006 FUL851938:FUL852006 GEH851938:GEH852006 GOD851938:GOD852006 GXZ851938:GXZ852006 HHV851938:HHV852006 HRR851938:HRR852006 IBN851938:IBN852006 ILJ851938:ILJ852006 IVF851938:IVF852006 JFB851938:JFB852006 JOX851938:JOX852006 JYT851938:JYT852006 KIP851938:KIP852006 KSL851938:KSL852006 LCH851938:LCH852006 LMD851938:LMD852006 LVZ851938:LVZ852006 MFV851938:MFV852006 MPR851938:MPR852006 MZN851938:MZN852006 NJJ851938:NJJ852006 NTF851938:NTF852006 ODB851938:ODB852006 OMX851938:OMX852006 OWT851938:OWT852006 PGP851938:PGP852006 PQL851938:PQL852006 QAH851938:QAH852006 QKD851938:QKD852006 QTZ851938:QTZ852006 RDV851938:RDV852006 RNR851938:RNR852006 RXN851938:RXN852006 SHJ851938:SHJ852006 SRF851938:SRF852006 TBB851938:TBB852006 TKX851938:TKX852006 TUT851938:TUT852006 UEP851938:UEP852006 UOL851938:UOL852006 UYH851938:UYH852006 VID851938:VID852006 VRZ851938:VRZ852006 WBV851938:WBV852006 WLR851938:WLR852006 WVN851938:WVN852006 F917474:F917542 JB917474:JB917542 SX917474:SX917542 ACT917474:ACT917542 AMP917474:AMP917542 AWL917474:AWL917542 BGH917474:BGH917542 BQD917474:BQD917542 BZZ917474:BZZ917542 CJV917474:CJV917542 CTR917474:CTR917542 DDN917474:DDN917542 DNJ917474:DNJ917542 DXF917474:DXF917542 EHB917474:EHB917542 EQX917474:EQX917542 FAT917474:FAT917542 FKP917474:FKP917542 FUL917474:FUL917542 GEH917474:GEH917542 GOD917474:GOD917542 GXZ917474:GXZ917542 HHV917474:HHV917542 HRR917474:HRR917542 IBN917474:IBN917542 ILJ917474:ILJ917542 IVF917474:IVF917542 JFB917474:JFB917542 JOX917474:JOX917542 JYT917474:JYT917542 KIP917474:KIP917542 KSL917474:KSL917542 LCH917474:LCH917542 LMD917474:LMD917542 LVZ917474:LVZ917542 MFV917474:MFV917542 MPR917474:MPR917542 MZN917474:MZN917542 NJJ917474:NJJ917542 NTF917474:NTF917542 ODB917474:ODB917542 OMX917474:OMX917542 OWT917474:OWT917542 PGP917474:PGP917542 PQL917474:PQL917542 QAH917474:QAH917542 QKD917474:QKD917542 QTZ917474:QTZ917542 RDV917474:RDV917542 RNR917474:RNR917542 RXN917474:RXN917542 SHJ917474:SHJ917542 SRF917474:SRF917542 TBB917474:TBB917542 TKX917474:TKX917542 TUT917474:TUT917542 UEP917474:UEP917542 UOL917474:UOL917542 UYH917474:UYH917542 VID917474:VID917542 VRZ917474:VRZ917542 WBV917474:WBV917542 WLR917474:WLR917542 WVN917474:WVN917542 F983010:F983078 JB983010:JB983078 SX983010:SX983078 ACT983010:ACT983078 AMP983010:AMP983078 AWL983010:AWL983078 BGH983010:BGH983078 BQD983010:BQD983078 BZZ983010:BZZ983078 CJV983010:CJV983078 CTR983010:CTR983078 DDN983010:DDN983078 DNJ983010:DNJ983078 DXF983010:DXF983078 EHB983010:EHB983078 EQX983010:EQX983078 FAT983010:FAT983078 FKP983010:FKP983078 FUL983010:FUL983078 GEH983010:GEH983078 GOD983010:GOD983078 GXZ983010:GXZ983078 HHV983010:HHV983078 HRR983010:HRR983078 IBN983010:IBN983078 ILJ983010:ILJ983078 IVF983010:IVF983078 JFB983010:JFB983078 JOX983010:JOX983078 JYT983010:JYT983078 KIP983010:KIP983078 KSL983010:KSL983078 LCH983010:LCH983078 LMD983010:LMD983078 LVZ983010:LVZ983078 MFV983010:MFV983078 MPR983010:MPR983078 MZN983010:MZN983078 NJJ983010:NJJ983078 NTF983010:NTF983078 ODB983010:ODB983078 OMX983010:OMX983078 OWT983010:OWT983078 PGP983010:PGP983078 PQL983010:PQL983078 QAH983010:QAH983078 QKD983010:QKD983078 QTZ983010:QTZ983078 RDV983010:RDV983078 RNR983010:RNR983078 RXN983010:RXN983078 SHJ983010:SHJ983078 SRF983010:SRF983078 TBB983010:TBB983078 TKX983010:TKX983078 TUT983010:TUT983078 UEP983010:UEP983078 UOL983010:UOL983078 UYH983010:UYH983078 VID983010:VID983078 VRZ983010:VRZ983078 WBV983010:WBV983078 WLR983010:WLR983078 WVN983010:WVN983078">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVN983013:WVN983081 F65509:F65577 JB65509:JB65577 SX65509:SX65577 ACT65509:ACT65577 AMP65509:AMP65577 AWL65509:AWL65577 BGH65509:BGH65577 BQD65509:BQD65577 BZZ65509:BZZ65577 CJV65509:CJV65577 CTR65509:CTR65577 DDN65509:DDN65577 DNJ65509:DNJ65577 DXF65509:DXF65577 EHB65509:EHB65577 EQX65509:EQX65577 FAT65509:FAT65577 FKP65509:FKP65577 FUL65509:FUL65577 GEH65509:GEH65577 GOD65509:GOD65577 GXZ65509:GXZ65577 HHV65509:HHV65577 HRR65509:HRR65577 IBN65509:IBN65577 ILJ65509:ILJ65577 IVF65509:IVF65577 JFB65509:JFB65577 JOX65509:JOX65577 JYT65509:JYT65577 KIP65509:KIP65577 KSL65509:KSL65577 LCH65509:LCH65577 LMD65509:LMD65577 LVZ65509:LVZ65577 MFV65509:MFV65577 MPR65509:MPR65577 MZN65509:MZN65577 NJJ65509:NJJ65577 NTF65509:NTF65577 ODB65509:ODB65577 OMX65509:OMX65577 OWT65509:OWT65577 PGP65509:PGP65577 PQL65509:PQL65577 QAH65509:QAH65577 QKD65509:QKD65577 QTZ65509:QTZ65577 RDV65509:RDV65577 RNR65509:RNR65577 RXN65509:RXN65577 SHJ65509:SHJ65577 SRF65509:SRF65577 TBB65509:TBB65577 TKX65509:TKX65577 TUT65509:TUT65577 UEP65509:UEP65577 UOL65509:UOL65577 UYH65509:UYH65577 VID65509:VID65577 VRZ65509:VRZ65577 WBV65509:WBV65577 WLR65509:WLR65577 WVN65509:WVN65577 F131045:F131113 JB131045:JB131113 SX131045:SX131113 ACT131045:ACT131113 AMP131045:AMP131113 AWL131045:AWL131113 BGH131045:BGH131113 BQD131045:BQD131113 BZZ131045:BZZ131113 CJV131045:CJV131113 CTR131045:CTR131113 DDN131045:DDN131113 DNJ131045:DNJ131113 DXF131045:DXF131113 EHB131045:EHB131113 EQX131045:EQX131113 FAT131045:FAT131113 FKP131045:FKP131113 FUL131045:FUL131113 GEH131045:GEH131113 GOD131045:GOD131113 GXZ131045:GXZ131113 HHV131045:HHV131113 HRR131045:HRR131113 IBN131045:IBN131113 ILJ131045:ILJ131113 IVF131045:IVF131113 JFB131045:JFB131113 JOX131045:JOX131113 JYT131045:JYT131113 KIP131045:KIP131113 KSL131045:KSL131113 LCH131045:LCH131113 LMD131045:LMD131113 LVZ131045:LVZ131113 MFV131045:MFV131113 MPR131045:MPR131113 MZN131045:MZN131113 NJJ131045:NJJ131113 NTF131045:NTF131113 ODB131045:ODB131113 OMX131045:OMX131113 OWT131045:OWT131113 PGP131045:PGP131113 PQL131045:PQL131113 QAH131045:QAH131113 QKD131045:QKD131113 QTZ131045:QTZ131113 RDV131045:RDV131113 RNR131045:RNR131113 RXN131045:RXN131113 SHJ131045:SHJ131113 SRF131045:SRF131113 TBB131045:TBB131113 TKX131045:TKX131113 TUT131045:TUT131113 UEP131045:UEP131113 UOL131045:UOL131113 UYH131045:UYH131113 VID131045:VID131113 VRZ131045:VRZ131113 WBV131045:WBV131113 WLR131045:WLR131113 WVN131045:WVN131113 F196581:F196649 JB196581:JB196649 SX196581:SX196649 ACT196581:ACT196649 AMP196581:AMP196649 AWL196581:AWL196649 BGH196581:BGH196649 BQD196581:BQD196649 BZZ196581:BZZ196649 CJV196581:CJV196649 CTR196581:CTR196649 DDN196581:DDN196649 DNJ196581:DNJ196649 DXF196581:DXF196649 EHB196581:EHB196649 EQX196581:EQX196649 FAT196581:FAT196649 FKP196581:FKP196649 FUL196581:FUL196649 GEH196581:GEH196649 GOD196581:GOD196649 GXZ196581:GXZ196649 HHV196581:HHV196649 HRR196581:HRR196649 IBN196581:IBN196649 ILJ196581:ILJ196649 IVF196581:IVF196649 JFB196581:JFB196649 JOX196581:JOX196649 JYT196581:JYT196649 KIP196581:KIP196649 KSL196581:KSL196649 LCH196581:LCH196649 LMD196581:LMD196649 LVZ196581:LVZ196649 MFV196581:MFV196649 MPR196581:MPR196649 MZN196581:MZN196649 NJJ196581:NJJ196649 NTF196581:NTF196649 ODB196581:ODB196649 OMX196581:OMX196649 OWT196581:OWT196649 PGP196581:PGP196649 PQL196581:PQL196649 QAH196581:QAH196649 QKD196581:QKD196649 QTZ196581:QTZ196649 RDV196581:RDV196649 RNR196581:RNR196649 RXN196581:RXN196649 SHJ196581:SHJ196649 SRF196581:SRF196649 TBB196581:TBB196649 TKX196581:TKX196649 TUT196581:TUT196649 UEP196581:UEP196649 UOL196581:UOL196649 UYH196581:UYH196649 VID196581:VID196649 VRZ196581:VRZ196649 WBV196581:WBV196649 WLR196581:WLR196649 WVN196581:WVN196649 F262117:F262185 JB262117:JB262185 SX262117:SX262185 ACT262117:ACT262185 AMP262117:AMP262185 AWL262117:AWL262185 BGH262117:BGH262185 BQD262117:BQD262185 BZZ262117:BZZ262185 CJV262117:CJV262185 CTR262117:CTR262185 DDN262117:DDN262185 DNJ262117:DNJ262185 DXF262117:DXF262185 EHB262117:EHB262185 EQX262117:EQX262185 FAT262117:FAT262185 FKP262117:FKP262185 FUL262117:FUL262185 GEH262117:GEH262185 GOD262117:GOD262185 GXZ262117:GXZ262185 HHV262117:HHV262185 HRR262117:HRR262185 IBN262117:IBN262185 ILJ262117:ILJ262185 IVF262117:IVF262185 JFB262117:JFB262185 JOX262117:JOX262185 JYT262117:JYT262185 KIP262117:KIP262185 KSL262117:KSL262185 LCH262117:LCH262185 LMD262117:LMD262185 LVZ262117:LVZ262185 MFV262117:MFV262185 MPR262117:MPR262185 MZN262117:MZN262185 NJJ262117:NJJ262185 NTF262117:NTF262185 ODB262117:ODB262185 OMX262117:OMX262185 OWT262117:OWT262185 PGP262117:PGP262185 PQL262117:PQL262185 QAH262117:QAH262185 QKD262117:QKD262185 QTZ262117:QTZ262185 RDV262117:RDV262185 RNR262117:RNR262185 RXN262117:RXN262185 SHJ262117:SHJ262185 SRF262117:SRF262185 TBB262117:TBB262185 TKX262117:TKX262185 TUT262117:TUT262185 UEP262117:UEP262185 UOL262117:UOL262185 UYH262117:UYH262185 VID262117:VID262185 VRZ262117:VRZ262185 WBV262117:WBV262185 WLR262117:WLR262185 WVN262117:WVN262185 F327653:F327721 JB327653:JB327721 SX327653:SX327721 ACT327653:ACT327721 AMP327653:AMP327721 AWL327653:AWL327721 BGH327653:BGH327721 BQD327653:BQD327721 BZZ327653:BZZ327721 CJV327653:CJV327721 CTR327653:CTR327721 DDN327653:DDN327721 DNJ327653:DNJ327721 DXF327653:DXF327721 EHB327653:EHB327721 EQX327653:EQX327721 FAT327653:FAT327721 FKP327653:FKP327721 FUL327653:FUL327721 GEH327653:GEH327721 GOD327653:GOD327721 GXZ327653:GXZ327721 HHV327653:HHV327721 HRR327653:HRR327721 IBN327653:IBN327721 ILJ327653:ILJ327721 IVF327653:IVF327721 JFB327653:JFB327721 JOX327653:JOX327721 JYT327653:JYT327721 KIP327653:KIP327721 KSL327653:KSL327721 LCH327653:LCH327721 LMD327653:LMD327721 LVZ327653:LVZ327721 MFV327653:MFV327721 MPR327653:MPR327721 MZN327653:MZN327721 NJJ327653:NJJ327721 NTF327653:NTF327721 ODB327653:ODB327721 OMX327653:OMX327721 OWT327653:OWT327721 PGP327653:PGP327721 PQL327653:PQL327721 QAH327653:QAH327721 QKD327653:QKD327721 QTZ327653:QTZ327721 RDV327653:RDV327721 RNR327653:RNR327721 RXN327653:RXN327721 SHJ327653:SHJ327721 SRF327653:SRF327721 TBB327653:TBB327721 TKX327653:TKX327721 TUT327653:TUT327721 UEP327653:UEP327721 UOL327653:UOL327721 UYH327653:UYH327721 VID327653:VID327721 VRZ327653:VRZ327721 WBV327653:WBV327721 WLR327653:WLR327721 WVN327653:WVN327721 F393189:F393257 JB393189:JB393257 SX393189:SX393257 ACT393189:ACT393257 AMP393189:AMP393257 AWL393189:AWL393257 BGH393189:BGH393257 BQD393189:BQD393257 BZZ393189:BZZ393257 CJV393189:CJV393257 CTR393189:CTR393257 DDN393189:DDN393257 DNJ393189:DNJ393257 DXF393189:DXF393257 EHB393189:EHB393257 EQX393189:EQX393257 FAT393189:FAT393257 FKP393189:FKP393257 FUL393189:FUL393257 GEH393189:GEH393257 GOD393189:GOD393257 GXZ393189:GXZ393257 HHV393189:HHV393257 HRR393189:HRR393257 IBN393189:IBN393257 ILJ393189:ILJ393257 IVF393189:IVF393257 JFB393189:JFB393257 JOX393189:JOX393257 JYT393189:JYT393257 KIP393189:KIP393257 KSL393189:KSL393257 LCH393189:LCH393257 LMD393189:LMD393257 LVZ393189:LVZ393257 MFV393189:MFV393257 MPR393189:MPR393257 MZN393189:MZN393257 NJJ393189:NJJ393257 NTF393189:NTF393257 ODB393189:ODB393257 OMX393189:OMX393257 OWT393189:OWT393257 PGP393189:PGP393257 PQL393189:PQL393257 QAH393189:QAH393257 QKD393189:QKD393257 QTZ393189:QTZ393257 RDV393189:RDV393257 RNR393189:RNR393257 RXN393189:RXN393257 SHJ393189:SHJ393257 SRF393189:SRF393257 TBB393189:TBB393257 TKX393189:TKX393257 TUT393189:TUT393257 UEP393189:UEP393257 UOL393189:UOL393257 UYH393189:UYH393257 VID393189:VID393257 VRZ393189:VRZ393257 WBV393189:WBV393257 WLR393189:WLR393257 WVN393189:WVN393257 F458725:F458793 JB458725:JB458793 SX458725:SX458793 ACT458725:ACT458793 AMP458725:AMP458793 AWL458725:AWL458793 BGH458725:BGH458793 BQD458725:BQD458793 BZZ458725:BZZ458793 CJV458725:CJV458793 CTR458725:CTR458793 DDN458725:DDN458793 DNJ458725:DNJ458793 DXF458725:DXF458793 EHB458725:EHB458793 EQX458725:EQX458793 FAT458725:FAT458793 FKP458725:FKP458793 FUL458725:FUL458793 GEH458725:GEH458793 GOD458725:GOD458793 GXZ458725:GXZ458793 HHV458725:HHV458793 HRR458725:HRR458793 IBN458725:IBN458793 ILJ458725:ILJ458793 IVF458725:IVF458793 JFB458725:JFB458793 JOX458725:JOX458793 JYT458725:JYT458793 KIP458725:KIP458793 KSL458725:KSL458793 LCH458725:LCH458793 LMD458725:LMD458793 LVZ458725:LVZ458793 MFV458725:MFV458793 MPR458725:MPR458793 MZN458725:MZN458793 NJJ458725:NJJ458793 NTF458725:NTF458793 ODB458725:ODB458793 OMX458725:OMX458793 OWT458725:OWT458793 PGP458725:PGP458793 PQL458725:PQL458793 QAH458725:QAH458793 QKD458725:QKD458793 QTZ458725:QTZ458793 RDV458725:RDV458793 RNR458725:RNR458793 RXN458725:RXN458793 SHJ458725:SHJ458793 SRF458725:SRF458793 TBB458725:TBB458793 TKX458725:TKX458793 TUT458725:TUT458793 UEP458725:UEP458793 UOL458725:UOL458793 UYH458725:UYH458793 VID458725:VID458793 VRZ458725:VRZ458793 WBV458725:WBV458793 WLR458725:WLR458793 WVN458725:WVN458793 F524261:F524329 JB524261:JB524329 SX524261:SX524329 ACT524261:ACT524329 AMP524261:AMP524329 AWL524261:AWL524329 BGH524261:BGH524329 BQD524261:BQD524329 BZZ524261:BZZ524329 CJV524261:CJV524329 CTR524261:CTR524329 DDN524261:DDN524329 DNJ524261:DNJ524329 DXF524261:DXF524329 EHB524261:EHB524329 EQX524261:EQX524329 FAT524261:FAT524329 FKP524261:FKP524329 FUL524261:FUL524329 GEH524261:GEH524329 GOD524261:GOD524329 GXZ524261:GXZ524329 HHV524261:HHV524329 HRR524261:HRR524329 IBN524261:IBN524329 ILJ524261:ILJ524329 IVF524261:IVF524329 JFB524261:JFB524329 JOX524261:JOX524329 JYT524261:JYT524329 KIP524261:KIP524329 KSL524261:KSL524329 LCH524261:LCH524329 LMD524261:LMD524329 LVZ524261:LVZ524329 MFV524261:MFV524329 MPR524261:MPR524329 MZN524261:MZN524329 NJJ524261:NJJ524329 NTF524261:NTF524329 ODB524261:ODB524329 OMX524261:OMX524329 OWT524261:OWT524329 PGP524261:PGP524329 PQL524261:PQL524329 QAH524261:QAH524329 QKD524261:QKD524329 QTZ524261:QTZ524329 RDV524261:RDV524329 RNR524261:RNR524329 RXN524261:RXN524329 SHJ524261:SHJ524329 SRF524261:SRF524329 TBB524261:TBB524329 TKX524261:TKX524329 TUT524261:TUT524329 UEP524261:UEP524329 UOL524261:UOL524329 UYH524261:UYH524329 VID524261:VID524329 VRZ524261:VRZ524329 WBV524261:WBV524329 WLR524261:WLR524329 WVN524261:WVN524329 F589797:F589865 JB589797:JB589865 SX589797:SX589865 ACT589797:ACT589865 AMP589797:AMP589865 AWL589797:AWL589865 BGH589797:BGH589865 BQD589797:BQD589865 BZZ589797:BZZ589865 CJV589797:CJV589865 CTR589797:CTR589865 DDN589797:DDN589865 DNJ589797:DNJ589865 DXF589797:DXF589865 EHB589797:EHB589865 EQX589797:EQX589865 FAT589797:FAT589865 FKP589797:FKP589865 FUL589797:FUL589865 GEH589797:GEH589865 GOD589797:GOD589865 GXZ589797:GXZ589865 HHV589797:HHV589865 HRR589797:HRR589865 IBN589797:IBN589865 ILJ589797:ILJ589865 IVF589797:IVF589865 JFB589797:JFB589865 JOX589797:JOX589865 JYT589797:JYT589865 KIP589797:KIP589865 KSL589797:KSL589865 LCH589797:LCH589865 LMD589797:LMD589865 LVZ589797:LVZ589865 MFV589797:MFV589865 MPR589797:MPR589865 MZN589797:MZN589865 NJJ589797:NJJ589865 NTF589797:NTF589865 ODB589797:ODB589865 OMX589797:OMX589865 OWT589797:OWT589865 PGP589797:PGP589865 PQL589797:PQL589865 QAH589797:QAH589865 QKD589797:QKD589865 QTZ589797:QTZ589865 RDV589797:RDV589865 RNR589797:RNR589865 RXN589797:RXN589865 SHJ589797:SHJ589865 SRF589797:SRF589865 TBB589797:TBB589865 TKX589797:TKX589865 TUT589797:TUT589865 UEP589797:UEP589865 UOL589797:UOL589865 UYH589797:UYH589865 VID589797:VID589865 VRZ589797:VRZ589865 WBV589797:WBV589865 WLR589797:WLR589865 WVN589797:WVN589865 F655333:F655401 JB655333:JB655401 SX655333:SX655401 ACT655333:ACT655401 AMP655333:AMP655401 AWL655333:AWL655401 BGH655333:BGH655401 BQD655333:BQD655401 BZZ655333:BZZ655401 CJV655333:CJV655401 CTR655333:CTR655401 DDN655333:DDN655401 DNJ655333:DNJ655401 DXF655333:DXF655401 EHB655333:EHB655401 EQX655333:EQX655401 FAT655333:FAT655401 FKP655333:FKP655401 FUL655333:FUL655401 GEH655333:GEH655401 GOD655333:GOD655401 GXZ655333:GXZ655401 HHV655333:HHV655401 HRR655333:HRR655401 IBN655333:IBN655401 ILJ655333:ILJ655401 IVF655333:IVF655401 JFB655333:JFB655401 JOX655333:JOX655401 JYT655333:JYT655401 KIP655333:KIP655401 KSL655333:KSL655401 LCH655333:LCH655401 LMD655333:LMD655401 LVZ655333:LVZ655401 MFV655333:MFV655401 MPR655333:MPR655401 MZN655333:MZN655401 NJJ655333:NJJ655401 NTF655333:NTF655401 ODB655333:ODB655401 OMX655333:OMX655401 OWT655333:OWT655401 PGP655333:PGP655401 PQL655333:PQL655401 QAH655333:QAH655401 QKD655333:QKD655401 QTZ655333:QTZ655401 RDV655333:RDV655401 RNR655333:RNR655401 RXN655333:RXN655401 SHJ655333:SHJ655401 SRF655333:SRF655401 TBB655333:TBB655401 TKX655333:TKX655401 TUT655333:TUT655401 UEP655333:UEP655401 UOL655333:UOL655401 UYH655333:UYH655401 VID655333:VID655401 VRZ655333:VRZ655401 WBV655333:WBV655401 WLR655333:WLR655401 WVN655333:WVN655401 F720869:F720937 JB720869:JB720937 SX720869:SX720937 ACT720869:ACT720937 AMP720869:AMP720937 AWL720869:AWL720937 BGH720869:BGH720937 BQD720869:BQD720937 BZZ720869:BZZ720937 CJV720869:CJV720937 CTR720869:CTR720937 DDN720869:DDN720937 DNJ720869:DNJ720937 DXF720869:DXF720937 EHB720869:EHB720937 EQX720869:EQX720937 FAT720869:FAT720937 FKP720869:FKP720937 FUL720869:FUL720937 GEH720869:GEH720937 GOD720869:GOD720937 GXZ720869:GXZ720937 HHV720869:HHV720937 HRR720869:HRR720937 IBN720869:IBN720937 ILJ720869:ILJ720937 IVF720869:IVF720937 JFB720869:JFB720937 JOX720869:JOX720937 JYT720869:JYT720937 KIP720869:KIP720937 KSL720869:KSL720937 LCH720869:LCH720937 LMD720869:LMD720937 LVZ720869:LVZ720937 MFV720869:MFV720937 MPR720869:MPR720937 MZN720869:MZN720937 NJJ720869:NJJ720937 NTF720869:NTF720937 ODB720869:ODB720937 OMX720869:OMX720937 OWT720869:OWT720937 PGP720869:PGP720937 PQL720869:PQL720937 QAH720869:QAH720937 QKD720869:QKD720937 QTZ720869:QTZ720937 RDV720869:RDV720937 RNR720869:RNR720937 RXN720869:RXN720937 SHJ720869:SHJ720937 SRF720869:SRF720937 TBB720869:TBB720937 TKX720869:TKX720937 TUT720869:TUT720937 UEP720869:UEP720937 UOL720869:UOL720937 UYH720869:UYH720937 VID720869:VID720937 VRZ720869:VRZ720937 WBV720869:WBV720937 WLR720869:WLR720937 WVN720869:WVN720937 F786405:F786473 JB786405:JB786473 SX786405:SX786473 ACT786405:ACT786473 AMP786405:AMP786473 AWL786405:AWL786473 BGH786405:BGH786473 BQD786405:BQD786473 BZZ786405:BZZ786473 CJV786405:CJV786473 CTR786405:CTR786473 DDN786405:DDN786473 DNJ786405:DNJ786473 DXF786405:DXF786473 EHB786405:EHB786473 EQX786405:EQX786473 FAT786405:FAT786473 FKP786405:FKP786473 FUL786405:FUL786473 GEH786405:GEH786473 GOD786405:GOD786473 GXZ786405:GXZ786473 HHV786405:HHV786473 HRR786405:HRR786473 IBN786405:IBN786473 ILJ786405:ILJ786473 IVF786405:IVF786473 JFB786405:JFB786473 JOX786405:JOX786473 JYT786405:JYT786473 KIP786405:KIP786473 KSL786405:KSL786473 LCH786405:LCH786473 LMD786405:LMD786473 LVZ786405:LVZ786473 MFV786405:MFV786473 MPR786405:MPR786473 MZN786405:MZN786473 NJJ786405:NJJ786473 NTF786405:NTF786473 ODB786405:ODB786473 OMX786405:OMX786473 OWT786405:OWT786473 PGP786405:PGP786473 PQL786405:PQL786473 QAH786405:QAH786473 QKD786405:QKD786473 QTZ786405:QTZ786473 RDV786405:RDV786473 RNR786405:RNR786473 RXN786405:RXN786473 SHJ786405:SHJ786473 SRF786405:SRF786473 TBB786405:TBB786473 TKX786405:TKX786473 TUT786405:TUT786473 UEP786405:UEP786473 UOL786405:UOL786473 UYH786405:UYH786473 VID786405:VID786473 VRZ786405:VRZ786473 WBV786405:WBV786473 WLR786405:WLR786473 WVN786405:WVN786473 F851941:F852009 JB851941:JB852009 SX851941:SX852009 ACT851941:ACT852009 AMP851941:AMP852009 AWL851941:AWL852009 BGH851941:BGH852009 BQD851941:BQD852009 BZZ851941:BZZ852009 CJV851941:CJV852009 CTR851941:CTR852009 DDN851941:DDN852009 DNJ851941:DNJ852009 DXF851941:DXF852009 EHB851941:EHB852009 EQX851941:EQX852009 FAT851941:FAT852009 FKP851941:FKP852009 FUL851941:FUL852009 GEH851941:GEH852009 GOD851941:GOD852009 GXZ851941:GXZ852009 HHV851941:HHV852009 HRR851941:HRR852009 IBN851941:IBN852009 ILJ851941:ILJ852009 IVF851941:IVF852009 JFB851941:JFB852009 JOX851941:JOX852009 JYT851941:JYT852009 KIP851941:KIP852009 KSL851941:KSL852009 LCH851941:LCH852009 LMD851941:LMD852009 LVZ851941:LVZ852009 MFV851941:MFV852009 MPR851941:MPR852009 MZN851941:MZN852009 NJJ851941:NJJ852009 NTF851941:NTF852009 ODB851941:ODB852009 OMX851941:OMX852009 OWT851941:OWT852009 PGP851941:PGP852009 PQL851941:PQL852009 QAH851941:QAH852009 QKD851941:QKD852009 QTZ851941:QTZ852009 RDV851941:RDV852009 RNR851941:RNR852009 RXN851941:RXN852009 SHJ851941:SHJ852009 SRF851941:SRF852009 TBB851941:TBB852009 TKX851941:TKX852009 TUT851941:TUT852009 UEP851941:UEP852009 UOL851941:UOL852009 UYH851941:UYH852009 VID851941:VID852009 VRZ851941:VRZ852009 WBV851941:WBV852009 WLR851941:WLR852009 WVN851941:WVN852009 F917477:F917545 JB917477:JB917545 SX917477:SX917545 ACT917477:ACT917545 AMP917477:AMP917545 AWL917477:AWL917545 BGH917477:BGH917545 BQD917477:BQD917545 BZZ917477:BZZ917545 CJV917477:CJV917545 CTR917477:CTR917545 DDN917477:DDN917545 DNJ917477:DNJ917545 DXF917477:DXF917545 EHB917477:EHB917545 EQX917477:EQX917545 FAT917477:FAT917545 FKP917477:FKP917545 FUL917477:FUL917545 GEH917477:GEH917545 GOD917477:GOD917545 GXZ917477:GXZ917545 HHV917477:HHV917545 HRR917477:HRR917545 IBN917477:IBN917545 ILJ917477:ILJ917545 IVF917477:IVF917545 JFB917477:JFB917545 JOX917477:JOX917545 JYT917477:JYT917545 KIP917477:KIP917545 KSL917477:KSL917545 LCH917477:LCH917545 LMD917477:LMD917545 LVZ917477:LVZ917545 MFV917477:MFV917545 MPR917477:MPR917545 MZN917477:MZN917545 NJJ917477:NJJ917545 NTF917477:NTF917545 ODB917477:ODB917545 OMX917477:OMX917545 OWT917477:OWT917545 PGP917477:PGP917545 PQL917477:PQL917545 QAH917477:QAH917545 QKD917477:QKD917545 QTZ917477:QTZ917545 RDV917477:RDV917545 RNR917477:RNR917545 RXN917477:RXN917545 SHJ917477:SHJ917545 SRF917477:SRF917545 TBB917477:TBB917545 TKX917477:TKX917545 TUT917477:TUT917545 UEP917477:UEP917545 UOL917477:UOL917545 UYH917477:UYH917545 VID917477:VID917545 VRZ917477:VRZ917545 WBV917477:WBV917545 WLR917477:WLR917545 WVN917477:WVN917545 F983013:F983081 JB983013:JB983081 SX983013:SX983081 ACT983013:ACT983081 AMP983013:AMP983081 AWL983013:AWL983081 BGH983013:BGH983081 BQD983013:BQD983081 BZZ983013:BZZ983081 CJV983013:CJV983081 CTR983013:CTR983081 DDN983013:DDN983081 DNJ983013:DNJ983081 DXF983013:DXF983081 EHB983013:EHB983081 EQX983013:EQX983081 FAT983013:FAT983081 FKP983013:FKP983081 FUL983013:FUL983081 GEH983013:GEH983081 GOD983013:GOD983081 GXZ983013:GXZ983081 HHV983013:HHV983081 HRR983013:HRR983081 IBN983013:IBN983081 ILJ983013:ILJ983081 IVF983013:IVF983081 JFB983013:JFB983081 JOX983013:JOX983081 JYT983013:JYT983081 KIP983013:KIP983081 KSL983013:KSL983081 LCH983013:LCH983081 LMD983013:LMD983081 LVZ983013:LVZ983081 MFV983013:MFV983081 MPR983013:MPR983081 MZN983013:MZN983081 NJJ983013:NJJ983081 NTF983013:NTF983081 ODB983013:ODB983081 OMX983013:OMX983081 OWT983013:OWT983081 PGP983013:PGP983081 PQL983013:PQL983081 QAH983013:QAH983081 QKD983013:QKD983081 QTZ983013:QTZ983081 RDV983013:RDV983081 RNR983013:RNR983081 RXN983013:RXN983081 SHJ983013:SHJ983081 SRF983013:SRF983081 TBB983013:TBB983081 TKX983013:TKX983081 TUT983013:TUT983081 UEP983013:UEP983081 UOL983013:UOL983081 UYH983013:UYH983081 VID983013:VID983081 VRZ983013:VRZ983081 WBV983013:WBV983081 WLR983013:WLR983081 F6:F41 JB6:JB41 SX6:SX41 ACT6:ACT41 AMP6:AMP41 AWL6:AWL41 BGH6:BGH41 BQD6:BQD41 BZZ6:BZZ41 CJV6:CJV41 CTR6:CTR41 DDN6:DDN41 DNJ6:DNJ41 DXF6:DXF41 EHB6:EHB41 EQX6:EQX41 FAT6:FAT41 FKP6:FKP41 FUL6:FUL41 GEH6:GEH41 GOD6:GOD41 GXZ6:GXZ41 HHV6:HHV41 HRR6:HRR41 IBN6:IBN41 ILJ6:ILJ41 IVF6:IVF41 JFB6:JFB41 JOX6:JOX41 JYT6:JYT41 KIP6:KIP41 KSL6:KSL41 LCH6:LCH41 LMD6:LMD41 LVZ6:LVZ41 MFV6:MFV41 MPR6:MPR41 MZN6:MZN41 NJJ6:NJJ41 NTF6:NTF41 ODB6:ODB41 OMX6:OMX41 OWT6:OWT41 PGP6:PGP41 PQL6:PQL41 QAH6:QAH41 QKD6:QKD41 QTZ6:QTZ41 RDV6:RDV41 RNR6:RNR41 RXN6:RXN41 SHJ6:SHJ41 SRF6:SRF41 TBB6:TBB41 TKX6:TKX41 TUT6:TUT41 UEP6:UEP41 UOL6:UOL41 UYH6:UYH41 VID6:VID41 VRZ6:VRZ41 WBV6:WBV41 WLR6:WLR41 WVN6:WVN41">
       <formula1>"Once,Annual,Semiannual,EveryFourthMonth,Quarterly,Bimonthly,Monthly"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>